<commit_message>
Changed max diameter of monopile to 12m. Max diam of tower to 10m. Changed tower thickness bounds.
</commit_message>
<xml_diff>
--- a/examples/99_tower_gbf/15mw/20m/outputs_mono/monotow_output.xlsx
+++ b/examples/99_tower_gbf/15mw/20m/outputs_mono/monotow_output.xlsx
@@ -914,7 +914,8 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[[0.077 0.077 0.077 0.077 0.077 0.077 0.077]]</t>
+          <t>[[0.077      0.077      0.10095695 0.10347047 0.1052105  0.09579198
+  0.08345544]]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -937,8 +938,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[12.43319258 12.4331927  12.4331927  12.43319276 12.43319278 12.43319278
- 12.43319278]</t>
+          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[12.43319278]</t>
+          <t>[10.]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[12.43319278]</t>
+          <t>[11.]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -2942,7 +2942,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>[3.29001049]</t>
+          <t>[2.8838056]</t>
         </is>
       </c>
       <c r="E111" t="inlineStr"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>[[0.02921938 0.01614151 0.01226288 0.01122482 0.01163286]]</t>
+          <t>[[0.04       0.04       0.03760199 0.015      0.015     ]]</t>
         </is>
       </c>
       <c r="E138" t="inlineStr"/>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 11.42989152  8.90073352  6.01183391]</t>
+          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
         </is>
       </c>
       <c r="E139" t="inlineStr"/>
@@ -4573,10 +4573,10 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          96476.17864374
-  96918.90641228  98252.45317392 100493.08222435 103668.49141771
- 107818.75539867 112997.76167827 126739.70475695 145701.26866961
- 171147.80374315      0.              0.              0.
+          <t>[     0.              0.              0.          76069.22818689
+  76419.81487525  77475.80310771  79250.00595527  81764.21915156
+  85049.92502601  89149.36708317 100022.09247963 115010.75107985
+ 135096.15327474      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -4827,10 +4827,8 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>[12.43319258 12.43319262 12.43319266 12.4331927  12.4331927  12.4331927
- 12.4331927  12.43319272 12.43319274 12.43319276 12.43319277 12.43319277
- 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278
- 12.43319278]</t>
+          <t>[11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11.
+ 11.]</t>
         </is>
       </c>
       <c r="E190" t="inlineStr"/>
@@ -4971,10 +4969,10 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          96476.17864374
-  96918.90641228  98252.45317392 100493.08222435 103668.49141771
- 107818.75539867 112997.76167827 126739.70475695 145701.26866961
- 171147.80374315      0.              0.              0.
+          <t>[     0.              0.              0.          76069.22818689
+  76419.81487525  77475.80310771  79250.00595527  81764.21915156
+  85049.92502601  89149.36708317 100022.09247963 115010.75107985
+ 135096.15327474      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -5117,10 +5115,10 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>[      0.               0.               0.          -96476.17864374
-  -96918.90641228  -98252.45317392 -100493.08222435 -103668.49141771
- -107818.75539867 -112997.76167827 -126739.70475695 -145701.26866961
- -171147.80374315       0.               0.               0.
+          <t>[      0.               0.               0.          -76069.22818689
+  -76419.81487525  -77475.80310771  -79250.00595527  -81764.21915156
+  -85049.92502601  -89149.36708317 -100022.09247963 -115010.75107985
+ -135096.15327474       0.               0.               0.
        0.               0.               0.        ]</t>
         </is>
       </c>
@@ -5171,8 +5169,7 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>[12.43319258 12.4331927  12.4331927  12.43319276 12.43319278 12.43319278
- 12.43319278]</t>
+          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
         </is>
       </c>
       <c r="E204" t="inlineStr"/>
@@ -5195,7 +5192,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>[0.077 0.077 0.077 0.077 0.077 0.077]</t>
+          <t>[0.077      0.08897847 0.10221371 0.10434048 0.10050124 0.08962371]</t>
         </is>
       </c>
       <c r="E205" t="inlineStr"/>
@@ -5261,8 +5258,7 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>[12.43319258 12.4331927  12.4331927  12.43319276 12.43319278 12.43319278
- 12.43319278]</t>
+          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
         </is>
       </c>
       <c r="E208" t="inlineStr"/>
@@ -5285,7 +5281,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>[0.077 0.077 0.077 0.077 0.077 0.077]</t>
+          <t>[0.077      0.08897847 0.10221371 0.10434048 0.10050124 0.08962371]</t>
         </is>
       </c>
       <c r="E209" t="inlineStr"/>
@@ -5548,8 +5544,9 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>[0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077
- 0.077 0.077 0.077 0.077 0.077 0.077]</t>
+          <t>[0.077      0.077      0.077      0.08897847 0.08897847 0.08897847
+ 0.10221371 0.10221371 0.10221371 0.10434048 0.10434048 0.10434048
+ 0.10050124 0.10050124 0.10050124 0.08962371 0.08962371 0.08962371]</t>
         </is>
       </c>
       <c r="E220" t="inlineStr"/>
@@ -5713,7 +5710,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>[1621500.22424683]</t>
+          <t>[1648375.1234354]</t>
         </is>
       </c>
       <c r="E227" t="inlineStr"/>
@@ -5736,7 +5733,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>[3961795.23695627]</t>
+          <t>[3980261.24221089]</t>
         </is>
       </c>
       <c r="E228" t="inlineStr"/>
@@ -5759,7 +5756,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>[32.4999999]</t>
+          <t>[34.4331827]</t>
         </is>
       </c>
       <c r="E229" t="inlineStr"/>
@@ -5782,7 +5779,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>[2.31455943e+09 2.31455943e+09 6.18932421e+07 0.00000000e+00
+          <t>[2.54169442e+09 2.54169442e+09 4.90525923e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -5806,7 +5803,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>[658532.04559183]</t>
+          <t>[1175518.62964259]</t>
         </is>
       </c>
       <c r="E231" t="inlineStr"/>
@@ -5829,7 +5826,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>[2150911.87879668]</t>
+          <t>[3187423.76365581]</t>
         </is>
       </c>
       <c r="E232" t="inlineStr"/>
@@ -5876,26 +5873,26 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>[[2.30719502e+10 6.04489020e+12 2.30719502e+10 6.04489020e+12
-  1.58821565e+10 1.79384436e+11]
- [2.09970029e+10 4.38691536e+12 2.09970029e+10 4.38691536e+12
-  1.47621565e+10 1.79384436e+11]
- [1.89220555e+10 3.08291584e+12 1.89220555e+10 3.08291584e+12
-  1.36421565e+10 1.79384436e+11]
- [1.68471081e+10 2.08864470e+12 1.68471081e+10 2.08864470e+12
-  1.25221565e+10 1.79384436e+11]
- [1.47721607e+10 1.35985505e+12 1.47721607e+10 1.35985505e+12
-  1.14021565e+10 1.79384436e+11]
- [1.26972134e+10 8.52299963e+11 1.26972134e+10 8.52299963e+11
-  1.02821565e+10 1.79384436e+11]
- [1.06222660e+10 5.21732532e+11 1.06222660e+10 5.21732532e+11
-  9.16215654e+09 1.79384436e+11]
- [8.54731864e+09 3.23905842e+11 8.54731864e+09 3.23905842e+11
-  8.04215654e+09 1.79384436e+11]
- [6.47237127e+09 2.14572979e+11 6.47237127e+09 2.14572979e+11
-  6.92215654e+09 1.79384436e+11]
- [4.39742390e+09 1.49487030e+11 4.39742390e+09 1.49487030e+11
-  5.80215654e+09 1.79384436e+11]]</t>
+          <t>[[2.25650526e+10 5.88608222e+12 2.25650526e+10 5.88608222e+12
+  1.52133333e+10 1.24226667e+11]
+ [2.04901053e+10 4.24064551e+12 2.04901053e+10 4.24064551e+12
+  1.40933333e+10 1.24226667e+11]
+ [1.84151579e+10 2.94918412e+12 1.84151579e+10 2.94918412e+12
+  1.29733333e+10 1.24226667e+11]
+ [1.63402105e+10 1.96745111e+12 1.63402105e+10 1.96745111e+12
+  1.18533333e+10 1.24226667e+11]
+ [1.42652632e+10 1.25119959e+12 1.42652632e+10 1.25119959e+12
+  1.07333333e+10 1.24226667e+11]
+ [1.21903158e+10 7.56182634e+11 1.21903158e+10 7.56182634e+11
+  9.61333333e+09 1.24226667e+11]
+ [1.01153684e+10 4.38153333e+11 1.01153684e+10 4.38153333e+11
+  8.49333333e+09 1.24226667e+11]
+ [8.04042105e+09 2.52864774e+11 8.04042105e+09 2.52864774e+11
+  7.37333333e+09 1.24226667e+11]
+ [5.96547368e+09 1.56070041e+11 5.96547368e+09 1.56070041e+11
+  6.25333333e+09 1.24226667e+11]
+ [3.89052632e+09 1.03522222e+11 3.89052632e+09 1.03522222e+11
+  5.13333333e+09 1.24226667e+11]]</t>
         </is>
       </c>
       <c r="E234" t="inlineStr"/>
@@ -5918,9 +5915,9 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>[3.19822531 3.19822532 3.19822533 3.19822529 3.19822529 3.19822529
- 3.19822526 3.19822526 3.19822527 3.19822527 3.19822527 3.19822527
- 3.19822527 3.19822527 3.19822527 3.19822527 3.19822527 3.19822527]</t>
+          <t>[2.82726365 2.82726365 2.82726365 3.263503   3.263503   3.263503
+ 3.74438999 3.74438999 3.74438999 3.82155405 3.82155405 3.82155405
+ 3.6822358  3.6822358  3.6822358  3.28697421 3.28697421 3.28697421]</t>
         </is>
       </c>
       <c r="E235" t="inlineStr"/>
@@ -5943,9 +5940,9 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>[1.81995474 1.81995474 1.81995475 1.81995473 1.81995472 1.81995472
- 1.81995471 1.81995471 1.81995471 1.81995471 1.81995472 1.81995472
- 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472]</t>
+          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
+ 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
+ 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599 ]</t>
         </is>
       </c>
       <c r="E236" t="inlineStr"/>
@@ -5968,9 +5965,9 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>[1.81995474 1.81995474 1.81995475 1.81995473 1.81995472 1.81995472
- 1.81995471 1.81995471 1.81995471 1.81995471 1.81995472 1.81995472
- 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472]</t>
+          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
+ 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
+ 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599 ]</t>
         </is>
       </c>
       <c r="E237" t="inlineStr"/>
@@ -5993,9 +5990,9 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>[61.03869951 61.03870008 61.03870064 61.03870009 61.03870008 61.03870008
- 61.03869957 61.0386999  61.03870023 61.03870043 61.03870051 61.0387006
- 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064]</t>
+          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
+ 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
+ 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073]</t>
         </is>
       </c>
       <c r="E238" t="inlineStr"/>
@@ -6018,9 +6015,9 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>[61.03869951 61.03870008 61.03870064 61.03870009 61.03870008 61.03870008
- 61.03869957 61.0386999  61.03870023 61.03870043 61.03870051 61.0387006
- 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064]</t>
+          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
+ 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
+ 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073]</t>
         </is>
       </c>
       <c r="E239" t="inlineStr"/>
@@ -6043,10 +6040,10 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>[122.07739902 122.07740015 122.07740128 122.07740017 122.07740017
- 122.07740016 122.07739914 122.07739979 122.07740045 122.07740086
- 122.07740103 122.07740119 122.07740128 122.07740128 122.07740128
- 122.07740128 122.07740128 122.07740128]</t>
+          <t>[ 84.33576062  84.33576062  84.33576062  97.1367864   97.1367864
+  97.1367864  111.18235328 111.18235328 111.18235328 113.42972734
+ 113.42972734 113.42972734 109.3708483  109.3708483  109.3708483
+  97.82392145  97.82392145  97.82392145]</t>
         </is>
       </c>
       <c r="E240" t="inlineStr"/>
@@ -6241,8 +6238,8 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>[0.94618249 0.94618249 0.94618249 0.58490872 0.5689426  0.55297649
- 0.43411361 0.40083242 0.36755123 0.32301245 0.28601711 0.24902177]</t>
+          <t>[1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
+ 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
         </is>
       </c>
       <c r="E247" t="inlineStr"/>
@@ -6265,8 +6262,8 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>[0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E248" t="inlineStr"/>
@@ -6289,8 +6286,8 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>[0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E249" t="inlineStr"/>
@@ -6313,8 +6310,8 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>[18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E250" t="inlineStr"/>
@@ -6337,8 +6334,8 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>[18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E251" t="inlineStr"/>
@@ -6361,8 +6358,8 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>[36.43307152 36.43307152 36.43307152 21.94960044 20.2007613  18.54737303
- 13.12388581 10.33096399  7.96537229  5.70856597  3.96319571  2.6156629 ]</t>
+          <t>[33.21380796 33.21380796 33.21380796 32.22982785 32.22982785 32.22982785
+ 19.88323673 16.18153341 12.97038057  5.79213059  4.36751812  3.19804084]</t>
         </is>
       </c>
       <c r="E252" t="inlineStr"/>
@@ -6456,9 +6453,9 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 12.43319278 12.43319278 12.09875903 11.76432528
- 11.42989152 10.58683885  9.74378618  8.90073352  7.93776698  6.97480044
-  6.01183391]</t>
+          <t>[10.         10.         10.         10.         10.         10.
+ 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
+  5.999     ]</t>
         </is>
       </c>
       <c r="E256" t="inlineStr"/>
@@ -6481,8 +6478,8 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>[0.02268044 0.02268044 0.02268044 0.0142022  0.0142022  0.0142022
- 0.01174385 0.01174385 0.01174385 0.01142884 0.01142884 0.01142884]</t>
+          <t>[0.04     0.04     0.04     0.038801 0.038801 0.038801 0.026301 0.026301
+ 0.026301 0.015    0.015    0.015   ]</t>
         </is>
       </c>
       <c r="E257" t="inlineStr"/>
@@ -6587,9 +6584,9 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>[[  2427925.55809716]
+          <t>[[  2427925.55809668]
  [    29094.73368413]
- [-13609523.83933535]]</t>
+ [-18668642.37894937]]</t>
         </is>
       </c>
       <c r="E261" t="inlineStr"/>
@@ -6612,8 +6609,8 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>[[-4.71357613e+06]
- [ 3.55687256e+08]
+          <t>[[-4.70896222e+06]
+ [ 3.55500528e+08]
  [ 1.29946107e+06]]</t>
         </is>
       </c>
@@ -6637,7 +6634,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>[1932303.53344269 1932303.53344269 3864607.06688539       0.
+          <t>[1512500.         1512500.         3024999.99999999       0.
        0.               0.        ]</t>
         </is>
       </c>
@@ -6730,7 +6727,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>[1625606.93571539]</t>
+          <t>[2142593.51976615]</t>
         </is>
       </c>
       <c r="E267" t="inlineStr"/>
@@ -6753,7 +6750,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>[-3.93513649e+00 -5.81329521e-02  1.22745569e+02]</t>
+          <t>[-2.98562705e+00 -4.41060468e-02  1.08214197e+02]</t>
         </is>
       </c>
       <c r="E268" t="inlineStr"/>
@@ -6776,7 +6773,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>[2.93222946e+10 2.91848076e+10 2.79277543e+08 7.86163621e+02
+          <t>[3.18866698e+10 3.17491828e+10 2.84709346e+08 7.86163621e+02
  1.35359722e+07 1.70976373e+05]</t>
         </is>
       </c>
@@ -6885,16 +6882,16 @@
           <t>[[      0.        ]
  [      0.        ]
  [      0.        ]
- [ -96476.17864374]
- [ -96918.90641228]
- [ -98252.45317392]
- [-100493.08222435]
- [-103668.49141771]
- [-107818.75539867]
- [-112997.76167827]
- [-126739.70475695]
- [-145701.26866961]
- [-171147.80374315]
+ [ -76069.22818689]
+ [ -76419.81487525]
+ [ -77475.80310771]
+ [ -79250.00595527]
+ [ -81764.21915156]
+ [ -85049.92502601]
+ [ -89149.36708317]
+ [-100022.09247963]
+ [-115010.75107985]
+ [-135096.15327474]
  [      0.        ]
  [      0.        ]
  [      0.        ]
@@ -6993,19 +6990,19 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>[[-417.76067857]
- [-480.09738431]
- [-523.65058445]
- [-557.91160668]
- [-581.92125008]
- [-597.20357718]
- [-606.4643562 ]
- [-576.1548744 ]
- [-542.98427067]
- [-506.9184334 ]
- [-460.2271512 ]
- [-409.29061826]
- [-353.04163049]]</t>
+          <t>[[-336.9560439 ]
+ [-388.43785582]
+ [-424.16473764]
+ [-452.12457083]
+ [-484.27449749]
+ [-510.65946695]
+ [-533.22010636]
+ [-511.58791739]
+ [-487.37587695]
+ [-460.61782438]
+ [-427.60678303]
+ [-391.57616974]
+ [-352.18249915]]</t>
         </is>
       </c>
       <c r="E275" t="inlineStr"/>
@@ -7028,24 +7025,24 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>[[-31179435.72038715]
- [-28733133.38425641]
- [-25809273.9770739 ]
- [-25242005.971014  ]
- [-24673272.54583432]
- [-24101590.42890056]
- [-23525440.07335947]
- [-22943246.03860893]
- [-22353355.35982918]
- [-21142354.43006401]
- [-19877392.72607838]
- [-18539157.66846403]
- [-17441329.69565723]
- [-16625895.58361371]
- [-15810461.47157015]
- [-15402744.41554845]
- [-14995027.35952632]
- [-14587310.30350392]]</t>
+          <t>[[-36123346.97588959]
+ [-33960790.79041462]
+ [-31421691.94796431]
+ [-30879849.66133218]
+ [-30336846.93487328]
+ [-29791509.30376027]
+ [-29181329.17357343]
+ [-28566364.10790942]
+ [-27945306.30131707]
+ [-26658812.50241386]
+ [-25329647.43537711]
+ [-23942610.16605137]
+ [-22780861.82640503]
+ [-21842022.14135061]
+ [-20903182.45629581]
+ [-20484151.47503773]
+ [-20065120.49377933]
+ [-19646089.51252162]]</t>
         </is>
       </c>
       <c r="E276" t="inlineStr"/>
@@ -7068,24 +7065,24 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>[[-3630432.17990122]
- [-8198899.84274795]
- [-7770118.21064171]
- [ 2428056.98943542]
- [ 2428073.38905587]
- [ 2428090.12906986]
- [ 2428107.34313002]
- [ 2428125.1727663 ]
- [ 2428143.77066976]
- [ 2428420.43316857]
- [ 2428507.89136093]
- [ 2428608.99916826]
- [ 2428599.3996326 ]
- [ 2428426.01496882]
- [ 2428465.30683914]
- [ 2428209.88216267]
- [ 2428219.36397806]
- [ 2428228.73207834]]</t>
+          <t>[[-3571386.85080247]
+ [-8980999.77048393]
+ [-9160127.16752138]
+ [ 2428093.82801644]
+ [ 2428113.53256131]
+ [ 2428133.56642783]
+ [ 2428177.55584712]
+ [ 2428198.07321296]
+ [ 2428219.29887818]
+ [ 2428588.30264015]
+ [ 2428684.72498103]
+ [ 2428793.4671491 ]
+ [ 2428772.71401341]
+ [ 2428620.0939148 ]
+ [ 2428670.77338876]
+ [ 2428275.82942879]
+ [ 2428288.03473593]
+ [ 2428300.09340087]]</t>
         </is>
       </c>
       <c r="E277" t="inlineStr"/>
@@ -7108,24 +7105,24 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>[[ -47410.92596769]
- [-107349.00461938]
- [-102767.23478233]
- [  29096.4415081 ]
- [  29096.65584818]
- [  29096.87478316]
- [  29097.10006327]
- [  29097.3335442 ]
- [  29097.57723025]
- [  29101.18729044]
- [  29102.33512868]
- [  29103.66334132]
- [  29103.54613785]
- [  29101.28472521]
- [  29101.80566794]
- [  29098.46161373]
- [  29098.58775759]
- [  29098.7125375 ]]</t>
+          <t>[[ -46612.79626053]
+ [-117471.93621095]
+ [-120846.42288106]
+ [  29096.92151658]
+ [  29097.17898185]
+ [  29097.44093214]
+ [  29098.01559855]
+ [  29098.28422904]
+ [  29098.56230757]
+ [  29103.37730347]
+ [  29104.64273106]
+ [  29106.07123526]
+ [  29105.80901867]
+ [  29103.82156847]
+ [  29104.49322739]
+ [  29099.32366656]
+ [  29099.48597565]
+ [  29099.64652502]]</t>
         </is>
       </c>
       <c r="E278" t="inlineStr"/>
@@ -7148,24 +7145,24 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>[[ -671569.38927988]
- [-2556545.26945517]
- [-4649408.3173616 ]
- [-5412555.49602903]
- [-5363780.52488637]
- [-5314981.82955081]
- [-5266161.10671832]
- [-5217320.06743728]
- [-5168460.44500652]
- [-5070681.72287733]
- [-4972848.36671396]
- [-4874975.95141809]
- [-4777081.15300104]
- [-4679164.50009334]
- [-4581220.77998569]
- [-4532247.55915087]
- [-4483271.00523964]
- [-4434292.00104467]]</t>
+          <t>[[ -526598.7774628 ]
+ [-2406071.56195532]
+ [-4715198.34905789]
+ [-5431349.17696918]
+ [-5382395.25464339]
+ [-5333402.76688932]
+ [-5284377.98404438]
+ [-5235325.59908948]
+ [-5186247.67118431]
+ [-5088011.01723978]
+ [-4989699.00157361]
+ [-4891329.46663574]
+ [-4792918.5016765 ]
+ [-4694465.88006755]
+ [-4595969.73165049]
+ [-4546715.11585086]
+ [-4497449.51364613]
+ [-4448174.12628585]]</t>
         </is>
       </c>
       <c r="E279" t="inlineStr"/>
@@ -7188,24 +7185,24 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>[[5.16435012e+07]
- [1.96221076e+08]
- [3.55840560e+08]
- [4.14083720e+08]
- [4.10015355e+08]
- [4.05945179e+08]
- [4.01873324e+08]
- [3.97799923e+08]
- [3.93725110e+08]
- [3.85570964e+08]
- [3.77412692e+08]
- [3.69251492e+08]
- [3.61088644e+08]
- [3.52924192e+08]
- [3.44757740e+08]
- [3.40674436e+08]
- [3.36590896e+08]
- [3.32507186e+08]]</t>
+          <t>[[4.05032729e+07]
+ [1.84726748e+08]
+ [3.60998049e+08]
+ [4.15644529e+08]
+ [4.11562418e+08]
+ [4.07477361e+08]
+ [4.03389850e+08]
+ [3.99300236e+08]
+ [3.95208680e+08]
+ [3.87019429e+08]
+ [3.78824481e+08]
+ [3.70625212e+08]
+ [3.62422859e+08]
+ [3.54217416e+08]
+ [3.46008748e+08]
+ [3.41903950e+08]
+ [3.37798342e+08]
+ [3.33692018e+08]]</t>
         </is>
       </c>
       <c r="E280" t="inlineStr"/>
@@ -7228,24 +7225,24 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>[[ 214260.6777001 ]
- [ 468224.68710593]
- [ 808955.83756311]
- [1299593.325459  ]
- [1299590.41838053]
- [1299587.50380529]
- [1299584.57413213]
- [1299581.62157415]
- [1299578.63805818]
- [1299575.61511389]
- [1299569.40928209]
- [1299562.92698901]
- [1299556.06927721]
- [1299550.44357231]
- [1299546.26499681]
- [1299542.08644818]
- [1299539.99718394]
- [1299537.90792641]]</t>
+          <t>[[ 214069.90260215]
+ [ 467905.66188862]
+ [ 808663.37487048]
+ [1299618.86705817]
+ [1299616.14571376]
+ [1299613.41855259]
+ [1299591.46407197]
+ [1299588.79319843]
+ [1299586.10139144]
+ [1299580.91306006]
+ [1299575.39564019]
+ [1299569.69526414]
+ [1299567.63171611]
+ [1299562.46088873]
+ [1299558.28223587]
+ [1299565.29142155]
+ [1299563.2020827 ]
+ [1299561.11275055]]</t>
         </is>
       </c>
       <c r="E281" t="inlineStr"/>
@@ -7297,12 +7294,12 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>[12.43319258 12.43319262 12.43319266 12.4331927  12.4331927  12.4331927
- 12.4331927  12.43319272 12.43319274 12.43319276 12.43319277 12.43319277
- 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278
- 12.43319278 12.43319278 12.43319278 12.43319278 12.09875903 11.76432528
- 11.42989152 10.58683885  9.74378618  8.90073352  7.93776698  6.97480044
-  6.01183391]</t>
+          <t>[11.         11.         11.         11.         11.         11.
+ 11.         11.         11.         11.         11.         11.
+ 11.         11.         11.         11.         11.         11.
+ 10.         10.         10.         10.         10.         10.
+ 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
+  5.999     ]</t>
         </is>
       </c>
       <c r="E283" t="inlineStr"/>
@@ -7325,11 +7322,11 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>[0.077      0.077      0.077      0.077      0.077      0.077
- 0.077      0.077      0.077      0.077      0.077      0.077
- 0.077      0.077      0.077      0.077      0.077      0.077
- 0.02268044 0.02268044 0.02268044 0.0142022  0.0142022  0.0142022
- 0.01174385 0.01174385 0.01174385 0.01142884 0.01142884 0.01142884]</t>
+          <t>[0.077      0.077      0.077      0.08897847 0.08897847 0.08897847
+ 0.10221371 0.10221371 0.10221371 0.10434048 0.10434048 0.10434048
+ 0.10050124 0.10050124 0.10050124 0.08962371 0.08962371 0.08962371
+ 0.04       0.04       0.04       0.038801   0.038801   0.038801
+ 0.026301   0.026301   0.026301   0.015      0.015      0.015     ]</t>
         </is>
       </c>
       <c r="E284" t="inlineStr"/>
@@ -7477,11 +7474,11 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>[3.19822531 3.19822532 3.19822533 3.19822529 3.19822529 3.19822529
- 3.19822526 3.19822526 3.19822527 3.19822527 3.19822527 3.19822527
- 3.19822527 3.19822527 3.19822527 3.19822527 3.19822527 3.19822527
- 0.94618249 0.94618249 0.94618249 0.58490872 0.5689426  0.55297649
- 0.43411361 0.40083242 0.36755123 0.32301245 0.28601711 0.24902177]</t>
+          <t>[2.82726365 2.82726365 2.82726365 3.263503   3.263503   3.263503
+ 3.74438999 3.74438999 3.74438999 3.82155405 3.82155405 3.82155405
+ 3.6822358  3.6822358  3.6822358  3.28697421 3.28697421 3.28697421
+ 1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
+ 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
         </is>
       </c>
       <c r="E290" t="inlineStr"/>
@@ -7504,11 +7501,11 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>[1.81995474 1.81995474 1.81995475 1.81995473 1.81995472 1.81995472
- 1.81995471 1.81995471 1.81995471 1.81995471 1.81995472 1.81995472
- 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472
- 0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
+ 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
+ 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
+ 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E291" t="inlineStr"/>
@@ -7531,11 +7528,11 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>[1.81995474 1.81995474 1.81995475 1.81995473 1.81995472 1.81995472
- 1.81995471 1.81995471 1.81995471 1.81995471 1.81995472 1.81995472
- 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472
- 0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
+ 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
+ 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
+ 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E292" t="inlineStr"/>
@@ -7558,11 +7555,11 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>[61.03869951 61.03870008 61.03870064 61.03870009 61.03870008 61.03870008
- 61.03869957 61.0386999  61.03870023 61.03870043 61.03870051 61.0387006
- 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064
- 18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
+ 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
+ 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
+ 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E293" t="inlineStr"/>
@@ -7585,11 +7582,11 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>[61.03869951 61.03870008 61.03870064 61.03870009 61.03870008 61.03870008
- 61.03869957 61.0386999  61.03870023 61.03870043 61.03870051 61.0387006
- 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064
- 18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
+ 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
+ 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
+ 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E294" t="inlineStr"/>
@@ -7612,12 +7609,12 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>[122.07739902 122.07740015 122.07740128 122.07740017 122.07740017
- 122.07740016 122.07739914 122.07739979 122.07740045 122.07740086
- 122.07740103 122.07740119 122.07740128 122.07740128 122.07740128
- 122.07740128 122.07740128 122.07740128  36.43307152  36.43307152
-  36.43307152  21.94960044  20.2007613   18.54737303  13.12388581
-  10.33096399   7.96537229   5.70856597   3.96319571   2.6156629 ]</t>
+          <t>[ 84.33576062  84.33576062  84.33576062  97.1367864   97.1367864
+  97.1367864  111.18235328 111.18235328 111.18235328 113.42972734
+ 113.42972734 113.42972734 109.3708483  109.3708483  109.3708483
+  97.82392145  97.82392145  97.82392145  33.21380796  33.21380796
+  33.21380796  32.22982785  32.22982785  32.22982785  19.88323673
+  16.18153341  12.97038057   5.79213059   4.36751812   3.19804084]</t>
         </is>
       </c>
       <c r="E295" t="inlineStr"/>
@@ -7640,36 +7637,36 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>[[-3.11794357e+07]
- [-2.87331334e+07]
- [-2.58092740e+07]
- [-2.52420060e+07]
- [-2.46732725e+07]
- [-2.41015904e+07]
- [-2.35254401e+07]
- [-2.29432460e+07]
- [-2.23533554e+07]
- [-2.11423544e+07]
- [-1.98773927e+07]
- [-1.85391577e+07]
- [-1.74413297e+07]
- [-1.66258956e+07]
- [-1.58104615e+07]
- [-1.54027444e+07]
- [-1.49950274e+07]
- [-1.45873103e+07]
- [-1.27305439e+07]
- [-1.18515418e+07]
- [-1.09719070e+07]
- [-1.01911563e+07]
- [-9.43096813e+06]
- [-8.69150452e+06]
- [-8.34177167e+06]
- [-8.01848614e+06]
- [-7.72186527e+06]
- [-7.47824924e+06]
- [-7.26235587e+06]
- [ 1.31112756e-08]]</t>
+          <t>[[-3.61233470e+07]
+ [-3.39607908e+07]
+ [-3.14216919e+07]
+ [-3.08798497e+07]
+ [-3.03368469e+07]
+ [-2.97915093e+07]
+ [-2.91813292e+07]
+ [-2.85663641e+07]
+ [-2.79453063e+07]
+ [-2.66588125e+07]
+ [-2.53296474e+07]
+ [-2.39426102e+07]
+ [-2.27808618e+07]
+ [-2.18420221e+07]
+ [-2.09031825e+07]
+ [-2.04841515e+07]
+ [-2.00651205e+07]
+ [-1.96460895e+07]
+ [-1.74269003e+07]
+ [-1.61860231e+07]
+ [-1.49446247e+07]
+ [-1.32233993e+07]
+ [-1.15016608e+07]
+ [-9.77942261e+06]
+ [-9.09862410e+06]
+ [-8.46264681e+06]
+ [-7.87173034e+06]
+ [-7.57979326e+06]
+ [-7.31395379e+06]
+ [ 4.36557457e-10]]</t>
         </is>
       </c>
       <c r="E296" t="inlineStr"/>
@@ -7692,36 +7689,36 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>[[-3.63043218e+06]
- [-8.19889984e+06]
- [-7.77011821e+06]
- [ 2.42805699e+06]
- [ 2.42807339e+06]
- [ 2.42809013e+06]
- [ 2.42810734e+06]
- [ 2.42812517e+06]
- [ 2.42814377e+06]
- [ 2.42842043e+06]
- [ 2.42850789e+06]
- [ 2.42860900e+06]
- [ 2.42859940e+06]
- [ 2.42842601e+06]
- [ 2.42846531e+06]
- [ 2.42820988e+06]
- [ 2.42821936e+06]
- [ 2.42822873e+06]
- [ 2.42883824e+06]
- [ 2.42928308e+06]
- [ 2.42968212e+06]
- [ 2.43001408e+06]
- [ 2.43058263e+06]
- [ 2.43102787e+06]
- [ 2.42957454e+06]
- [ 2.42957782e+06]
- [ 2.42954745e+06]
- [ 2.42932438e+06]
- [ 2.42919063e+06]
- [ 1.07860585e+03]]</t>
+          <t>[[-3.57138685e+06]
+ [-8.98099977e+06]
+ [-9.16012717e+06]
+ [ 2.42809383e+06]
+ [ 2.42811353e+06]
+ [ 2.42813357e+06]
+ [ 2.42817756e+06]
+ [ 2.42819807e+06]
+ [ 2.42821930e+06]
+ [ 2.42858830e+06]
+ [ 2.42868472e+06]
+ [ 2.42879347e+06]
+ [ 2.42877271e+06]
+ [ 2.42862009e+06]
+ [ 2.42867077e+06]
+ [ 2.42827583e+06]
+ [ 2.42828803e+06]
+ [ 2.42830009e+06]
+ [ 2.42942913e+06]
+ [ 2.43011791e+06]
+ [ 2.43073661e+06]
+ [ 2.43274959e+06]
+ [ 2.43367362e+06]
+ [ 2.43439828e+06]
+ [ 2.43070100e+06]
+ [ 2.43067999e+06]
+ [ 2.43061537e+06]
+ [ 2.42932413e+06]
+ [ 2.42922801e+06]
+ [ 1.14939088e+03]]</t>
         </is>
       </c>
       <c r="E297" t="inlineStr"/>
@@ -7744,36 +7741,36 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>[[-4.74109260e+04]
- [-1.07349005e+05]
- [-1.02767235e+05]
- [ 2.90964415e+04]
- [ 2.90966558e+04]
- [ 2.90968748e+04]
- [ 2.90971001e+04]
- [ 2.90973335e+04]
- [ 2.90975772e+04]
- [ 2.91011873e+04]
- [ 2.91023351e+04]
- [ 2.91036633e+04]
- [ 2.91035461e+04]
- [ 2.91012847e+04]
- [ 2.91018057e+04]
- [ 2.90984616e+04]
- [ 2.90985878e+04]
- [ 2.90987125e+04]
- [ 2.91067528e+04]
- [ 2.91127423e+04]
- [ 2.91181795e+04]
- [ 2.91228650e+04]
- [ 2.91309879e+04]
- [ 2.91376687e+04]
- [ 2.91178825e+04]
- [ 2.91183035e+04]
- [ 2.91183766e+04]
- [ 2.91157463e+04]
- [ 2.91146263e+04]
- [ 1.75412890e+01]]</t>
+          <t>[[-4.66127963e+04]
+ [-1.17471936e+05]
+ [-1.20846423e+05]
+ [ 2.90969215e+04]
+ [ 2.90971790e+04]
+ [ 2.90974409e+04]
+ [ 2.90980156e+04]
+ [ 2.90982842e+04]
+ [ 2.90985623e+04]
+ [ 2.91033773e+04]
+ [ 2.91046427e+04]
+ [ 2.91060712e+04]
+ [ 2.91058090e+04]
+ [ 2.91038216e+04]
+ [ 2.91044932e+04]
+ [ 2.90993237e+04]
+ [ 2.90994860e+04]
+ [ 2.90996465e+04]
+ [ 2.91145355e+04]
+ [ 2.91238056e+04]
+ [ 2.91322314e+04]
+ [ 2.91595534e+04]
+ [ 2.91726762e+04]
+ [ 2.91834001e+04]
+ [ 2.91331718e+04]
+ [ 2.91333875e+04]
+ [ 2.91331398e+04]
+ [ 2.91153261e+04]
+ [ 2.91149474e+04]
+ [ 1.84960460e+01]]</t>
         </is>
       </c>
       <c r="E298" t="inlineStr"/>
@@ -7796,36 +7793,36 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>[[-6.71569389e+05]
- [-2.55654527e+06]
- [-4.64940832e+06]
- [-5.41255550e+06]
- [-5.36378052e+06]
- [-5.31498183e+06]
- [-5.26616111e+06]
- [-5.21732007e+06]
- [-5.16846045e+06]
- [-5.07068172e+06]
- [-4.97284837e+06]
- [-4.87497595e+06]
- [-4.77708115e+06]
- [-4.67916450e+06]
- [-4.58122078e+06]
- [-4.53224756e+06]
- [-4.48327101e+06]
- [-4.43429200e+06]
- [-4.07857587e+06]
- [-3.72106632e+06]
- [-3.36222737e+06]
- [-2.84687235e+06]
- [-2.32838009e+06]
- [-1.80776549e+06]
- [-1.49481546e+06]
- [-1.18119602e+06]
- [-8.66936826e+05]
- [-5.73109442e+05]
- [-2.78840152e+05]
- [-4.49704115e-04]]</t>
+          <t>[[-5.26598777e+05]
+ [-2.40607156e+06]
+ [-4.71519835e+06]
+ [-5.43134918e+06]
+ [-5.38239525e+06]
+ [-5.33340277e+06]
+ [-5.28437798e+06]
+ [-5.23532560e+06]
+ [-5.18624767e+06]
+ [-5.08801102e+06]
+ [-4.98969900e+06]
+ [-4.89132947e+06]
+ [-4.79291850e+06]
+ [-4.69446588e+06]
+ [-4.59596973e+06]
+ [-4.54671512e+06]
+ [-4.49744951e+06]
+ [-4.44817413e+06]
+ [-4.08976416e+06]
+ [-3.72869453e+06]
+ [-3.36567846e+06]
+ [-2.84455227e+06]
+ [-2.32217436e+06]
+ [-1.80001961e+06]
+ [-1.48754428e+06]
+ [-1.17506364e+06]
+ [-8.62644874e+05]
+ [-5.70954763e+05]
+ [-2.78858769e+05]
+ [-4.93283089e-04]]</t>
         </is>
       </c>
       <c r="E299" t="inlineStr"/>
@@ -7848,36 +7845,36 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>[[ 5.16435012e+07]
- [ 1.96221076e+08]
- [ 3.55840560e+08]
- [ 4.14083720e+08]
- [ 4.10015355e+08]
- [ 4.05945179e+08]
- [ 4.01873324e+08]
- [ 3.97799923e+08]
- [ 3.93725110e+08]
- [ 3.85570964e+08]
- [ 3.77412692e+08]
- [ 3.69251492e+08]
- [ 3.61088644e+08]
- [ 3.52924192e+08]
- [ 3.44757740e+08]
- [ 3.40674436e+08]
- [ 3.36590896e+08]
- [ 3.32507186e+08]
- [ 3.02856876e+08]
- [ 2.73073876e+08]
- [ 2.43194183e+08]
- [ 2.00313765e+08]
- [ 1.57216393e+08]
- [ 1.13983004e+08]
- [ 8.80131860e+07]
- [ 6.20098904e+07]
- [ 3.59815986e+07]
- [ 1.16790315e+07]
- [-1.26133766e+07]
- [ 2.76522860e-02]]</t>
+          <t>[[ 4.05032729e+07]
+ [ 1.84726748e+08]
+ [ 3.60998049e+08]
+ [ 4.15644529e+08]
+ [ 4.11562418e+08]
+ [ 4.07477361e+08]
+ [ 4.03389850e+08]
+ [ 3.99300236e+08]
+ [ 3.95208680e+08]
+ [ 3.87019429e+08]
+ [ 3.78824481e+08]
+ [ 3.70625212e+08]
+ [ 3.62422859e+08]
+ [ 3.54217416e+08]
+ [ 3.46008748e+08]
+ [ 3.41903950e+08]
+ [ 3.37798342e+08]
+ [ 3.33692018e+08]
+ [ 3.03837180e+08]
+ [ 2.73785524e+08]
+ [ 2.43592339e+08]
+ [ 2.00279949e+08]
+ [ 1.56888351e+08]
+ [ 1.13528454e+08]
+ [ 8.75813616e+07]
+ [ 6.16446447e+07]
+ [ 3.57262528e+07]
+ [ 1.15515326e+07]
+ [-1.26120054e+07]
+ [ 3.06533657e-02]]</t>
         </is>
       </c>
       <c r="E300" t="inlineStr"/>
@@ -7900,35 +7897,35 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>[[ 214260.6777001 ]
- [ 468224.68710593]
- [ 808955.83756311]
- [1299593.325459  ]
- [1299590.41838053]
- [1299587.50380529]
- [1299584.57413213]
- [1299581.62157415]
- [1299578.63805818]
- [1299575.61511389]
- [1299569.40928209]
- [1299562.92698901]
- [1299556.06927721]
- [1299550.44357231]
- [1299546.26499681]
- [1299542.08644818]
- [1299539.99718394]
- [1299537.90792641]
- [1299696.76647942]
- [1299681.58766421]
- [1299666.35950518]
- [1299768.53255836]
- [1299754.66513967]
- [1299740.60683059]
- [1299789.23811668]
- [1299802.18781541]
- [1299818.66277765]
- [1299852.92757498]
- [1299889.66301773]
+          <t>[[ 214069.90260215]
+ [ 467905.66188862]
+ [ 808663.37487048]
+ [1299618.86705817]
+ [1299616.14571376]
+ [1299613.41855259]
+ [1299591.46407197]
+ [1299588.79319843]
+ [1299586.10139144]
+ [1299580.91306006]
+ [1299575.39564019]
+ [1299569.69526414]
+ [1299567.63171611]
+ [1299562.46088873]
+ [1299558.28223587]
+ [1299565.29142155]
+ [1299563.2020827 ]
+ [1299561.11275055]
+ [1299689.5032564 ]
+ [1299674.34321372]
+ [1299659.155116  ]
+ [1299649.59058574]
+ [1299627.87565582]
+ [1299606.15497853]
+ [1299648.86747394]
+ [1299648.21346755]
+ [1299648.45194692]
+ [1299792.67972821]
+ [1299811.89339675]
  [      0.        ]]</t>
         </is>
       </c>
@@ -8074,7 +8071,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>[12.43319258]</t>
+          <t>[11.]</t>
         </is>
       </c>
       <c r="E306" t="inlineStr"/>
@@ -8626,7 +8623,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>[2150911.87879668]</t>
+          <t>[3187423.76365581]</t>
         </is>
       </c>
       <c r="E330" t="inlineStr"/>
@@ -8649,7 +8646,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>[658532.04559183]</t>
+          <t>[1175518.62964259]</t>
         </is>
       </c>
       <c r="E331" t="inlineStr"/>
@@ -8672,7 +8669,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>[3095911.87879668]</t>
+          <t>[4132423.76365581]</t>
         </is>
       </c>
       <c r="E332" t="inlineStr"/>
@@ -8695,7 +8692,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>[206.39412525]</t>
+          <t>[275.49491758]</t>
         </is>
       </c>
       <c r="E333" t="inlineStr"/>
@@ -8718,7 +8715,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>[658532.04559183]</t>
+          <t>[1175518.62964259]</t>
         </is>
       </c>
       <c r="E334" t="inlineStr"/>
@@ -8787,7 +8784,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>[2150911.87879668]</t>
+          <t>[3187423.76365581]</t>
         </is>
       </c>
       <c r="E337" t="inlineStr"/>
@@ -8810,7 +8807,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>[2150911.87879668]</t>
+          <t>[3187423.76365581]</t>
         </is>
       </c>
       <c r="E338" t="inlineStr"/>
@@ -8833,9 +8830,9 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>[417.76067857 480.09738431 523.65058445 557.91160668 581.92125008
- 597.20357718 606.4643562  576.1548744  542.98427067 506.9184334
- 460.2271512  409.29061826 353.04163049]</t>
+          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
+ 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
+ 427.60678303 391.57616974 352.18249915]</t>
         </is>
       </c>
       <c r="E339" t="inlineStr"/>
@@ -9050,9 +9047,9 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 12.43319278 12.43319278 12.09875903 11.76432528
- 11.42989152 10.58683885  9.74378618  8.90073352  7.93776698  6.97480044
-  6.01183391]</t>
+          <t>[10.         10.         10.         10.         10.         10.
+ 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
+  5.999     ]</t>
         </is>
       </c>
       <c r="E348" t="inlineStr"/>
@@ -9146,9 +9143,9 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>[417.76067857 480.09738431 523.65058445 557.91160668 581.92125008
- 597.20357718 606.4643562  576.1548744  542.98427067 506.9184334
- 460.2271512  409.29061826 353.04163049]</t>
+          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
+ 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
+ 427.60678303 391.57616974 352.18249915]</t>
         </is>
       </c>
       <c r="E352" t="inlineStr"/>
@@ -9288,9 +9285,9 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>[-417.76067857 -480.09738431 -523.65058445 -557.91160668 -581.92125008
- -597.20357718 -606.4643562  -576.1548744  -542.98427067 -506.9184334
- -460.2271512  -409.29061826 -353.04163049]</t>
+          <t>[-336.9560439  -388.43785582 -424.16473764 -452.12457083 -484.27449749
+ -510.65946695 -533.22010636 -511.58791739 -487.37587695 -460.61782438
+ -427.60678303 -391.57616974 -352.18249915]</t>
         </is>
       </c>
       <c r="E358" t="inlineStr"/>
@@ -9338,7 +9335,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 11.42989152  8.90073352  6.01183391]</t>
+          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
         </is>
       </c>
       <c r="E360" t="inlineStr"/>
@@ -9361,7 +9358,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>[0.02268044 0.0142022  0.01174385 0.01142884]</t>
+          <t>[0.04     0.038801 0.026301 0.015   ]</t>
         </is>
       </c>
       <c r="E361" t="inlineStr"/>
@@ -9426,7 +9423,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 11.42989152  8.90073352  6.01183391]</t>
+          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
         </is>
       </c>
       <c r="E364" t="inlineStr"/>
@@ -9449,7 +9446,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>[0.02268044 0.0142022  0.01174385 0.01142884]</t>
+          <t>[0.04     0.038801 0.026301 0.015   ]</t>
         </is>
       </c>
       <c r="E365" t="inlineStr"/>
@@ -9685,8 +9682,8 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>[0.02268044 0.02268044 0.02268044 0.0142022  0.0142022  0.0142022
- 0.01174385 0.01174385 0.01174385 0.01142884 0.01142884 0.01142884]</t>
+          <t>[0.04     0.04     0.04     0.038801 0.038801 0.038801 0.026301 0.026301
+ 0.026301 0.015    0.015    0.015   ]</t>
         </is>
       </c>
       <c r="E375" t="inlineStr"/>
@@ -9869,8 +9866,8 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>[0.94618249 0.94618249 0.94618249 0.58490872 0.5689426  0.55297649
- 0.43411361 0.40083242 0.36755123 0.32301245 0.28601711 0.24902177]</t>
+          <t>[1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
+ 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
         </is>
       </c>
       <c r="E383" t="inlineStr"/>
@@ -9893,8 +9890,8 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>[0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E384" t="inlineStr"/>
@@ -9917,8 +9914,8 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>[0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E385" t="inlineStr"/>
@@ -9941,8 +9938,8 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>[18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E386" t="inlineStr"/>
@@ -9965,8 +9962,8 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>[18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E387" t="inlineStr"/>
@@ -9989,8 +9986,8 @@
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>[36.43307152 36.43307152 36.43307152 21.94960044 20.2007613  18.54737303
- 13.12388581 10.33096399  7.96537229  5.70856597  3.96319571  2.6156629 ]</t>
+          <t>[33.21380796 33.21380796 33.21380796 32.22982785 32.22982785 32.22982785
+ 19.88323673 16.18153341 12.97038057  5.79213059  4.36751812  3.19804084]</t>
         </is>
       </c>
       <c r="E388" t="inlineStr"/>
@@ -10084,17 +10081,17 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>[[-12730521.72143568]
- [-11850886.87887046]
- [-10970787.07175203]
- [-10189538.98252747]
- [ -9429015.43524477]
- [ -8689342.32671024]
- [ -8339717.27880802]
- [ -8016756.87143007]
- [ -7720490.61221403]
- [ -7477270.18058252]
- [ -7261843.49422376]
+          <t>[[-17427765.12991663]
+ [-16186366.78221211]
+ [-14944587.88685458]
+ [-13222849.37497341]
+ [-11500611.20008019]
+ [ -9777955.21838797]
+ [ -9097151.95187112]
+ [ -8461409.45930777]
+ [ -7870754.04360263]
+ [ -7579102.67267725]
+ [ -7313593.23878349]
  [ -7074256.2758736 ]]</t>
         </is>
       </c>
@@ -10118,18 +10115,18 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>[[2428202.60258269]
- [2428678.38301451]
- [2429111.49063849]
- [2429560.06791994]
- [2430215.49135759]
- [2430750.37827718]
- [2429479.23253397]
- [2429523.57455143]
- [2429538.88915186]
- [2429361.17520323]
- [2429276.72132152]
- [2429134.03768572]]</t>
+          <t>[[2428340.58969823]
+ [2429076.44059267]
+ [2429745.66121794]
+ [2431464.41489253]
+ [2432495.54674606]
+ [2433328.43446587]
+ [2430320.56243432]
+ [2430367.54182217]
+ [2430375.83291243]
+ [2429248.39987909]
+ [2429220.83731715]
+ [2429127.58409672]]</t>
         </is>
       </c>
       <c r="E393" t="inlineStr"/>
@@ -10152,18 +10149,18 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>[[29098.38222475]
- [29104.74146934]
- [29110.58948486]
- [29116.76283907]
- [29125.95242289]
- [29133.73436025]
- [29116.45599326]
- [29117.39204292]
- [29118.03862504]
- [29115.99795827]
- [29115.49432309]
- [29114.44234276]]</t>
+          <t>[[29100.21334624]
+ [29110.04393666]
+ [29119.07546929]
+ [29142.38007936]
+ [29156.79240186]
+ [29168.82090949]
+ [29127.92088216]
+ [29128.99893601]
+ [29129.67529452]
+ [29114.12772248]
+ [29114.60165251]
+ [29114.41196808]]</t>
         </is>
       </c>
       <c r="E394" t="inlineStr"/>
@@ -10186,18 +10183,18 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>[[-4361007.15030931]
- [-4006298.04736741]
- [-3649931.2024322 ]
- [-3137543.02001618]
- [-2621388.15215144]
- [-2102512.96128891]
- [-1790296.78649906]
- [-1477154.77232377]
- [-1163071.91054673]
- [ -869072.3886961 ]
- [ -574194.72779434]
- [ -278501.85530974]]</t>
+          <t>[[-4355770.84979259]
+ [-3999369.51509918]
+ [-3640497.12021613]
+ [-3124519.02847233]
+ [-2606354.23982125]
+ [-2087563.38387338]
+ [-1776650.06345185]
+ [-1465466.49623692]
+ [-1154071.36764904]
+ [ -862996.74568595]
+ [ -571078.64832484]
+ [ -278501.90073832]]</t>
         </is>
       </c>
       <c r="E395" t="inlineStr"/>
@@ -10220,18 +10217,18 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>[[ 3.26275934e+08]
- [ 2.96704586e+08]
- [ 2.67010748e+08]
- [ 2.24351073e+08]
- [ 1.81424129e+08]
- [ 1.38313439e+08]
- [ 1.12392639e+08]
- [ 8.64176612e+07]
- [ 6.03932815e+07]
- [ 3.60669741e+07]
- [ 1.17151829e+07]
- [-1.26341964e+07]]</t>
+          <t>[[ 3.26042330e+08]
+ [ 2.96343964e+08]
+ [ 2.66462894e+08]
+ [ 2.23535771e+08]
+ [ 1.80456648e+08]
+ [ 1.37343596e+08]
+ [ 1.11509659e+08]
+ [ 8.56652885e+07]
+ [ 5.98176693e+07]
+ [ 3.56818040e+07]
+ [ 1.15214098e+07]
+ [-1.26341969e+07]]</t>
         </is>
       </c>
       <c r="E396" t="inlineStr"/>
@@ -10254,18 +10251,18 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>[[1299696.81579559]
- [1299681.58727972]
- [1299666.34815927]
- [1299768.50116918]
- [1299754.61853755]
- [1299740.54894056]
- [1299789.15645825]
- [1299802.10378469]
- [1299818.58563886]
- [1299852.85779559]
- [1299889.60688801]
- [1299939.10849629]]</t>
+          <t>[[1299689.54225215]
+ [1299674.3537992 ]
+ [1299659.15932317]
+ [1299649.59012126]
+ [1299627.86871814]
+ [1299606.14173766]
+ [1299648.83929164]
+ [1299648.18318422]
+ [1299648.4245459 ]
+ [1299792.63859019]
+ [1299811.86142551]
+ [1299836.63664036]]</t>
         </is>
       </c>
       <c r="E397" t="inlineStr"/>
@@ -10439,19 +10436,19 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>[[-417.76067857]
- [-480.09738431]
- [-523.65058445]
- [-557.91160668]
- [-581.92125008]
- [-597.20357718]
- [-606.4643562 ]
- [-576.1548744 ]
- [-542.98427067]
- [-506.9184334 ]
- [-460.2271512 ]
- [-409.29061826]
- [-353.04163049]]</t>
+          <t>[[-336.9560439 ]
+ [-388.43785582]
+ [-424.16473764]
+ [-452.12457083]
+ [-484.27449749]
+ [-510.65946695]
+ [-533.22010636]
+ [-511.58791739]
+ [-487.37587695]
+ [-460.61782438]
+ [-427.60678303]
+ [-391.57616974]
+ [-352.18249915]]</t>
         </is>
       </c>
       <c r="E403" t="inlineStr"/>
@@ -10474,7 +10471,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>[658532.04559183]</t>
+          <t>[1175518.62964259]</t>
         </is>
       </c>
       <c r="E404" t="inlineStr"/>
@@ -10497,7 +10494,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>[57.02694138]</t>
+          <t>[59.4435992]</t>
         </is>
       </c>
       <c r="E405" t="inlineStr"/>
@@ -10520,7 +10517,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>[3.22713234e+09 3.22713234e+09 2.19266101e+07 0.00000000e+00
+          <t>[5.79150755e+09 5.79150755e+09 2.73584130e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -10575,10 +10572,10 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          96476.17864374
-  96918.90641228  98252.45317392 100493.08222435 103668.49141771
- 107818.75539867 112997.76167827 126739.70475695 145701.26866961
- 171147.80374315      0.              0.              0.
+          <t>[     0.              0.              0.          76069.22818689
+  76419.81487525  77475.80310771  79250.00595527  81764.21915156
+  85049.92502601  89149.36708317 100022.09247963 115010.75107985
+ 135096.15327474      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -10829,10 +10826,10 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          96476.17864374
-  96918.90641228  98252.45317392 100493.08222435 103668.49141771
- 107818.75539867 112997.76167827 126739.70475695 145701.26866961
- 171147.80374315      0.              0.              0.
+          <t>[     0.              0.              0.          76069.22818689
+  76419.81487525  77475.80310771  79250.00595527  81764.21915156
+  85049.92502601  89149.36708317 100022.09247963 115010.75107985
+ 135096.15327474      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -11214,10 +11211,10 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>[      0.               0.               0.          -96476.17864374
-  -96918.90641228  -98252.45317392 -100493.08222435 -103668.49141771
- -107818.75539867 -112997.76167827 -126739.70475695 -145701.26866961
- -171147.80374315       0.               0.               0.
+          <t>[      0.               0.               0.          -76069.22818689
+  -76419.81487525  -77475.80310771  -79250.00595527  -81764.21915156
+  -85049.92502601  -89149.36708317 -100022.09247963 -115010.75107985
+ -135096.15327474       0.               0.               0.
        0.               0.               0.        ]</t>
         </is>
       </c>
@@ -11264,8 +11261,8 @@
       <c r="C436" t="inlineStr"/>
       <c r="D436" t="inlineStr">
         <is>
-          <t>[161.4700302  161.47003319 161.47003544 161.47003598 161.47003609
- 161.47003609]</t>
+          <t>[142.85714286 123.62540609 107.61766064 105.42408783 109.45138599
+ 122.73537912]</t>
         </is>
       </c>
       <c r="E436" t="inlineStr"/>
@@ -11284,7 +11281,7 @@
       <c r="C437" t="inlineStr"/>
       <c r="D437" t="inlineStr">
         <is>
-          <t>[0.99999999 1.         0.99999999 1.         1.         1.        ]</t>
+          <t>[1. 1. 1. 1. 1. 1.]</t>
         </is>
       </c>
       <c r="E437" t="inlineStr"/>
@@ -11303,7 +11300,7 @@
       <c r="C438" t="inlineStr"/>
       <c r="D438" t="inlineStr">
         <is>
-          <t>[1.00000001 1.         1.00000001 1.         1.         1.        ]</t>
+          <t>[1. 1. 1. 1. 1. 1.]</t>
         </is>
       </c>
       <c r="E438" t="inlineStr"/>
@@ -11322,7 +11319,7 @@
       <c r="C439" t="inlineStr"/>
       <c r="D439" t="inlineStr">
         <is>
-          <t>[0.99999999 0.99999999 1.         1.         1.        ]</t>
+          <t>[1.1555646  1.14874645 1.02080713 0.96320469 0.89176721]</t>
         </is>
       </c>
       <c r="E439" t="inlineStr"/>
@@ -11366,10 +11363,8 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>[6.21659629 6.21659631 6.21659633 6.21659635 6.21659635 6.21659635
- 6.21659635 6.21659636 6.21659637 6.21659638 6.21659638 6.21659639
- 6.21659639 6.21659639 6.21659639 6.21659639 6.21659639 6.21659639
- 6.21659639]</t>
+          <t>[5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5
+ 5.5]</t>
         </is>
       </c>
       <c r="E441" t="inlineStr"/>
@@ -11392,7 +11387,7 @@
       </c>
       <c r="D442" t="inlineStr">
         <is>
-          <t>[  0.           0.         -24.99999986]</t>
+          <t>[  0.   0. -25.]</t>
         </is>
       </c>
       <c r="E442" t="inlineStr"/>
@@ -11415,7 +11410,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>[6070.51048865]</t>
+          <t>[4751.65888855]</t>
         </is>
       </c>
       <c r="E443" t="inlineStr"/>
@@ -11438,7 +11433,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>[61017664.84818722]</t>
+          <t>[47761243.48631421]</t>
         </is>
       </c>
       <c r="E444" t="inlineStr"/>
@@ -11457,7 +11452,7 @@
       <c r="C445" t="inlineStr"/>
       <c r="D445" t="inlineStr">
         <is>
-          <t>[3.]</t>
+          <t>[2.]</t>
         </is>
       </c>
       <c r="E445" t="inlineStr"/>
@@ -11480,7 +11475,7 @@
       </c>
       <c r="D446" t="inlineStr">
         <is>
-          <t>[121.4102117]</t>
+          <t>[95.03317777]</t>
         </is>
       </c>
       <c r="E446" t="inlineStr"/>
@@ -11503,7 +11498,7 @@
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>[1173.00690535]</t>
+          <t>[718.68840689]</t>
         </is>
       </c>
       <c r="E447" t="inlineStr"/>
@@ -11526,7 +11521,7 @@
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>[1173.00690535]</t>
+          <t>[718.68840689]</t>
         </is>
       </c>
       <c r="E448" t="inlineStr"/>
@@ -11549,8 +11544,8 @@
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>[6.22227325e+06 6.22227325e+06 3.28337599e+05 1.29637240e+09
- 1.29637240e+09 0.00000000e+00]</t>
+          <t>[4.87045036e+06 4.87045036e+06 2.27379167e+05 1.01472840e+09
+ 1.01472840e+09 0.00000000e+00]</t>
         </is>
       </c>
       <c r="E449" t="inlineStr"/>
@@ -11622,10 +11617,8 @@
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>[12.43319258 12.43319262 12.43319266 12.4331927  12.4331927  12.4331927
- 12.4331927  12.43319272 12.43319274 12.43319276 12.43319277 12.43319277
- 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278
- 12.43319278]</t>
+          <t>[11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11.
+ 11.]</t>
         </is>
       </c>
       <c r="E452" t="inlineStr"/>
@@ -11879,8 +11872,8 @@
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>[24946.15748256 24946.15725121 24946.15703844 24946.15712251
- 24946.15713978 24946.15713979]</t>
+          <t>[22052.65645424 25455.32343855 29206.24191018 29808.12162885
+ 28721.4392631  25638.39882899]</t>
         </is>
       </c>
       <c r="E463" t="inlineStr">
@@ -11907,8 +11900,8 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>[476101.86060254 476101.86064991 476101.85919272 476101.86400614
- 476101.86499502 476101.8649954 ]</t>
+          <t>[328909.46641626 378833.46697552 433611.1778083  442375.93663105
+ 426546.30836535 381513.2936722 ]</t>
         </is>
       </c>
       <c r="E464" t="inlineStr">
@@ -11935,8 +11928,8 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>[476101.86060254 476101.86064991 476101.85919272 476101.86400614
- 476101.86499502 476101.8649954 ]</t>
+          <t>[328909.46641626 378833.46697552 433611.1778083  442375.93663105
+ 426546.30836535 381513.2936722 ]</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
@@ -11963,8 +11956,8 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>[1.14091028e+13 1.14091028e+13 1.14091028e+13 1.14091029e+13
- 1.14091029e+13 1.14091029e+13]</t>
+          <t>[7.88184679e+12 9.07820434e+12 1.03908741e+13 1.06009091e+13
+ 1.02215746e+13 9.14242257e+12]</t>
         </is>
       </c>
       <c r="E466" t="inlineStr">
@@ -11991,8 +11984,8 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>[1.14091028e+13 1.14091028e+13 1.14091028e+13 1.14091029e+13
- 1.14091029e+13 1.14091029e+13]</t>
+          <t>[7.88184679e+12 9.07820434e+12 1.03908741e+13 1.06009091e+13
+ 1.02215746e+13 9.14242257e+12]</t>
         </is>
       </c>
       <c r="E467" t="inlineStr">
@@ -12019,8 +12012,8 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>[9.04741853e+12 9.04741854e+12 9.04741851e+12 9.04741860e+12
- 9.04741862e+12 9.04741862e+12]</t>
+          <t>[6.25030450e+12 7.19901604e+12 8.23996319e+12 8.40652091e+12
+ 8.10570866e+12 7.24994109e+12]</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
@@ -12047,8 +12040,8 @@
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>[5.97799125e+11 5.97799119e+11 5.97799114e+11 5.97799116e+11
- 5.97799117e+11 5.97799117e+11]</t>
+          <t>[5.28460495e+11 6.10000562e+11 6.99885979e+11 7.14309169e+11
+ 6.88268374e+11 6.14387703e+11]</t>
         </is>
       </c>
       <c r="E469" t="inlineStr">
@@ -12156,12 +12149,12 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>[[0.         0.         0.33456054 0.10897608 0.10897608 0.        ]
- [0.         0.         0.33456055 0.10897608 0.10897608 0.        ]
- [0.         0.         0.33456055 0.10897608 0.10897608 0.        ]
- [0.         0.         0.33456055 0.10897608 0.10897608 0.        ]
- [0.         0.         0.33456055 0.10897608 0.10897608 0.        ]
- [0.         0.         0.33456055 0.10897608 0.10897608 0.        ]]</t>
+          <t>[[0.         0.         0.37845781 0.1395612  0.1395612  0.        ]
+ [0.         0.         0.32786855 0.12116934 0.12116934 0.        ]
+ [0.         0.         0.28576083 0.10586212 0.10586212 0.        ]
+ [0.         0.         0.27999081 0.10376469 0.10376469 0.        ]
+ [0.         0.         0.29058432 0.10761551 0.10761551 0.        ]
+ [0.         0.         0.32552735 0.12031822 0.12031822 0.        ]]</t>
         </is>
       </c>
       <c r="E473" t="inlineStr"/>
@@ -12184,12 +12177,12 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>[[0.54946421 0.54946421 0.         0.         0.         0.05448804]
- [0.54946422 0.54946422 0.         0.         0.         0.05448804]
- [0.54946422 0.54946422 0.         0.         0.         0.05448804]
- [0.54946422 0.54946422 0.         0.         0.         0.05448804]
- [0.54946422 0.54946422 0.         0.         0.         0.05448804]
- [0.54946422 0.54946422 0.         0.         0.         0.05448804]]</t>
+          <t>[[0.62132644 0.62132644 0.         0.         0.         0.0697806 ]
+ [0.53799878 0.53799878 0.         0.         0.         0.06058467]
+ [0.4686384  0.4686384  0.         0.         0.         0.05293106]
+ [0.45913365 0.45913365 0.         0.         0.         0.05188234]
+ [0.4765839  0.4765839  0.         0.         0.         0.05380776]
+ [0.53414241 0.53414241 0.         0.         0.         0.06015911]]</t>
         </is>
       </c>
       <c r="E474" t="inlineStr"/>
@@ -12212,7 +12205,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>[1189.99671226]</t>
+          <t>[1184.91130973]</t>
         </is>
       </c>
       <c r="E475" t="inlineStr"/>
@@ -12235,7 +12228,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>[3961795.23695627]</t>
+          <t>[3980261.24221089]</t>
         </is>
       </c>
       <c r="E476" t="inlineStr"/>
@@ -12258,7 +12251,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>[1621500.22424683]</t>
+          <t>[1648375.1234354]</t>
         </is>
       </c>
       <c r="E477" t="inlineStr"/>
@@ -12281,7 +12274,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>[32.4999999]</t>
+          <t>[34.4331827]</t>
         </is>
       </c>
       <c r="E478" t="inlineStr"/>
@@ -12304,7 +12297,7 @@
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>[2.31455943e+09 2.31455943e+09 6.18932421e+07 0.00000000e+00
+          <t>[2.54169442e+09 2.54169442e+09 4.90525923e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -12328,9 +12321,7 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>[12.4331926  12.43319264 12.43319268 12.4331927  12.4331927  12.4331927
- 12.43319271 12.43319273 12.43319275 12.43319276 12.43319277 12.43319278
- 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278]</t>
+          <t>[11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11.]</t>
         </is>
       </c>
       <c r="E480" t="inlineStr"/>
@@ -12353,8 +12344,9 @@
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>[0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239
- 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239]</t>
+          <t>[0.08239    0.08239    0.08239    0.09520697 0.09520697 0.09520697
+ 0.10936867 0.10936867 0.10936867 0.11164431 0.11164431 0.11164431
+ 0.10753633 0.10753633 0.10753633 0.09589737 0.09589737 0.09589737]</t>
         </is>
       </c>
       <c r="E481" t="inlineStr"/>
@@ -12402,7 +12394,7 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>[1721500.22424683]</t>
+          <t>[1748375.1234354]</t>
         </is>
       </c>
       <c r="E483" t="inlineStr"/>
@@ -12425,7 +12417,7 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>[4461795.23695627]</t>
+          <t>[4480261.24221089]</t>
         </is>
       </c>
       <c r="E484" t="inlineStr"/>
@@ -12448,7 +12440,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>[34.38788813]</t>
+          <t>[36.18148127]</t>
         </is>
       </c>
       <c r="E485" t="inlineStr"/>
@@ -12471,7 +12463,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>[2.73899173e+09 2.73899173e+09 6.57578491e+07 0.00000000e+00
+          <t>[2.96570692e+09 2.96570692e+09 5.20775923e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -12495,7 +12487,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>[2380032.26983866]</t>
+          <t>[2923893.75307798]</t>
         </is>
       </c>
       <c r="E487" t="inlineStr"/>
@@ -12518,7 +12510,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>[6612707.11575295]</t>
+          <t>[7667685.0058667]</t>
         </is>
       </c>
       <c r="E488" t="inlineStr"/>
@@ -12568,7 +12560,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>[0.22]</t>
+          <t>[0.21999755]</t>
         </is>
       </c>
       <c r="E490" t="inlineStr"/>
@@ -12591,7 +12583,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>[0.22187621]</t>
+          <t>[0.22134505]</t>
         </is>
       </c>
       <c r="E491" t="inlineStr"/>
@@ -12614,7 +12606,7 @@
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>[0.22       0.22187621 0.8304938  1.01982627 1.1957237  2.45336155]</t>
+          <t>[0.21999755 0.22134505 0.92117535 1.01638648 1.15669516 2.0485555 ]</t>
         </is>
       </c>
       <c r="E492" t="inlineStr"/>
@@ -12637,7 +12629,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>[0.22187621 1.1957237  2.5212143 ]</t>
+          <t>[0.22134505 1.15669516 2.16529265]</t>
         </is>
       </c>
       <c r="E493" t="inlineStr"/>
@@ -12660,7 +12652,7 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>[0.22       1.01982627 2.45336155]</t>
+          <t>[0.21999755 1.01638648 2.0485555 ]</t>
         </is>
       </c>
       <c r="E494" t="inlineStr"/>
@@ -12683,7 +12675,7 @@
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>[3.84637857 0.         0.        ]</t>
+          <t>[4.49500558 0.         0.        ]</t>
         </is>
       </c>
       <c r="E495" t="inlineStr"/>
@@ -12702,9 +12694,9 @@
       <c r="C496" t="inlineStr"/>
       <c r="D496" t="inlineStr">
         <is>
-          <t>[[  0.37195323   0.44274994   1.81489166  -2.55169117   0.92209633]
- [ -2.3257177   -1.2980874    0.63935322   3.44434889   0.540103  ]
- [ -4.94508763   0.73564094  12.0638034    4.71771665 -11.57207337]]</t>
+          <t>[[ 0.55427077  0.5457551   2.07469104 -4.02909738  1.85438047]
+ [-2.46956588 -0.10350813  6.57977706 -6.90431     3.89760695]
+ [-4.7733934   4.65370807  9.71866059 -1.375797   -7.22317826]]</t>
         </is>
       </c>
       <c r="E496" t="inlineStr"/>
@@ -12723,9 +12715,9 @@
       <c r="C497" t="inlineStr"/>
       <c r="D497" t="inlineStr">
         <is>
-          <t>[[  0.36733967   0.43876625   1.81385353  -2.55230905   0.93234961]
- [ -2.48645309  -1.57703816   0.58940192   2.28884613   2.18524321]
- [ -4.64271728   0.50653213  10.23441017   6.24768797 -11.34591299]]</t>
+          <t>[[ 0.54901338  0.54222202  2.08831205 -4.05198517  1.87243771]
+ [-2.49204522 -0.43200223  7.21681417 -8.90689773  5.61413101]
+ [-4.28862793  3.69929876  8.14639839 -0.02219398 -6.53487523]]</t>
         </is>
       </c>
       <c r="E497" t="inlineStr"/>
@@ -12744,9 +12736,9 @@
       <c r="C498" t="inlineStr"/>
       <c r="D498" t="inlineStr">
         <is>
-          <t>[[ 0.10077492  3.53829425 -6.2784073   6.71388701 -3.07454888]
- [ 0.          0.          0.          0.          0.        ]
- [ 0.          0.          0.          0.          0.        ]]</t>
+          <t>[[ -0.37046014   8.78814819 -22.55378557  24.22299285  -9.08689533]
+ [  0.           0.           0.           0.           0.        ]
+ [  0.           0.           0.           0.           0.        ]]</t>
         </is>
       </c>
       <c r="E498" t="inlineStr"/>
@@ -12765,9 +12757,9 @@
       <c r="C499" t="inlineStr"/>
       <c r="D499" t="inlineStr">
         <is>
-          <t>[[ 0.8487975   0.86885388 -1.77323241  1.75064156 -0.69506053]
- [-1.84147874  5.05088091 -9.34476388 10.26518831 -3.12982659]
- [-0.18103748  0.48469651  6.09960071 -5.80520536  0.40194563]]</t>
+          <t>[[ 1.26998237  0.90469816 -3.80129328  4.14778648 -1.52117373]
+ [-1.38300795  5.21937195 -8.02311143  6.90137788 -1.71463045]
+ [ 0.13856119  4.05804497 -5.24306741  6.15051553 -4.10405427]]</t>
         </is>
       </c>
       <c r="E499" t="inlineStr"/>
@@ -12786,9 +12778,9 @@
       <c r="C500" t="inlineStr"/>
       <c r="D500" t="inlineStr">
         <is>
-          <t>[[  0.83611019   0.89088762  -1.81922801   1.79722771  -0.70499752]
- [ -2.0746146    5.58143877 -10.76823679  11.53535361  -3.27394098]
- [ -0.31040172   0.80428658   4.94779187  -4.41959713  -0.0220796 ]]</t>
+          <t>[[ 1.25695893  0.92266435 -3.81647118  4.14850008 -1.51165218]
+ [-1.5459125   5.31553908 -8.04385047  6.47682499 -1.2026011 ]
+ [-0.12934916  4.35351419 -6.0359276   6.94963259 -4.13787003]]</t>
         </is>
       </c>
       <c r="E500" t="inlineStr"/>
@@ -12807,7 +12799,7 @@
       <c r="C501" t="inlineStr"/>
       <c r="D501" t="inlineStr">
         <is>
-          <t>[[  -6.71232786   52.32449332 -130.13143115  139.35258536  -53.83331968]
+          <t>[[ -24.52354263  191.15304427 -535.87123688  615.41382219 -245.17208694]
  [   0.            0.            0.            0.            0.        ]
  [   0.            0.            0.            0.            0.        ]]</t>
         </is>
@@ -12832,37 +12824,37 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>[[1.57365443e-04]
- [2.71198640e-04]
- [4.03424702e-05]
- [2.31936051e-03]
- [3.08972854e-03]
- [3.95433963e-03]
- [4.91226708e-03]
- [5.96258378e-03]
- [7.10436223e-03]
- [8.33667456e-03]
- [1.10691936e-02]
- [1.41527063e-02]
- [1.75797787e-02]
- [2.13429734e-02]
- [2.54348599e-02]
- [2.98480095e-02]
- [3.21727303e-02]
- [3.45749776e-02]
- [3.70538215e-02]
- [6.22262976e-02]
- [9.95156093e-02]
- [1.47729798e-01]
- [2.39976563e-01]
- [3.60508565e-01]
- [5.05178099e-01]
- [6.02740823e-01]
- [7.08471424e-01]
- [8.21581945e-01]
- [9.32434871e-01]
- [1.04554166e+00]
- [1.15623590e+00]]</t>
+          <t>[[1.58283357e-04]
+ [3.31093003e-04]
+ [1.77440549e-05]
+ [2.97887336e-03]
+ [4.01191585e-03]
+ [5.16384957e-03]
+ [6.43350597e-03]
+ [7.80880180e-03]
+ [9.28490152e-03]
+ [1.08607824e-02]
+ [1.43029322e-02]
+ [1.81242559e-02]
+ [2.23167179e-02]
+ [2.68807713e-02]
+ [3.18130653e-02]
+ [3.71052640e-02]
+ [3.98918630e-02]
+ [4.27755621e-02]
+ [4.57551948e-02]
+ [7.50776058e-02]
+ [1.17733957e-01]
+ [1.72405073e-01]
+ [2.69056055e-01]
+ [3.84190550e-01]
+ [5.13803785e-01]
+ [5.98169622e-01]
+ [6.87785919e-01]
+ [7.81970594e-01]
+ [8.74468209e-01]
+ [9.69054622e-01]
+ [1.06164387e+00]]</t>
         </is>
       </c>
       <c r="E502" t="inlineStr"/>
@@ -12885,7 +12877,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>[1.1562359]</t>
+          <t>[1.06164387]</t>
         </is>
       </c>
       <c r="E503" t="inlineStr"/>
@@ -12908,24 +12900,24 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>[[-31179435.72038715]
- [-28733133.38425641]
- [-25809273.9770739 ]
- [-25242005.971014  ]
- [-24673272.54583432]
- [-24101590.42890056]
- [-23525440.07335947]
- [-22943246.03860893]
- [-22353355.35982918]
- [-21142354.43006401]
- [-19877392.72607838]
- [-18539157.66846403]
- [-17441329.69565723]
- [-16625895.58361371]
- [-15810461.47157015]
- [-15402744.41554845]
- [-14995027.35952632]
- [-14587310.30350392]]</t>
+          <t>[[-36123346.97588959]
+ [-33960790.79041462]
+ [-31421691.94796431]
+ [-30879849.66133218]
+ [-30336846.93487328]
+ [-29791509.30376027]
+ [-29181329.17357343]
+ [-28566364.10790942]
+ [-27945306.30131707]
+ [-26658812.50241386]
+ [-25329647.43537711]
+ [-23942610.16605137]
+ [-22780861.82640503]
+ [-21842022.14135061]
+ [-20903182.45629581]
+ [-20484151.47503773]
+ [-20065120.49377933]
+ [-19646089.51252162]]</t>
         </is>
       </c>
       <c r="E504" t="inlineStr"/>
@@ -12948,24 +12940,24 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>[[-3630432.17990122]
- [-8198899.84274795]
- [-7770118.21064171]
- [ 2428056.98943542]
- [ 2428073.38905587]
- [ 2428090.12906986]
- [ 2428107.34313002]
- [ 2428125.1727663 ]
- [ 2428143.77066976]
- [ 2428420.43316857]
- [ 2428507.89136093]
- [ 2428608.99916826]
- [ 2428599.3996326 ]
- [ 2428426.01496882]
- [ 2428465.30683914]
- [ 2428209.88216267]
- [ 2428219.36397806]
- [ 2428228.73207834]]</t>
+          <t>[[-3571386.85080247]
+ [-8980999.77048393]
+ [-9160127.16752138]
+ [ 2428093.82801644]
+ [ 2428113.53256131]
+ [ 2428133.56642783]
+ [ 2428177.55584712]
+ [ 2428198.07321296]
+ [ 2428219.29887818]
+ [ 2428588.30264015]
+ [ 2428684.72498103]
+ [ 2428793.4671491 ]
+ [ 2428772.71401341]
+ [ 2428620.0939148 ]
+ [ 2428670.77338876]
+ [ 2428275.82942879]
+ [ 2428288.03473593]
+ [ 2428300.09340087]]</t>
         </is>
       </c>
       <c r="E505" t="inlineStr"/>
@@ -12988,24 +12980,24 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>[[ -47410.92596769]
- [-107349.00461938]
- [-102767.23478233]
- [  29096.4415081 ]
- [  29096.65584818]
- [  29096.87478316]
- [  29097.10006327]
- [  29097.3335442 ]
- [  29097.57723025]
- [  29101.18729044]
- [  29102.33512868]
- [  29103.66334132]
- [  29103.54613785]
- [  29101.28472521]
- [  29101.80566794]
- [  29098.46161373]
- [  29098.58775759]
- [  29098.7125375 ]]</t>
+          <t>[[ -46612.79626053]
+ [-117471.93621095]
+ [-120846.42288106]
+ [  29096.92151658]
+ [  29097.17898185]
+ [  29097.44093214]
+ [  29098.01559855]
+ [  29098.28422904]
+ [  29098.56230757]
+ [  29103.37730347]
+ [  29104.64273106]
+ [  29106.07123526]
+ [  29105.80901867]
+ [  29103.82156847]
+ [  29104.49322739]
+ [  29099.32366656]
+ [  29099.48597565]
+ [  29099.64652502]]</t>
         </is>
       </c>
       <c r="E506" t="inlineStr"/>
@@ -13028,24 +13020,24 @@
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>[[ -671569.38927988]
- [-2556545.26945517]
- [-4649408.3173616 ]
- [-5412555.49602903]
- [-5363780.52488637]
- [-5314981.82955081]
- [-5266161.10671832]
- [-5217320.06743728]
- [-5168460.44500652]
- [-5070681.72287733]
- [-4972848.36671396]
- [-4874975.95141809]
- [-4777081.15300104]
- [-4679164.50009334]
- [-4581220.77998569]
- [-4532247.55915087]
- [-4483271.00523964]
- [-4434292.00104467]]</t>
+          <t>[[ -526598.7774628 ]
+ [-2406071.56195532]
+ [-4715198.34905789]
+ [-5431349.17696918]
+ [-5382395.25464339]
+ [-5333402.76688932]
+ [-5284377.98404438]
+ [-5235325.59908948]
+ [-5186247.67118431]
+ [-5088011.01723978]
+ [-4989699.00157361]
+ [-4891329.46663574]
+ [-4792918.5016765 ]
+ [-4694465.88006755]
+ [-4595969.73165049]
+ [-4546715.11585086]
+ [-4497449.51364613]
+ [-4448174.12628585]]</t>
         </is>
       </c>
       <c r="E507" t="inlineStr"/>
@@ -13068,24 +13060,24 @@
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>[[5.16435012e+07]
- [1.96221076e+08]
- [3.55840560e+08]
- [4.14083720e+08]
- [4.10015355e+08]
- [4.05945179e+08]
- [4.01873324e+08]
- [3.97799923e+08]
- [3.93725110e+08]
- [3.85570964e+08]
- [3.77412692e+08]
- [3.69251492e+08]
- [3.61088644e+08]
- [3.52924192e+08]
- [3.44757740e+08]
- [3.40674436e+08]
- [3.36590896e+08]
- [3.32507186e+08]]</t>
+          <t>[[4.05032729e+07]
+ [1.84726748e+08]
+ [3.60998049e+08]
+ [4.15644529e+08]
+ [4.11562418e+08]
+ [4.07477361e+08]
+ [4.03389850e+08]
+ [3.99300236e+08]
+ [3.95208680e+08]
+ [3.87019429e+08]
+ [3.78824481e+08]
+ [3.70625212e+08]
+ [3.62422859e+08]
+ [3.54217416e+08]
+ [3.46008748e+08]
+ [3.41903950e+08]
+ [3.37798342e+08]
+ [3.33692018e+08]]</t>
         </is>
       </c>
       <c r="E508" t="inlineStr"/>
@@ -13108,24 +13100,24 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>[[ 214260.6777001 ]
- [ 468224.68710593]
- [ 808955.83756311]
- [1299593.325459  ]
- [1299590.41838053]
- [1299587.50380529]
- [1299584.57413213]
- [1299581.62157415]
- [1299578.63805818]
- [1299575.61511389]
- [1299569.40928209]
- [1299562.92698901]
- [1299556.06927721]
- [1299550.44357231]
- [1299546.26499681]
- [1299542.08644818]
- [1299539.99718394]
- [1299537.90792641]]</t>
+          <t>[[ 214069.90260215]
+ [ 467905.66188862]
+ [ 808663.37487048]
+ [1299618.86705817]
+ [1299616.14571376]
+ [1299613.41855259]
+ [1299591.46407197]
+ [1299588.79319843]
+ [1299586.10139144]
+ [1299580.91306006]
+ [1299575.39564019]
+ [1299569.69526414]
+ [1299567.63171611]
+ [1299562.46088873]
+ [1299558.28223587]
+ [1299565.29142155]
+ [1299563.2020827 ]
+ [1299561.11275055]]</t>
         </is>
       </c>
       <c r="E509" t="inlineStr"/>
@@ -13148,9 +13140,9 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>[[  2428056.98943542]
- [    29096.4415081 ]
- [-25809273.97707409]]</t>
+          <t>[[ 2.42809383e+06]
+ [ 2.90969215e+04]
+ [-3.14216919e+07]]</t>
         </is>
       </c>
       <c r="E510" t="inlineStr"/>
@@ -13173,9 +13165,9 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>[[-5.46130505e+06]
- [ 4.18150144e+08]
- [ 1.29959333e+06]]</t>
+          <t>[[-5.48026241e+06]
+ [ 4.19723529e+08]
+ [ 1.29961887e+06]]</t>
         </is>
       </c>
       <c r="E511" t="inlineStr"/>
@@ -13227,12 +13219,12 @@
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>[12.43319258 12.43319262 12.43319266 12.4331927  12.4331927  12.4331927
- 12.4331927  12.43319272 12.43319274 12.43319276 12.43319277 12.43319277
- 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278 12.43319278
- 12.43319278 12.43319278 12.43319278 12.43319278 12.09875903 11.76432528
- 11.42989152 10.58683885  9.74378618  8.90073352  7.93776698  6.97480044
-  6.01183391]</t>
+          <t>[11.         11.         11.         11.         11.         11.
+ 11.         11.         11.         11.         11.         11.
+ 11.         11.         11.         11.         11.         11.
+ 10.         10.         10.         10.         10.         10.
+ 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
+  5.999     ]</t>
         </is>
       </c>
       <c r="E513" t="inlineStr"/>
@@ -13255,11 +13247,11 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>[0.077      0.077      0.077      0.077      0.077      0.077
- 0.077      0.077      0.077      0.077      0.077      0.077
- 0.077      0.077      0.077      0.077      0.077      0.077
- 0.02268044 0.02268044 0.02268044 0.0142022  0.0142022  0.0142022
- 0.01174385 0.01174385 0.01174385 0.01142884 0.01142884 0.01142884]</t>
+          <t>[0.077      0.077      0.077      0.08897847 0.08897847 0.08897847
+ 0.10221371 0.10221371 0.10221371 0.10434048 0.10434048 0.10434048
+ 0.10050124 0.10050124 0.10050124 0.08962371 0.08962371 0.08962371
+ 0.04       0.04       0.04       0.038801   0.038801   0.038801
+ 0.026301   0.026301   0.026301   0.015      0.015      0.015     ]</t>
         </is>
       </c>
       <c r="E514" t="inlineStr"/>
@@ -13358,11 +13350,11 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>[3.19822531 3.19822532 3.19822533 3.19822529 3.19822529 3.19822529
- 3.19822526 3.19822526 3.19822527 3.19822527 3.19822527 3.19822527
- 3.19822527 3.19822527 3.19822527 3.19822527 3.19822527 3.19822527
- 0.94618249 0.94618249 0.94618249 0.58490872 0.5689426  0.55297649
- 0.43411361 0.40083242 0.36755123 0.32301245 0.28601711 0.24902177]</t>
+          <t>[2.82726365 2.82726365 2.82726365 3.263503   3.263503   3.263503
+ 3.74438999 3.74438999 3.74438999 3.82155405 3.82155405 3.82155405
+ 3.6822358  3.6822358  3.6822358  3.28697421 3.28697421 3.28697421
+ 1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
+ 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
         </is>
       </c>
       <c r="E518" t="inlineStr"/>
@@ -13385,11 +13377,11 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>[1.81995474 1.81995474 1.81995475 1.81995473 1.81995472 1.81995472
- 1.81995471 1.81995471 1.81995471 1.81995471 1.81995472 1.81995472
- 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472
- 0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
+ 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
+ 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
+ 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E519" t="inlineStr"/>
@@ -13412,11 +13404,11 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>[1.81995474 1.81995474 1.81995475 1.81995473 1.81995472 1.81995472
- 1.81995471 1.81995471 1.81995471 1.81995471 1.81995472 1.81995472
- 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472 1.81995472
- 0.53736216 0.53736216 0.53736216 0.33208718 0.32302691 0.31396663
- 0.246462   0.22757595 0.20868991 0.1834094  0.16241572 0.14142205]</t>
+          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
+ 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
+ 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
+ 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
+ 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
         </is>
       </c>
       <c r="E520" t="inlineStr"/>
@@ -13439,12 +13431,12 @@
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>[122.07739902 122.07740015 122.07740128 122.07740017 122.07740017
- 122.07740016 122.07739914 122.07739979 122.07740045 122.07740086
- 122.07740103 122.07740119 122.07740128 122.07740128 122.07740128
- 122.07740128 122.07740128 122.07740128  36.43307152  36.43307152
-  36.43307152  21.94960044  20.2007613   18.54737303  13.12388581
-  10.33096399   7.96537229   5.70856597   3.96319571   2.6156629 ]</t>
+          <t>[ 84.33576062  84.33576062  84.33576062  97.1367864   97.1367864
+  97.1367864  111.18235328 111.18235328 111.18235328 113.42972734
+ 113.42972734 113.42972734 109.3708483  109.3708483  109.3708483
+  97.82392145  97.82392145  97.82392145  33.21380796  33.21380796
+  33.21380796  32.22982785  32.22982785  32.22982785  19.88323673
+  16.18153341  12.97038057   5.79213059   4.36751812   3.19804084]</t>
         </is>
       </c>
       <c r="E521" t="inlineStr"/>
@@ -13467,11 +13459,11 @@
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>[61.03869951 61.03870008 61.03870064 61.03870009 61.03870008 61.03870008
- 61.03869957 61.0386999  61.03870023 61.03870043 61.03870051 61.0387006
- 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064
- 18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
+ 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
+ 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
+ 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E522" t="inlineStr"/>
@@ -13494,11 +13486,11 @@
       </c>
       <c r="D523" t="inlineStr">
         <is>
-          <t>[61.03869951 61.03870008 61.03870064 61.03870009 61.03870008 61.03870008
- 61.03869957 61.0386999  61.03870023 61.03870043 61.03870051 61.0387006
- 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064 61.03870064
- 18.21653576 18.21653576 18.21653576 10.97480022 10.10038065  9.27368651
-  6.5619429   5.16548199  3.98268614  2.85428299  1.98159786  1.30783145]</t>
+          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
+ 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
+ 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
+ 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
+  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
         </is>
       </c>
       <c r="E523" t="inlineStr"/>
@@ -13623,36 +13615,36 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>[[-3.11794357e+07]
- [-2.87331334e+07]
- [-2.58092740e+07]
- [-2.52420060e+07]
- [-2.46732725e+07]
- [-2.41015904e+07]
- [-2.35254401e+07]
- [-2.29432460e+07]
- [-2.23533554e+07]
- [-2.11423544e+07]
- [-1.98773927e+07]
- [-1.85391577e+07]
- [-1.74413297e+07]
- [-1.66258956e+07]
- [-1.58104615e+07]
- [-1.54027444e+07]
- [-1.49950274e+07]
- [-1.45873103e+07]
- [-1.27305439e+07]
- [-1.18515418e+07]
- [-1.09719070e+07]
- [-1.01911563e+07]
- [-9.43096813e+06]
- [-8.69150452e+06]
- [-8.34177167e+06]
- [-8.01848614e+06]
- [-7.72186527e+06]
- [-7.47824924e+06]
- [-7.26235587e+06]
- [ 1.31112756e-08]]</t>
+          <t>[[-3.61233470e+07]
+ [-3.39607908e+07]
+ [-3.14216919e+07]
+ [-3.08798497e+07]
+ [-3.03368469e+07]
+ [-2.97915093e+07]
+ [-2.91813292e+07]
+ [-2.85663641e+07]
+ [-2.79453063e+07]
+ [-2.66588125e+07]
+ [-2.53296474e+07]
+ [-2.39426102e+07]
+ [-2.27808618e+07]
+ [-2.18420221e+07]
+ [-2.09031825e+07]
+ [-2.04841515e+07]
+ [-2.00651205e+07]
+ [-1.96460895e+07]
+ [-1.74269003e+07]
+ [-1.61860231e+07]
+ [-1.49446247e+07]
+ [-1.32233993e+07]
+ [-1.15016608e+07]
+ [-9.77942261e+06]
+ [-9.09862410e+06]
+ [-8.46264681e+06]
+ [-7.87173034e+06]
+ [-7.57979326e+06]
+ [-7.31395379e+06]
+ [ 4.36557457e-10]]</t>
         </is>
       </c>
       <c r="E527" t="inlineStr"/>
@@ -13675,36 +13667,36 @@
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>[[-3.63043218e+06]
- [-8.19889984e+06]
- [-7.77011821e+06]
- [ 2.42805699e+06]
- [ 2.42807339e+06]
- [ 2.42809013e+06]
- [ 2.42810734e+06]
- [ 2.42812517e+06]
- [ 2.42814377e+06]
- [ 2.42842043e+06]
- [ 2.42850789e+06]
- [ 2.42860900e+06]
- [ 2.42859940e+06]
- [ 2.42842601e+06]
- [ 2.42846531e+06]
- [ 2.42820988e+06]
- [ 2.42821936e+06]
- [ 2.42822873e+06]
- [ 2.42883824e+06]
- [ 2.42928308e+06]
- [ 2.42968212e+06]
- [ 2.43001408e+06]
- [ 2.43058263e+06]
- [ 2.43102787e+06]
- [ 2.42957454e+06]
- [ 2.42957782e+06]
- [ 2.42954745e+06]
- [ 2.42932438e+06]
- [ 2.42919063e+06]
- [ 1.07860585e+03]]</t>
+          <t>[[-3.57138685e+06]
+ [-8.98099977e+06]
+ [-9.16012717e+06]
+ [ 2.42809383e+06]
+ [ 2.42811353e+06]
+ [ 2.42813357e+06]
+ [ 2.42817756e+06]
+ [ 2.42819807e+06]
+ [ 2.42821930e+06]
+ [ 2.42858830e+06]
+ [ 2.42868472e+06]
+ [ 2.42879347e+06]
+ [ 2.42877271e+06]
+ [ 2.42862009e+06]
+ [ 2.42867077e+06]
+ [ 2.42827583e+06]
+ [ 2.42828803e+06]
+ [ 2.42830009e+06]
+ [ 2.42942913e+06]
+ [ 2.43011791e+06]
+ [ 2.43073661e+06]
+ [ 2.43274959e+06]
+ [ 2.43367362e+06]
+ [ 2.43439828e+06]
+ [ 2.43070100e+06]
+ [ 2.43067999e+06]
+ [ 2.43061537e+06]
+ [ 2.42932413e+06]
+ [ 2.42922801e+06]
+ [ 1.14939088e+03]]</t>
         </is>
       </c>
       <c r="E528" t="inlineStr"/>
@@ -13727,36 +13719,36 @@
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>[[-4.74109260e+04]
- [-1.07349005e+05]
- [-1.02767235e+05]
- [ 2.90964415e+04]
- [ 2.90966558e+04]
- [ 2.90968748e+04]
- [ 2.90971001e+04]
- [ 2.90973335e+04]
- [ 2.90975772e+04]
- [ 2.91011873e+04]
- [ 2.91023351e+04]
- [ 2.91036633e+04]
- [ 2.91035461e+04]
- [ 2.91012847e+04]
- [ 2.91018057e+04]
- [ 2.90984616e+04]
- [ 2.90985878e+04]
- [ 2.90987125e+04]
- [ 2.91067528e+04]
- [ 2.91127423e+04]
- [ 2.91181795e+04]
- [ 2.91228650e+04]
- [ 2.91309879e+04]
- [ 2.91376687e+04]
- [ 2.91178825e+04]
- [ 2.91183035e+04]
- [ 2.91183766e+04]
- [ 2.91157463e+04]
- [ 2.91146263e+04]
- [ 1.75412890e+01]]</t>
+          <t>[[-4.66127963e+04]
+ [-1.17471936e+05]
+ [-1.20846423e+05]
+ [ 2.90969215e+04]
+ [ 2.90971790e+04]
+ [ 2.90974409e+04]
+ [ 2.90980156e+04]
+ [ 2.90982842e+04]
+ [ 2.90985623e+04]
+ [ 2.91033773e+04]
+ [ 2.91046427e+04]
+ [ 2.91060712e+04]
+ [ 2.91058090e+04]
+ [ 2.91038216e+04]
+ [ 2.91044932e+04]
+ [ 2.90993237e+04]
+ [ 2.90994860e+04]
+ [ 2.90996465e+04]
+ [ 2.91145355e+04]
+ [ 2.91238056e+04]
+ [ 2.91322314e+04]
+ [ 2.91595534e+04]
+ [ 2.91726762e+04]
+ [ 2.91834001e+04]
+ [ 2.91331718e+04]
+ [ 2.91333875e+04]
+ [ 2.91331398e+04]
+ [ 2.91153261e+04]
+ [ 2.91149474e+04]
+ [ 1.84960460e+01]]</t>
         </is>
       </c>
       <c r="E529" t="inlineStr"/>
@@ -13779,36 +13771,36 @@
       </c>
       <c r="D530" t="inlineStr">
         <is>
-          <t>[[-6.71569389e+05]
- [-2.55654527e+06]
- [-4.64940832e+06]
- [-5.41255550e+06]
- [-5.36378052e+06]
- [-5.31498183e+06]
- [-5.26616111e+06]
- [-5.21732007e+06]
- [-5.16846045e+06]
- [-5.07068172e+06]
- [-4.97284837e+06]
- [-4.87497595e+06]
- [-4.77708115e+06]
- [-4.67916450e+06]
- [-4.58122078e+06]
- [-4.53224756e+06]
- [-4.48327101e+06]
- [-4.43429200e+06]
- [-4.07857587e+06]
- [-3.72106632e+06]
- [-3.36222737e+06]
- [-2.84687235e+06]
- [-2.32838009e+06]
- [-1.80776549e+06]
- [-1.49481546e+06]
- [-1.18119602e+06]
- [-8.66936826e+05]
- [-5.73109442e+05]
- [-2.78840152e+05]
- [-4.49704115e-04]]</t>
+          <t>[[-5.26598777e+05]
+ [-2.40607156e+06]
+ [-4.71519835e+06]
+ [-5.43134918e+06]
+ [-5.38239525e+06]
+ [-5.33340277e+06]
+ [-5.28437798e+06]
+ [-5.23532560e+06]
+ [-5.18624767e+06]
+ [-5.08801102e+06]
+ [-4.98969900e+06]
+ [-4.89132947e+06]
+ [-4.79291850e+06]
+ [-4.69446588e+06]
+ [-4.59596973e+06]
+ [-4.54671512e+06]
+ [-4.49744951e+06]
+ [-4.44817413e+06]
+ [-4.08976416e+06]
+ [-3.72869453e+06]
+ [-3.36567846e+06]
+ [-2.84455227e+06]
+ [-2.32217436e+06]
+ [-1.80001961e+06]
+ [-1.48754428e+06]
+ [-1.17506364e+06]
+ [-8.62644874e+05]
+ [-5.70954763e+05]
+ [-2.78858769e+05]
+ [-4.93283089e-04]]</t>
         </is>
       </c>
       <c r="E530" t="inlineStr"/>
@@ -13831,36 +13823,36 @@
       </c>
       <c r="D531" t="inlineStr">
         <is>
-          <t>[[ 5.16435012e+07]
- [ 1.96221076e+08]
- [ 3.55840560e+08]
- [ 4.14083720e+08]
- [ 4.10015355e+08]
- [ 4.05945179e+08]
- [ 4.01873324e+08]
- [ 3.97799923e+08]
- [ 3.93725110e+08]
- [ 3.85570964e+08]
- [ 3.77412692e+08]
- [ 3.69251492e+08]
- [ 3.61088644e+08]
- [ 3.52924192e+08]
- [ 3.44757740e+08]
- [ 3.40674436e+08]
- [ 3.36590896e+08]
- [ 3.32507186e+08]
- [ 3.02856876e+08]
- [ 2.73073876e+08]
- [ 2.43194183e+08]
- [ 2.00313765e+08]
- [ 1.57216393e+08]
- [ 1.13983004e+08]
- [ 8.80131860e+07]
- [ 6.20098904e+07]
- [ 3.59815986e+07]
- [ 1.16790315e+07]
- [-1.26133766e+07]
- [ 2.76522860e-02]]</t>
+          <t>[[ 4.05032729e+07]
+ [ 1.84726748e+08]
+ [ 3.60998049e+08]
+ [ 4.15644529e+08]
+ [ 4.11562418e+08]
+ [ 4.07477361e+08]
+ [ 4.03389850e+08]
+ [ 3.99300236e+08]
+ [ 3.95208680e+08]
+ [ 3.87019429e+08]
+ [ 3.78824481e+08]
+ [ 3.70625212e+08]
+ [ 3.62422859e+08]
+ [ 3.54217416e+08]
+ [ 3.46008748e+08]
+ [ 3.41903950e+08]
+ [ 3.37798342e+08]
+ [ 3.33692018e+08]
+ [ 3.03837180e+08]
+ [ 2.73785524e+08]
+ [ 2.43592339e+08]
+ [ 2.00279949e+08]
+ [ 1.56888351e+08]
+ [ 1.13528454e+08]
+ [ 8.75813616e+07]
+ [ 6.16446447e+07]
+ [ 3.57262528e+07]
+ [ 1.15515326e+07]
+ [-1.26120054e+07]
+ [ 3.06533657e-02]]</t>
         </is>
       </c>
       <c r="E531" t="inlineStr"/>
@@ -13883,35 +13875,35 @@
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>[[ 214260.6777001 ]
- [ 468224.68710593]
- [ 808955.83756311]
- [1299593.325459  ]
- [1299590.41838053]
- [1299587.50380529]
- [1299584.57413213]
- [1299581.62157415]
- [1299578.63805818]
- [1299575.61511389]
- [1299569.40928209]
- [1299562.92698901]
- [1299556.06927721]
- [1299550.44357231]
- [1299546.26499681]
- [1299542.08644818]
- [1299539.99718394]
- [1299537.90792641]
- [1299696.76647942]
- [1299681.58766421]
- [1299666.35950518]
- [1299768.53255836]
- [1299754.66513967]
- [1299740.60683059]
- [1299789.23811668]
- [1299802.18781541]
- [1299818.66277765]
- [1299852.92757498]
- [1299889.66301773]
+          <t>[[ 214069.90260215]
+ [ 467905.66188862]
+ [ 808663.37487048]
+ [1299618.86705817]
+ [1299616.14571376]
+ [1299613.41855259]
+ [1299591.46407197]
+ [1299588.79319843]
+ [1299586.10139144]
+ [1299580.91306006]
+ [1299575.39564019]
+ [1299569.69526414]
+ [1299567.63171611]
+ [1299562.46088873]
+ [1299558.28223587]
+ [1299565.29142155]
+ [1299563.2020827 ]
+ [1299561.11275055]
+ [1299689.5032564 ]
+ [1299674.34321372]
+ [1299659.155116  ]
+ [1299649.59058574]
+ [1299627.87565582]
+ [1299606.15497853]
+ [1299648.86747394]
+ [1299648.21346755]
+ [1299648.45194692]
+ [1299792.67972821]
+ [1299811.89339675]
  [      0.        ]]</t>
         </is>
       </c>
@@ -13935,24 +13927,24 @@
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>[[-4488810.2618741 ]
- [11002098.29228969]
- [28174442.27678555]
- [34284200.86725761]
- [34047649.16495978]
- [33811835.03296962]
- [33577247.29757702]
- [33344391.31707139]
- [33113798.03190549]
- [32661912.96192548]
- [32226479.74316878]
- [31813658.94097381]
- [31325501.42574162]
- [30748883.4714948 ]
- [30172061.91752999]
- [29883643.21271906]
- [29595200.39531134]
- [29306740.36121462]]</t>
+          <t>[[-7493457.5293111 ]
+ [12084249.57549396]
+ [35975545.69216007]
+ [37610411.33137283]
+ [37314496.88095672]
+ [37018964.30323167]
+ [32120083.294518  ]
+ [31879678.51544838]
+ [31640708.7096287 ]
+ [30559062.8958482 ]
+ [30112097.61916249]
+ [29679856.9200609 ]
+ [30267262.75396389]
+ [29696904.16724063]
+ [29126221.1770942 ]
+ [32217532.71577787]
+ [31883319.16482491]
+ [31549025.04878658]]</t>
         </is>
       </c>
       <c r="E533" t="inlineStr"/>
@@ -13975,24 +13967,24 @@
       </c>
       <c r="D534" t="inlineStr">
         <is>
-          <t>[[2005873.54325258]
- [4529231.77077679]
- [4310970.05428396]
- [1400405.93552247]
- [1400414.79928067]
- [1400423.84970801]
- [1400433.174244  ]
- [1400442.81884385]
- [1400452.88403938]
- [1400604.75745632]
- [1400652.50002855]
- [1400707.72914658]
- [1400702.10459646]
- [1400606.54138291]
- [1400627.91993754]
- [1400487.34848946]
- [1400492.45248646]
- [1400497.49399693]]</t>
+          <t>[[2233146.75679488]
+ [5611124.66811099]
+ [5744661.88449172]
+ [1379991.28185071]
+ [1380001.72968485]
+ [1380012.35438049]
+ [1202307.51439414]
+ [1202316.99831437]
+ [1202326.81316458]
+ [1178140.98071276]
+ [1178184.98770823]
+ [1178234.64277084]
+ [1222949.25834957]
+ [1222876.25591098]
+ [1222900.20089956]
+ [1370204.29938101]
+ [1370210.70185411]
+ [1370217.02599413]]</t>
         </is>
       </c>
       <c r="E534" t="inlineStr"/>
@@ -14017,17 +14009,17 @@
         <is>
           <t>[[       -0.        ]
  [       -0.        ]
- [ -8628234.33126603]
- [-16586955.02965773]
- [-15253062.79322555]
- [-13929525.60982153]
- [-12616568.88796056]
- [-11314534.65838669]
- [-10023887.94880238]
- [ -8115530.29132211]
- [ -5611896.87202155]
- [ -3169760.3858186 ]
- [  -982655.08272861]
+ [ -7627447.09919977]
+ [-12675152.21247375]
+ [-11655839.92170454]
+ [-10644440.5885838 ]
+ [ -8382556.02585416]
+ [ -7517473.3600212 ]
+ [ -6659956.66271766]
+ [ -5281090.90962319]
+ [ -3651879.35714917]
+ [ -2062686.25009233]
+ [  -664113.42747926]
  [       -0.        ]
  [       -0.        ]
  [       -0.        ]
@@ -14091,24 +14083,24 @@
       <c r="C537" t="inlineStr"/>
       <c r="D537" t="inlineStr">
         <is>
-          <t>[[0.02887492]
- [0.06873756]
- [0.17378451]
- [0.22891798]
- [0.22273161]
- [0.21666722]
- [0.21073282]
- [0.20493725]
- [0.19929023]
- [0.19058215]
- [0.18033792]
- [0.17091598]
- [0.16237839]
- [0.15690428]
- [0.15397929]
- [0.15251678]
- [0.15105435]
- [0.14959192]]</t>
+          <t>[[0.04289747]
+ [0.07888609]
+ [0.21132756]
+ [0.23075016]
+ [0.22571849]
+ [0.22076848]
+ [0.18866726]
+ [0.18459539]
+ [0.18060859]
+ [0.17079569]
+ [0.16359171]
+ [0.15683455]
+ [0.15605734]
+ [0.15145061]
+ [0.14855509]
+ [0.16433325]
+ [0.16263776]
+ [0.16094197]]</t>
         </is>
       </c>
       <c r="E537" t="inlineStr"/>
@@ -14127,24 +14119,24 @@
       <c r="C538" t="inlineStr"/>
       <c r="D538" t="inlineStr">
         <is>
-          <t>[[0.05479743]
- [0.06732037]
- [0.17191571]
- [0.06201918]
- [0.0579533 ]
- [0.05398549]
- [0.05013057]
- [0.04640758]
- [0.04284092]
- [0.05607102]
- [0.04559774]
- [0.03690084]
- [0.0303443 ]
- [0.02753895]
- [0.02641933]
- [0.02308523]
- [0.02256537]
- [0.02204721]]</t>
+          <t>[[0.06517142]
+ [0.08107839]
+ [0.16551556]
+ [0.0485888 ]
+ [0.04607327]
+ [0.04367489]
+ [0.03339134]
+ [0.03162263]
+ [0.0299975 ]
+ [0.03394068]
+ [0.02998886]
+ [0.02691042]
+ [0.02650527]
+ [0.02546888]
+ [0.02449908]
+ [0.02617813]
+ [0.02569723]
+ [0.02521719]]</t>
         </is>
       </c>
       <c r="E538" t="inlineStr"/>
@@ -14163,24 +14155,24 @@
       <c r="C539" t="inlineStr"/>
       <c r="D539" t="inlineStr">
         <is>
-          <t>[[0.0780364 ]
- [0.14621045]
- [0.22103653]
- [0.2491743 ]
- [0.2461717 ]
- [0.24316352]
- [0.24014724]
- [0.23712024]
- [0.23407978]
- [0.22794451]
- [0.22171679]
- [0.21536445]
- [0.20942197]
- [0.20396032]
- [0.19849868]
- [0.19576819]
- [0.19303783]
- [0.19030764]]</t>
+          <t>[[0.08447172]
+ [0.16285742]
+ [0.25873801]
+ [0.25047413]
+ [0.24764075]
+ [0.24480281]
+ [0.21105853]
+ [0.2084927 ]
+ [0.20591841]
+ [0.19670041]
+ [0.19154174]
+ [0.18630866]
+ [0.18814666]
+ [0.18331159]
+ [0.17847625]
+ [0.19706939]
+ [0.19443731]
+ [0.19180519]]</t>
         </is>
       </c>
       <c r="E539" t="inlineStr"/>
@@ -14203,36 +14195,36 @@
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>[[-4.48881026e+06]
- [ 1.10020983e+07]
- [ 2.81744423e+07]
- [ 3.42842009e+07]
- [ 3.40476492e+07]
- [ 3.38118350e+07]
- [ 3.35772473e+07]
- [ 3.33443913e+07]
- [ 3.31137980e+07]
- [ 3.26619130e+07]
- [ 3.22264797e+07]
- [ 3.18136589e+07]
- [ 3.13255014e+07]
- [ 3.07488835e+07]
- [ 3.01720619e+07]
- [ 2.98836432e+07]
- [ 2.95952004e+07]
- [ 2.93067404e+07]
- [ 8.99080258e+07]
- [ 8.06725224e+07]
- [ 7.14046904e+07]
- [ 9.45280584e+07]
- [ 7.62934453e+07]
- [ 5.55613947e+07]
- [ 5.46207991e+07]
- [ 4.10220787e+07]
- [ 2.11142740e+07]
- [-5.90609418e+06]
- [-1.65496023e+06]
- [ 6.86552322e-02]]</t>
+          <t>[[-7.49345753e+06]
+ [ 1.20842496e+07]
+ [ 3.59755457e+07]
+ [ 3.76104113e+07]
+ [ 3.73144969e+07]
+ [ 3.70189643e+07]
+ [ 3.21200833e+07]
+ [ 3.18796785e+07]
+ [ 3.16407087e+07]
+ [ 3.05590629e+07]
+ [ 3.01120976e+07]
+ [ 2.96798569e+07]
+ [ 3.02672628e+07]
+ [ 2.96969042e+07]
+ [ 2.91262212e+07]
+ [ 3.22175327e+07]
+ [ 3.18833192e+07]
+ [ 2.98432988e+07]
+ [ 7.84747709e+07]
+ [ 7.03527526e+07]
+ [ 6.21885106e+07]
+ [ 5.19696214e+07]
+ [ 3.98306986e+07]
+ [ 2.77020271e+07]
+ [ 3.19822276e+07]
+ [ 2.38206137e+07]
+ [ 1.25048784e+07]
+ [-4.04261505e+06]
+ [-3.22409417e+05]
+ [ 6.08299014e-02]]</t>
         </is>
       </c>
       <c r="E540" t="inlineStr"/>
@@ -14255,36 +14247,36 @@
       </c>
       <c r="D541" t="inlineStr">
         <is>
-          <t>[[2.00587354e+06]
- [4.52923177e+06]
- [4.31097005e+06]
- [1.40040594e+06]
- [1.40041480e+06]
- [1.40042385e+06]
- [1.40043317e+06]
- [1.40044282e+06]
- [1.40045288e+06]
- [1.40060476e+06]
- [1.40065250e+06]
- [1.40070773e+06]
- [1.40070210e+06]
- [1.40060654e+06]
- [1.40062792e+06]
- [1.40048735e+06]
- [1.40049245e+06]
- [1.40049749e+06]
- [4.74202053e+06]
- [4.74284583e+06]
- [4.74358589e+06]
- [7.68109472e+06]
- [7.90878603e+06]
- [8.14985004e+06]
- [1.04036477e+07]
- [1.13161457e+07]
- [1.24033583e+07]
- [1.42048568e+07]
- [1.61804915e+07]
- [7.62786603e+03]]</t>
+          <t>[[2.23314676e+06]
+ [5.61112467e+06]
+ [5.74466188e+06]
+ [1.37999128e+06]
+ [1.38000173e+06]
+ [1.38001235e+06]
+ [1.20230751e+06]
+ [1.20231700e+06]
+ [1.20232681e+06]
+ [1.17814098e+06]
+ [1.17818499e+06]
+ [1.17823464e+06]
+ [1.22294926e+06]
+ [1.22287626e+06]
+ [1.22290020e+06]
+ [1.37020430e+06]
+ [1.37021070e+06]
+ [1.36689585e+06]
+ [3.38694610e+06]
+ [3.38784861e+06]
+ [3.38865907e+06]
+ [3.49580729e+06]
+ [3.49705519e+06]
+ [3.49803311e+06]
+ [5.32952133e+06]
+ [5.73199810e+06]
+ [6.19988214e+06]
+ [1.18614448e+07]
+ [1.31245905e+07]
+ [6.33962609e+03]]</t>
         </is>
       </c>
       <c r="E541" t="inlineStr"/>
@@ -14309,34 +14301,34 @@
         <is>
           <t>[[-0.00000000e+00]
  [-0.00000000e+00]
- [-8.62823433e+06]
- [-1.65869550e+07]
- [-1.52530628e+07]
- [-1.39295256e+07]
- [-1.26165689e+07]
- [-1.13145347e+07]
- [-1.00238879e+07]
- [-8.11553029e+06]
- [-5.61189687e+06]
- [-3.16976039e+06]
- [-9.82655083e+05]
+ [-7.62744710e+06]
+ [-1.26751522e+07]
+ [-1.16558399e+07]
+ [-1.06444406e+07]
+ [-8.38255603e+06]
+ [-7.51747336e+06]
+ [-6.65995666e+06]
+ [-5.28109091e+06]
+ [-3.65187936e+06]
+ [-2.06268625e+06]
+ [-6.64113427e+05]
  [-0.00000000e+00]
  [-0.00000000e+00]
  [-0.00000000e+00]
  [-0.00000000e+00]
- [-1.90959118e+03]
- [-1.40143819e+04]
- [-1.56999011e+04]
- [-1.69403846e+04]
- [-2.85627126e+04]
- [-2.95465989e+04]
- [-3.01547547e+04]
- [-3.57941152e+04]
- [-3.37840649e+04]
- [-3.16086642e+04]
- [-2.98630692e+04]
- [-2.68734315e+04]
- [-2.37542547e+04]]</t>
+ [-1.38226070e+03]
+ [-6.37727477e+03]
+ [-7.14427391e+03]
+ [-7.70875864e+03]
+ [-8.50011278e+03]
+ [-9.03966576e+03]
+ [-9.49210348e+03]
+ [-1.40303966e+04]
+ [-1.33902336e+04]
+ [-1.26912628e+04]
+ [-2.08826573e+04]
+ [-1.93167339e+04]
+ [-1.76762289e+04]]</t>
         </is>
       </c>
       <c r="E542" t="inlineStr"/>
@@ -14407,36 +14399,36 @@
       <c r="C544" t="inlineStr"/>
       <c r="D544" t="inlineStr">
         <is>
-          <t>[[2.88749219e-02]
- [6.87375625e-02]
- [1.73784514e-01]
- [2.28917984e-01]
- [2.22731609e-01]
- [2.16667223e-01]
- [2.10732823e-01]
- [2.04937255e-01]
- [1.99290230e-01]
- [1.90582147e-01]
- [1.80337921e-01]
- [1.70915978e-01]
- [1.62378386e-01]
- [1.56904280e-01]
- [1.53979291e-01]
- [1.52516783e-01]
- [1.51054347e-01]
- [1.49596760e-01]
- [4.59298191e-01]
- [4.12539517e-01]
- [3.65672024e-01]
- [4.85671224e-01]
- [3.94381591e-01]
- [2.91691831e-01]
- [2.92670065e-01]
- [2.31351038e-01]
- [1.53286372e-01]
- [1.28695007e-01]
- [1.42808552e-01]
- [1.38269735e-04]]</t>
+          <t>[[4.28974749e-02]
+ [7.88860917e-02]
+ [2.11327556e-01]
+ [2.30750165e-01]
+ [2.25718487e-01]
+ [2.20768480e-01]
+ [1.88667257e-01]
+ [1.84595387e-01]
+ [1.80608592e-01]
+ [1.70795691e-01]
+ [1.63591709e-01]
+ [1.56834551e-01]
+ [1.56057343e-01]
+ [1.51450613e-01]
+ [1.48555089e-01]
+ [1.64333246e-01]
+ [1.62637763e-01]
+ [1.52292039e-01]
+ [4.00327783e-01]
+ [3.59142193e-01]
+ [3.17775596e-01]
+ [2.66176932e-01]
+ [2.04969183e-01]
+ [1.44273661e-01]
+ [1.69367633e-01]
+ [1.31309334e-01]
+ [8.38725544e-02]
+ [1.06503471e-01]
+ [1.15649998e-01]
+ [1.05855485e-04]]</t>
         </is>
       </c>
       <c r="E544" t="inlineStr"/>
@@ -14455,36 +14447,36 @@
       <c r="C545" t="inlineStr"/>
       <c r="D545" t="inlineStr">
         <is>
-          <t>[[0.05479743]
- [0.06732037]
- [0.17191571]
- [0.06201918]
- [0.0579533 ]
- [0.05398549]
- [0.05013057]
- [0.04640758]
- [0.04284092]
- [0.05607102]
- [0.04559774]
- [0.03690084]
- [0.0303443 ]
- [0.02753895]
- [0.02641933]
- [0.02308523]
- [0.02256537]
- [0.02204618]
- [0.29141785]
- [0.28000723]
- [0.26855619]
- [0.81550366]
- [0.78695206]
- [0.75971712]
- [1.        ]
- [0.98098993]
- [0.96599022]
- [0.99764311]
- [0.99383902]
- [0.00474795]]</t>
+          <t>[[0.06517142]
+ [0.08107839]
+ [0.16551556]
+ [0.0485888 ]
+ [0.04607327]
+ [0.04367489]
+ [0.03339134]
+ [0.03162263]
+ [0.0299975 ]
+ [0.03394068]
+ [0.02998886]
+ [0.02691042]
+ [0.02650527]
+ [0.02546888]
+ [0.02449908]
+ [0.02617813]
+ [0.02569723]
+ [0.02603512]
+ [0.11264868]
+ [0.1072023 ]
+ [0.1017812 ]
+ [0.10666565]
+ [0.09898535]
+ [0.0914236 ]
+ [0.17445981]
+ [0.17064628]
+ [0.16781383]
+ [0.54871723]
+ [0.54737998]
+ [0.00234186]]</t>
         </is>
       </c>
       <c r="E545" t="inlineStr"/>
@@ -14503,36 +14495,36 @@
       <c r="C546" t="inlineStr"/>
       <c r="D546" t="inlineStr">
         <is>
-          <t>[[1.34541781e-01]
- [2.29460327e-01]
- [3.32487812e-01]
- [3.71617972e-01]
- [3.66687338e-01]
- [3.61750747e-01]
- [3.56802856e-01]
- [3.51838142e-01]
- [3.46850854e-01]
- [3.36779705e-01]
- [3.26538153e-01]
- [3.16059988e-01]
- [3.06461298e-01]
- [2.97882653e-01]
- [2.89318754e-01]
- [2.85042784e-01]
- [2.80770659e-01]
- [2.76502421e-01]
- [8.73523649e-01]
- [7.88205868e-01]
- [7.03411012e-01]
- [9.96614020e-01]
- [8.52824322e-01]
- [6.90423770e-01]
- [7.78821624e-01]
- [7.31096492e-01]
- [6.53075041e-01]
- [5.69060901e-01]
- [8.26513438e-01]
- [4.56932686e-10]]</t>
+          <t>[[1.93459039e-01]
+ [3.34017754e-01]
+ [5.04148090e-01]
+ [4.80211833e-01]
+ [4.74203166e-01]
+ [4.68191007e-01]
+ [4.00883477e-01]
+ [3.95464372e-01]
+ [3.90029023e-01]
+ [3.71189428e-01]
+ [3.60288147e-01]
+ [3.49208296e-01]
+ [3.52020409e-01]
+ [3.42216977e-01]
+ [3.32434656e-01]
+ [3.67894944e-01]
+ [3.62601467e-01]
+ [3.48185814e-01]
+ [9.20762948e-01]
+ [8.29017780e-01]
+ [7.38198019e-01]
+ [6.30827493e-01]
+ [5.01451044e-01]
+ [3.74633818e-01]
+ [4.91929873e-01]
+ [4.48171765e-01]
+ [3.84438425e-01]
+ [5.66298940e-01]
+ [7.51708203e-01]
+ [4.46387277e-10]]</t>
         </is>
       </c>
       <c r="E546" t="inlineStr"/>
@@ -14574,7 +14566,7 @@
       <c r="C548" t="inlineStr"/>
       <c r="D548" t="inlineStr">
         <is>
-          <t>[1.]</t>
+          <t>[0.90909091]</t>
         </is>
       </c>
       <c r="E548" t="inlineStr"/>
@@ -14621,26 +14613,26 @@
       </c>
       <c r="D550" t="inlineStr">
         <is>
-          <t>[[2.30719502e+10 6.04489020e+12 2.30719502e+10 6.04489020e+12
-  1.58821565e+10 1.79384436e+11]
- [2.09970029e+10 4.38691536e+12 2.09970029e+10 4.38691536e+12
-  1.47621565e+10 1.79384436e+11]
- [1.89220555e+10 3.08291584e+12 1.89220555e+10 3.08291584e+12
-  1.36421565e+10 1.79384436e+11]
- [1.68471081e+10 2.08864470e+12 1.68471081e+10 2.08864470e+12
-  1.25221565e+10 1.79384436e+11]
- [1.47721607e+10 1.35985505e+12 1.47721607e+10 1.35985505e+12
-  1.14021565e+10 1.79384436e+11]
- [1.26972134e+10 8.52299963e+11 1.26972134e+10 8.52299963e+11
-  1.02821565e+10 1.79384436e+11]
- [1.06222660e+10 5.21732532e+11 1.06222660e+10 5.21732532e+11
-  9.16215654e+09 1.79384436e+11]
- [8.54731864e+09 3.23905842e+11 8.54731864e+09 3.23905842e+11
-  8.04215654e+09 1.79384436e+11]
- [6.47237127e+09 2.14572979e+11 6.47237127e+09 2.14572979e+11
-  6.92215654e+09 1.79384436e+11]
- [4.39742390e+09 1.49487030e+11 4.39742390e+09 1.49487030e+11
-  5.80215654e+09 1.79384436e+11]]</t>
+          <t>[[2.25650526e+10 5.88608222e+12 2.25650526e+10 5.88608222e+12
+  1.52133333e+10 1.24226667e+11]
+ [2.04901053e+10 4.24064551e+12 2.04901053e+10 4.24064551e+12
+  1.40933333e+10 1.24226667e+11]
+ [1.84151579e+10 2.94918412e+12 1.84151579e+10 2.94918412e+12
+  1.29733333e+10 1.24226667e+11]
+ [1.63402105e+10 1.96745111e+12 1.63402105e+10 1.96745111e+12
+  1.18533333e+10 1.24226667e+11]
+ [1.42652632e+10 1.25119959e+12 1.42652632e+10 1.25119959e+12
+  1.07333333e+10 1.24226667e+11]
+ [1.21903158e+10 7.56182634e+11 1.21903158e+10 7.56182634e+11
+  9.61333333e+09 1.24226667e+11]
+ [1.01153684e+10 4.38153333e+11 1.01153684e+10 4.38153333e+11
+  8.49333333e+09 1.24226667e+11]
+ [8.04042105e+09 2.52864774e+11 8.04042105e+09 2.52864774e+11
+  7.37333333e+09 1.24226667e+11]
+ [5.96547368e+09 1.56070041e+11 5.96547368e+09 1.56070041e+11
+  6.25333333e+09 1.24226667e+11]
+ [3.89052632e+09 1.03522222e+11 3.89052632e+09 1.03522222e+11
+  5.13333333e+09 1.24226667e+11]]</t>
         </is>
       </c>
       <c r="E550" t="inlineStr"/>
@@ -14663,9 +14655,9 @@
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>[417.76067857 480.09738431 523.65058445 557.91160668 581.92125008
- 597.20357718 606.4643562  576.1548744  542.98427067 506.9184334
- 460.2271512  409.29061826 353.04163049]</t>
+          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
+ 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
+ 427.60678303 391.57616974 352.18249915]</t>
         </is>
       </c>
       <c r="E551" t="inlineStr"/>
@@ -14784,9 +14776,9 @@
       </c>
       <c r="D556" t="inlineStr">
         <is>
-          <t>[417.76067857 480.09738431 523.65058445 557.91160668 581.92125008
- 597.20357718 606.4643562  576.1548744  542.98427067 506.9184334
- 460.2271512  409.29061826 353.04163049]</t>
+          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
+ 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
+ 427.60678303 391.57616974 352.18249915]</t>
         </is>
       </c>
       <c r="E556" t="inlineStr"/>
@@ -14974,9 +14966,9 @@
       </c>
       <c r="D564" t="inlineStr">
         <is>
-          <t>[-417.76067857 -480.09738431 -523.65058445 -557.91160668 -581.92125008
- -597.20357718 -606.4643562  -576.1548744  -542.98427067 -506.9184334
- -460.2271512  -409.29061826 -353.04163049]</t>
+          <t>[-336.9560439  -388.43785582 -424.16473764 -452.12457083 -484.27449749
+ -510.65946695 -533.22010636 -511.58791739 -487.37587695 -460.61782438
+ -427.60678303 -391.57616974 -352.18249915]</t>
         </is>
       </c>
       <c r="E564" t="inlineStr"/>
@@ -15020,7 +15012,7 @@
       <c r="C566" t="inlineStr"/>
       <c r="D566" t="inlineStr">
         <is>
-          <t>[548.19001728 840.11957466 865.58606981 652.40952981]</t>
+          <t>[250.         257.72533448 343.6766274  469.23586931]</t>
         </is>
       </c>
       <c r="E566" t="inlineStr"/>
@@ -15039,7 +15031,7 @@
       <c r="C567" t="inlineStr"/>
       <c r="D567" t="inlineStr">
         <is>
-          <t>[1.         0.91930462 0.77872423 0.67543129]</t>
+          <t>[1.         1.         0.80780761 0.74262732]</t>
         </is>
       </c>
       <c r="E567" t="inlineStr"/>
@@ -15058,7 +15050,7 @@
       <c r="C568" t="inlineStr"/>
       <c r="D568" t="inlineStr">
         <is>
-          <t>[1.         0.91930462 0.77872423 0.67543129]</t>
+          <t>[1.         1.         0.80780761 0.74262732]</t>
         </is>
       </c>
       <c r="E568" t="inlineStr"/>
@@ -15077,7 +15069,7 @@
       <c r="C569" t="inlineStr"/>
       <c r="D569" t="inlineStr">
         <is>
-          <t>[0.62618683 0.82690382 0.97317659]</t>
+          <t>[0.97002493 0.67784333 0.57032058]</t>
         </is>
       </c>
       <c r="E569" t="inlineStr"/>
@@ -15120,9 +15112,9 @@
       </c>
       <c r="D571" t="inlineStr">
         <is>
-          <t>[6.21659639 6.21659639 6.21659639 6.21659639 6.04937951 5.88216264
- 5.71494576 5.29341943 4.87189309 4.45036676 3.96888349 3.48740022
- 3.00591695]</t>
+          <t>[5.         5.         5.         5.         5.         5.
+ 5.         4.67967935 4.35935869 4.03903804 3.69252536 3.34601268
+ 2.9995    ]</t>
         </is>
       </c>
       <c r="E571" t="inlineStr"/>
@@ -15373,9 +15365,9 @@
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 12.43319278 12.43319278 12.09875903 11.76432528
- 11.42989152 10.58683885  9.74378618  8.90073352  7.93776698  6.97480044
-  6.01183391]</t>
+          <t>[10.         10.         10.         10.         10.         10.
+ 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
+  5.999     ]</t>
         </is>
       </c>
       <c r="E582" t="inlineStr"/>
@@ -15628,7 +15620,7 @@
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>[7380.22340843 4437.75229644 3126.49285032 2230.93346263]</t>
+          <t>[10445.94134309 10134.04334639  6215.22949562  2762.32930662]</t>
         </is>
       </c>
       <c r="E593" t="inlineStr">
@@ -15655,7 +15647,7 @@
       </c>
       <c r="D594" t="inlineStr">
         <is>
-          <t>[142088.97893518  78782.96905178  40290.75954232  15456.46328398]</t>
+          <t>[129533.85103079 125696.32860397  63107.98029353  17033.32067808]</t>
         </is>
       </c>
       <c r="E594" t="inlineStr">
@@ -15682,7 +15674,7 @@
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>[142088.97893518  78782.96905178  40290.75954232  15456.46328398]</t>
+          <t>[129533.85103079 125696.32860397  63107.98029353  17033.32067808]</t>
         </is>
       </c>
       <c r="E595" t="inlineStr">
@@ -15709,7 +15701,7 @@
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>[3.40495996e+12 1.88792162e+12 9.65510653e+11 3.70392123e+11]</t>
+          <t>[3.10409420e+12 3.01213344e+12 1.51229284e+12 4.08179264e+11]</t>
         </is>
       </c>
       <c r="E596" t="inlineStr">
@@ -15736,7 +15728,7 @@
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>[3.40495996e+12 1.88792162e+12 9.65510653e+11 3.70392123e+11]</t>
+          <t>[3.10409420e+12 3.01213344e+12 1.51229284e+12 4.08179264e+11]</t>
         </is>
       </c>
       <c r="E597" t="inlineStr">
@@ -15763,7 +15755,7 @@
       </c>
       <c r="D598" t="inlineStr">
         <is>
-          <t>[2.70013324e+12 1.49712184e+12 7.65649948e+11 2.93720953e+11]</t>
+          <t>[2.46154670e+12 2.38862182e+12 1.19924822e+12 3.23686156e+11]</t>
         </is>
       </c>
       <c r="E598" t="inlineStr">
@@ -15790,7 +15782,7 @@
       </c>
       <c r="D599" t="inlineStr">
         <is>
-          <t>[1.76856540e+11 1.06344412e+11 7.49219470e+10 5.34611422e+10]</t>
+          <t>[2.50322103e+11 2.42847911e+11 1.48939120e+11 6.61952865e+10]</t>
         </is>
       </c>
       <c r="E599" t="inlineStr">
@@ -15898,10 +15890,10 @@
       </c>
       <c r="D603" t="inlineStr">
         <is>
-          <t>[[0.         0.         1.13086008 0.36514946 0.36514946 0.        ]
- [0.         0.         1.88068181 0.63199351 0.63199351 0.        ]
- [0.         0.         2.66944477 1.05284312 1.05284312 0.        ]
- [0.         0.         3.74103493 2.01307837 2.01307837 0.        ]]</t>
+          <t>[[0.         0.         0.7989706  0.32215517 0.32215517 0.        ]
+ [0.         0.         0.82356072 0.3319906  0.3319906  0.        ]
+ [0.         0.         1.34283054 0.59770421 0.59770421 0.        ]
+ [0.         0.         3.02136316 1.72437423 1.72437423 0.        ]]</t>
         </is>
       </c>
       <c r="E603" t="inlineStr"/>
@@ -15924,10 +15916,10 @@
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>[[1.86094236 1.86094236 0.         0.         0.         0.18257473]
- [3.09571733 3.09571733 0.         0.         0.         0.31599676]
- [4.39413739 4.39413739 0.         0.         0.         0.52642156]
- [6.15703966 6.15703966 0.         0.         0.         1.00653919]]</t>
+          <t>[[1.3135028  1.3135028  0.         0.         0.         0.16107759]
+ [1.35400229 1.35400229 0.         0.         0.         0.1659953 ]
+ [2.20869034 2.20869034 0.         0.         0.         0.29885211]
+ [4.97127384 4.97127384 0.         0.         0.         0.86218712]]</t>
         </is>
       </c>
       <c r="E604" t="inlineStr"/>
@@ -15950,7 +15942,7 @@
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>[464.14503893]</t>
+          <t>[603.37566942]</t>
         </is>
       </c>
       <c r="E605" t="inlineStr"/>
@@ -15973,7 +15965,7 @@
       </c>
       <c r="D606" t="inlineStr">
         <is>
-          <t>[2150911.87879668]</t>
+          <t>[3187423.76365581]</t>
         </is>
       </c>
       <c r="E606" t="inlineStr"/>
@@ -15996,8 +15988,8 @@
       </c>
       <c r="D607" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 12.43319278 12.2659759  11.93154215 11.5971084
- 11.00836519 10.16531252  9.32225985  8.41925025  7.45628371  6.49331718]</t>
+          <t>[10.         10.         10.         10.         10.         10.
+  9.67967935  9.03903804  8.39839673  7.7315634   7.03853804  6.34551268]</t>
         </is>
       </c>
       <c r="E607" t="inlineStr"/>
@@ -16020,8 +16012,8 @@
       </c>
       <c r="D608" t="inlineStr">
         <is>
-          <t>[0.02426807 0.02426807 0.02426807 0.01519635 0.01519635 0.01519635
- 0.01256592 0.01256592 0.01256592 0.01222886 0.01222886 0.01222886]</t>
+          <t>[0.0428     0.0428     0.0428     0.04151707 0.04151707 0.04151707
+ 0.02814207 0.02814207 0.02814207 0.01605    0.01605    0.01605   ]</t>
         </is>
       </c>
       <c r="E608" t="inlineStr"/>
@@ -16068,18 +16060,18 @@
       </c>
       <c r="D610" t="inlineStr">
         <is>
-          <t>[[ 9.79006382e+07]
- [ 8.87380371e+07]
- [ 7.95341247e+07]
- [ 1.07964417e+08]
- [ 9.05961339e+07]
- [ 7.07794149e+07]
- [ 7.50764220e+07]
- [ 6.50441509e+07]
- [ 4.96890701e+07]
- [ 3.00600870e+07]
- [-3.32235403e+06]
- [ 2.96350962e+06]]</t>
+          <t>[[85160115.64781867]
+ [77144862.65686788]
+ [69074882.4691234 ]
+ [59186173.25535725]
+ [47144587.25933338]
+ [35092813.37801799]
+ [43633613.40594918]
+ [37240893.81442108]
+ [28105994.82361823]
+ [28164299.01609978]
+ [-2061129.37148159]
+ [ 2912294.9222079 ]]</t>
         </is>
       </c>
       <c r="E610" t="inlineStr"/>
@@ -16102,18 +16094,18 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>[[ 4740837.5493982 ]
- [ 4741720.42915094]
- [ 4742523.88976027]
- [ 7679727.44018502]
- [ 7907649.33788322]
- [ 8148966.10483214]
- [10403260.98396178]
- [11315907.29393051]
- [12403317.19509637]
- [14205057.34714487]
- [16181021.57427453]
- [18791253.60108348]]</t>
+          <t>[[ 3385516.18198728]
+ [ 3386480.52306403]
+ [ 3387357.33789641]
+ [ 3494067.01412618]
+ [ 3495459.93285181]
+ [ 3496584.40829886]
+ [ 5328736.66915661]
+ [ 5731307.92404687]
+ [ 6199312.57267463]
+ [11861102.04008803]
+ [13124554.77252488]
+ [14686980.33880659]]</t>
         </is>
       </c>
       <c r="E611" t="inlineStr"/>
@@ -16136,18 +16128,18 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>[[-14014.38189606]
- [-15699.90106053]
- [-16940.38463472]
- [-28562.71262839]
- [-29546.59889714]
- [-30154.75466364]
- [-35794.11519753]
- [-33784.064856  ]
- [-31608.66420552]
- [-29863.06924407]
- [-26873.43145875]
- [-23754.25469068]]</t>
+          <t>[[ -6377.27477098]
+ [ -7144.27390968]
+ [ -7708.75864117]
+ [ -8500.11278108]
+ [ -9039.66575638]
+ [ -9492.10348399]
+ [-14030.3966498 ]
+ [-13390.233557  ]
+ [-12691.26282513]
+ [-20882.65728422]
+ [-19316.73388956]
+ [-17676.22885516]]</t>
         </is>
       </c>
       <c r="E612" t="inlineStr"/>
@@ -16200,18 +16192,18 @@
       <c r="C614" t="inlineStr"/>
       <c r="D614" t="inlineStr">
         <is>
-          <t>[[0.4998005 ]
- [0.45337554]
- [0.40678159]
- [0.55343502]
- [0.46616981]
- [0.36721618]
- [0.39284485]
- [0.34565446]
- [0.27545304]
- [0.19766334]
- [0.14355909]
- [0.16625766]]</t>
+          <t>[[0.43424776]
+ [0.39358338]
+ [0.35266569]
+ [0.30266886]
+ [0.24181473]
+ [0.1811783 ]
+ [0.22690854]
+ [0.19609057]
+ [0.15308259]
+ [0.17737901]
+ [0.11610867]
+ [0.13025544]]</t>
         </is>
       </c>
       <c r="E614" t="inlineStr"/>
@@ -16230,18 +16222,18 @@
       <c r="C615" t="inlineStr"/>
       <c r="D615" t="inlineStr">
         <is>
-          <t>[[0.29138726]
- [0.2799697 ]
- [0.26851411]
- [0.81536769]
- [0.7868178 ]
- [0.75959018]
- [0.99986315]
- [0.98088246]
- [0.96591403]
- [0.99759662]
- [0.99383111]
- [0.99808554]]</t>
+          <t>[[0.11263765]
+ [0.10718942]
+ [0.10176716]
+ [0.10664006]
+ [0.09895912]
+ [0.09139726]
+ [0.17443303]
+ [0.17062383]
+ [0.16779618]
+ [0.54868759]
+ [0.5473687 ]
+ [0.5494845 ]]</t>
         </is>
       </c>
       <c r="E615" t="inlineStr"/>
@@ -16260,18 +16252,18 @@
       <c r="C616" t="inlineStr"/>
       <c r="D616" t="inlineStr">
         <is>
-          <t>[[3.92207714]
- [3.56872823]
- [3.21557995]
- [4.53674587]
- [3.93499514]
- [3.25462659]
- [3.66936598]
- [3.44167137]
- [3.05916221]
- [2.62338504]
- [1.68532965]
- [2.36047832]]</t>
+          <t>[[1.153462  ]
+ [1.04809631]
+ [0.9428673 ]
+ [0.81865437]
+ [0.66548001]
+ [0.51362695]
+ [0.68369468]
+ [0.63849648]
+ [0.56491612]
+ [0.85718382]
+ [0.57120487]
+ [0.74229725]]</t>
         </is>
       </c>
       <c r="E616" t="inlineStr"/>
@@ -16387,7 +16379,7 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>[0.22292286]</t>
+          <t>[0.24028912]</t>
         </is>
       </c>
       <c r="E621" t="inlineStr"/>
@@ -16410,7 +16402,7 @@
       </c>
       <c r="D622" t="inlineStr">
         <is>
-          <t>[0.22546129]</t>
+          <t>[0.24257794]</t>
         </is>
       </c>
       <c r="E622" t="inlineStr"/>
@@ -16433,7 +16425,7 @@
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>[0.22292286 0.22546129 0.73298488 0.91691248 1.09108072 2.99985094]</t>
+          <t>[0.24028912 0.24257794 0.82002628 0.94741571 1.11042389 2.45606311]</t>
         </is>
       </c>
       <c r="E623" t="inlineStr"/>
@@ -16452,12 +16444,12 @@
       <c r="C624" t="inlineStr"/>
       <c r="D624" t="inlineStr">
         <is>
-          <t>[[ 9.49413522e-01 -1.41882066e-02  2.47608632e-01 -3.05299281e-01
-   1.22465334e-01]
- [ 2.38663040e+01  1.07429183e+01 -9.20258390e+01  1.27376642e+02
-  -6.89600249e+01]
- [-1.01195462e+02  2.49131108e+02 -4.02083107e+02  4.70035874e+02
-  -2.14888413e+02]]</t>
+          <t>[[ 1.34501898e+00  2.63037747e-02 -1.62860718e+00  1.86305912e+00
+  -6.05774696e-01]
+ [ 2.43922509e+02 -1.26897846e+02 -5.50694287e+02  9.84822297e+02
+  -5.50152673e+02]
+ [-6.62604757e+01  2.04175058e+02 -3.45153122e+02  3.55715411e+02
+  -1.47476871e+02]]</t>
         </is>
       </c>
       <c r="E624" t="inlineStr"/>
@@ -16476,12 +16468,12 @@
       <c r="C625" t="inlineStr"/>
       <c r="D625" t="inlineStr">
         <is>
-          <t>[[ 9.40664851e-01 -3.09581354e-02  3.20071407e-01 -4.02083207e-01
-   1.72305084e-01]
- [ 1.21940429e+01  9.45572002e+00 -5.72969301e+01  7.81666259e+01
-  -4.15194588e+01]
- [-9.88603449e+01  2.40765067e+02 -3.87648259e+02  4.53084675e+02
-  -2.06341138e+02]]</t>
+          <t>[[ 1.33441864e+00  1.08008412e-02 -1.53938295e+00  1.73648648e+00
+  -5.42323007e-01]
+ [ 3.34067160e+01 -2.76697235e+00 -1.17287288e+02  1.86946290e+02
+  -9.92987464e+01]
+ [-6.28982452e+01  1.89813976e+02 -3.17392821e+02  3.25276034e+02
+  -1.33798945e+02]]</t>
         </is>
       </c>
       <c r="E625" t="inlineStr"/>
@@ -16500,7 +16492,7 @@
       <c r="C626" t="inlineStr"/>
       <c r="D626" t="inlineStr">
         <is>
-          <t>[[  5.30600273 -17.72928442  30.10491313 -24.26841271   7.58678128]
+          <t>[[  7.20897396 -26.02206851  41.96140358 -31.41461906   9.26631002]
  [  0.           0.           0.           0.           0.        ]
  [  0.           0.           0.           0.           0.        ]]</t>
         </is>
@@ -16525,7 +16517,7 @@
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>[0.22546129 1.09108072 3.04297678]</t>
+          <t>[0.24257794 1.11042389 2.52992596]</t>
         </is>
       </c>
       <c r="E627" t="inlineStr"/>
@@ -16548,7 +16540,7 @@
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>[0.22292286 0.91691248 2.99985094]</t>
+          <t>[0.24028912 0.94741571 2.45606311]</t>
         </is>
       </c>
       <c r="E628" t="inlineStr"/>
@@ -16571,7 +16563,7 @@
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>[3.92698209 0.         0.        ]</t>
+          <t>[4.93880443 0.         0.        ]</t>
         </is>
       </c>
       <c r="E629" t="inlineStr"/>
@@ -16595,18 +16587,18 @@
       <c r="D630" t="inlineStr">
         <is>
           <t>[[0.        ]
- [0.00760812]
- [0.02827031]
- [0.06080304]
- [0.13294296]
- [0.23676733]
- [0.36845331]
- [0.46038808]
- [0.56274937]
- [0.67539685]
- [0.7893445 ]
- [0.91040975]
- [1.0347329 ]]</t>
+ [0.00807209]
+ [0.03045285]
+ [0.06583858]
+ [0.13671459]
+ [0.2282204 ]
+ [0.33638004]
+ [0.40917257]
+ [0.48865184]
+ [0.57448606]
+ [0.66205771]
+ [0.75623898]
+ [0.85318342]]</t>
         </is>
       </c>
       <c r="E630" t="inlineStr"/>
@@ -16629,7 +16621,7 @@
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>[1.0347329]</t>
+          <t>[0.85318342]</t>
         </is>
       </c>
       <c r="E631" t="inlineStr"/>
@@ -16652,17 +16644,17 @@
       </c>
       <c r="D632" t="inlineStr">
         <is>
-          <t>[[-12730521.72143568]
- [-11850886.87887046]
- [-10970787.07175203]
- [-10189538.98252747]
- [ -9429015.43524477]
- [ -8689342.32671024]
- [ -8339717.27880802]
- [ -8016756.87143007]
- [ -7720490.61221403]
- [ -7477270.18058252]
- [ -7261843.49422376]
+          <t>[[-17427765.12991663]
+ [-16186366.78221211]
+ [-14944587.88685458]
+ [-13222849.37497341]
+ [-11500611.20008019]
+ [ -9777955.21838797]
+ [ -9097151.95187112]
+ [ -8461409.45930777]
+ [ -7870754.04360263]
+ [ -7579102.67267725]
+ [ -7313593.23878349]
  [ -7074256.2758736 ]]</t>
         </is>
       </c>
@@ -16686,18 +16678,18 @@
       </c>
       <c r="D633" t="inlineStr">
         <is>
-          <t>[[2428202.60258269]
- [2428678.38301451]
- [2429111.49063849]
- [2429560.06791994]
- [2430215.49135759]
- [2430750.37827718]
- [2429479.23253397]
- [2429523.57455143]
- [2429538.88915186]
- [2429361.17520323]
- [2429276.72132152]
- [2429134.03768572]]</t>
+          <t>[[2428340.58969823]
+ [2429076.44059267]
+ [2429745.66121794]
+ [2431464.41489253]
+ [2432495.54674606]
+ [2433328.43446587]
+ [2430320.56243432]
+ [2430367.54182217]
+ [2430375.83291243]
+ [2429248.39987909]
+ [2429220.83731715]
+ [2429127.58409672]]</t>
         </is>
       </c>
       <c r="E633" t="inlineStr"/>
@@ -16720,18 +16712,18 @@
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>[[29098.38222475]
- [29104.74146934]
- [29110.58948486]
- [29116.76283907]
- [29125.95242289]
- [29133.73436025]
- [29116.45599326]
- [29117.39204292]
- [29118.03862504]
- [29115.99795827]
- [29115.49432309]
- [29114.44234276]]</t>
+          <t>[[29100.21334624]
+ [29110.04393666]
+ [29119.07546929]
+ [29142.38007936]
+ [29156.79240186]
+ [29168.82090949]
+ [29127.92088216]
+ [29128.99893601]
+ [29129.67529452]
+ [29114.12772248]
+ [29114.60165251]
+ [29114.41196808]]</t>
         </is>
       </c>
       <c r="E634" t="inlineStr"/>
@@ -16754,18 +16746,18 @@
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>[[-4361007.15030931]
- [-4006298.04736741]
- [-3649931.2024322 ]
- [-3137543.02001618]
- [-2621388.15215144]
- [-2102512.96128891]
- [-1790296.78649906]
- [-1477154.77232377]
- [-1163071.91054673]
- [ -869072.3886961 ]
- [ -574194.72779434]
- [ -278501.85530974]]</t>
+          <t>[[-4355770.84979259]
+ [-3999369.51509918]
+ [-3640497.12021613]
+ [-3124519.02847233]
+ [-2606354.23982125]
+ [-2087563.38387338]
+ [-1776650.06345185]
+ [-1465466.49623692]
+ [-1154071.36764904]
+ [ -862996.74568595]
+ [ -571078.64832484]
+ [ -278501.90073832]]</t>
         </is>
       </c>
       <c r="E635" t="inlineStr"/>
@@ -16788,18 +16780,18 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>[[ 3.26275934e+08]
- [ 2.96704586e+08]
- [ 2.67010748e+08]
- [ 2.24351073e+08]
- [ 1.81424129e+08]
- [ 1.38313439e+08]
- [ 1.12392639e+08]
- [ 8.64176612e+07]
- [ 6.03932815e+07]
- [ 3.60669741e+07]
- [ 1.17151829e+07]
- [-1.26341964e+07]]</t>
+          <t>[[ 3.26042330e+08]
+ [ 2.96343964e+08]
+ [ 2.66462894e+08]
+ [ 2.23535771e+08]
+ [ 1.80456648e+08]
+ [ 1.37343596e+08]
+ [ 1.11509659e+08]
+ [ 8.56652885e+07]
+ [ 5.98176693e+07]
+ [ 3.56818040e+07]
+ [ 1.15214098e+07]
+ [-1.26341969e+07]]</t>
         </is>
       </c>
       <c r="E636" t="inlineStr"/>
@@ -16822,18 +16814,18 @@
       </c>
       <c r="D637" t="inlineStr">
         <is>
-          <t>[[1299696.81579559]
- [1299681.58727972]
- [1299666.34815927]
- [1299768.50116918]
- [1299754.61853755]
- [1299740.54894056]
- [1299789.15645825]
- [1299802.10378469]
- [1299818.58563886]
- [1299852.85779559]
- [1299889.60688801]
- [1299939.10849629]]</t>
+          <t>[[1299689.54225215]
+ [1299674.3537992 ]
+ [1299659.15932317]
+ [1299649.59012126]
+ [1299627.86871814]
+ [1299606.14173766]
+ [1299648.83929164]
+ [1299648.18318422]
+ [1299648.4245459 ]
+ [1299792.63859019]
+ [1299811.86142551]
+ [1299836.63664036]]</t>
         </is>
       </c>
       <c r="E637" t="inlineStr"/>
@@ -16856,9 +16848,9 @@
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>[[  2427925.55809716]
+          <t>[[  2427925.55809668]
  [    29094.73368413]
- [-13609523.83933535]]</t>
+ [-18668642.37894937]]</t>
         </is>
       </c>
       <c r="E638" t="inlineStr"/>
@@ -16881,8 +16873,8 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>[[-4.71357613e+06]
- [ 3.55687256e+08]
+          <t>[[-4.70896222e+06]
+ [ 3.55500528e+08]
  [ 1.29946107e+06]]</t>
         </is>
       </c>
@@ -16906,7 +16898,7 @@
       </c>
       <c r="D640" t="inlineStr">
         <is>
-          <t>[1625606.93571539]</t>
+          <t>[2142593.51976615]</t>
         </is>
       </c>
       <c r="E640" t="inlineStr"/>
@@ -16929,7 +16921,7 @@
       </c>
       <c r="D641" t="inlineStr">
         <is>
-          <t>[-3.93513649e+00 -5.81329521e-02  1.22745569e+02]</t>
+          <t>[-2.98562705e+00 -4.41060468e-02  1.08214197e+02]</t>
         </is>
       </c>
       <c r="E641" t="inlineStr"/>
@@ -16952,7 +16944,7 @@
       </c>
       <c r="D642" t="inlineStr">
         <is>
-          <t>[2.93222946e+10 2.91848076e+10 2.79277543e+08 7.86163621e+02
+          <t>[3.18866698e+10 3.17491828e+10 2.84709346e+08 7.86163621e+02
  1.35359722e+07 1.70976373e+05]</t>
         </is>
       </c>
@@ -18461,7 +18453,7 @@
       </c>
       <c r="D695" t="inlineStr">
         <is>
-          <t>[3.29001049]</t>
+          <t>[2.8838056]</t>
         </is>
       </c>
       <c r="E695" t="inlineStr"/>
@@ -19593,8 +19585,7 @@
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>[12.43319258 12.4331927  12.4331927  12.43319276 12.43319278 12.43319278
- 12.43319278]</t>
+          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
         </is>
       </c>
       <c r="E737" t="inlineStr">
@@ -19621,7 +19612,8 @@
       </c>
       <c r="D738" t="inlineStr">
         <is>
-          <t>[[0.077 0.077 0.077 0.077 0.077 0.077 0.077]]</t>
+          <t>[[0.077      0.077      0.10095695 0.10347047 0.1052105  0.09579198
+  0.08345544]]</t>
         </is>
       </c>
       <c r="E738" t="inlineStr">
@@ -19837,7 +19829,7 @@
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>[12.43319278 12.43319278 11.42989152  8.90073352  6.01183391]</t>
+          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
         </is>
       </c>
       <c r="E746" t="inlineStr">
@@ -19887,7 +19879,7 @@
       </c>
       <c r="D748" t="inlineStr">
         <is>
-          <t>[[0.02921938 0.01614151 0.01226288 0.01122482 0.01163286]]</t>
+          <t>[[0.04       0.04       0.03760199 0.015      0.015     ]]</t>
         </is>
       </c>
       <c r="E748" t="inlineStr">

</xml_diff>

<commit_message>
Updated driver script to reset monopile diam before opt
</commit_message>
<xml_diff>
--- a/examples/99_tower_gbf/15mw/20m/outputs_mono/monotow_output.xlsx
+++ b/examples/99_tower_gbf/15mw/20m/outputs_mono/monotow_output.xlsx
@@ -914,8 +914,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>[[0.077      0.077      0.10095695 0.10347047 0.1052105  0.09579198
-  0.08345544]]</t>
+          <t>[[0.077 0.077 0.077 0.077 0.077 0.077 0.077]]</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
@@ -938,7 +937,8 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494085 11.18494083 11.18494083
+ 11.18494083]</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
@@ -1635,7 +1635,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>[10.]</t>
+          <t>[11.18408627]</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>[11.]</t>
+          <t>[11.18494083]</t>
         </is>
       </c>
       <c r="E53" t="inlineStr"/>
@@ -3519,7 +3519,7 @@
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>[[0.04       0.04       0.03760199 0.015      0.015     ]]</t>
+          <t>[[0.03877828 0.03036317 0.01500077 0.015      0.015     ]]</t>
         </is>
       </c>
       <c r="E138" t="inlineStr"/>
@@ -3542,7 +3542,7 @@
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
+          <t>[11.18408627 11.18408435 11.18420297  7.68807778  5.99900001]</t>
         </is>
       </c>
       <c r="E139" t="inlineStr"/>
@@ -4573,10 +4573,10 @@
       </c>
       <c r="D180" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          76069.22818689
-  76419.81487525  77475.80310771  79250.00595527  81764.21915156
-  85049.92502601  89149.36708317 100022.09247963 115010.75107985
- 135096.15327474      0.              0.              0.
+          <t>[     0.              0.              0.          78565.31757154
+  78927.1602561   80017.05386019  81848.22904544  84443.19581949
+  87834.4763627   92065.72326944 103288.62402897 118761.87556321
+ 139500.77063907      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -4827,8 +4827,10 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>[11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11.
- 11.]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494084 11.18494084 11.18494084
+ 11.18494084 11.18494085 11.18494085 11.18494085 11.18494084 11.18494084
+ 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083
+ 11.18494083]</t>
         </is>
       </c>
       <c r="E190" t="inlineStr"/>
@@ -4969,10 +4971,10 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          76069.22818689
-  76419.81487525  77475.80310771  79250.00595527  81764.21915156
-  85049.92502601  89149.36708317 100022.09247963 115010.75107985
- 135096.15327474      0.              0.              0.
+          <t>[     0.              0.              0.          78565.31757154
+  78927.1602561   80017.05386019  81848.22904544  84443.19581949
+  87834.4763627   92065.72326944 103288.62402897 118761.87556321
+ 139500.77063907      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -5115,10 +5117,10 @@
       </c>
       <c r="D202" t="inlineStr">
         <is>
-          <t>[      0.               0.               0.          -76069.22818689
-  -76419.81487525  -77475.80310771  -79250.00595527  -81764.21915156
-  -85049.92502601  -89149.36708317 -100022.09247963 -115010.75107985
- -135096.15327474       0.               0.               0.
+          <t>[      0.               0.               0.          -78565.31757154
+  -78927.1602561   -80017.05386019  -81848.22904544  -84443.19581949
+  -87834.4763627   -92065.72326944 -103288.62402897 -118761.87556321
+ -139500.77063907       0.               0.               0.
        0.               0.               0.        ]</t>
         </is>
       </c>
@@ -5169,7 +5171,8 @@
       </c>
       <c r="D204" t="inlineStr">
         <is>
-          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494085 11.18494083 11.18494083
+ 11.18494083]</t>
         </is>
       </c>
       <c r="E204" t="inlineStr"/>
@@ -5192,7 +5195,7 @@
       </c>
       <c r="D205" t="inlineStr">
         <is>
-          <t>[0.077      0.08897847 0.10221371 0.10434048 0.10050124 0.08962371]</t>
+          <t>[0.077 0.077 0.077 0.077 0.077 0.077]</t>
         </is>
       </c>
       <c r="E205" t="inlineStr"/>
@@ -5258,7 +5261,8 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494085 11.18494083 11.18494083
+ 11.18494083]</t>
         </is>
       </c>
       <c r="E208" t="inlineStr"/>
@@ -5281,7 +5285,7 @@
       </c>
       <c r="D209" t="inlineStr">
         <is>
-          <t>[0.077      0.08897847 0.10221371 0.10434048 0.10050124 0.08962371]</t>
+          <t>[0.077 0.077 0.077 0.077 0.077 0.077]</t>
         </is>
       </c>
       <c r="E209" t="inlineStr"/>
@@ -5544,9 +5548,8 @@
       </c>
       <c r="D220" t="inlineStr">
         <is>
-          <t>[0.077      0.077      0.077      0.08897847 0.08897847 0.08897847
- 0.10221371 0.10221371 0.10221371 0.10434048 0.10434048 0.10434048
- 0.10050124 0.10050124 0.10050124 0.08962371 0.08962371 0.08962371]</t>
+          <t>[0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077 0.077
+ 0.077 0.077 0.077 0.077 0.077 0.077]</t>
         </is>
       </c>
       <c r="E220" t="inlineStr"/>
@@ -5710,7 +5713,7 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>[1648375.1234354]</t>
+          <t>[1457692.41156949]</t>
         </is>
       </c>
       <c r="E227" t="inlineStr"/>
@@ -5733,7 +5736,7 @@
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>[3980261.24221089]</t>
+          <t>[3565596.39650365]</t>
         </is>
       </c>
       <c r="E228" t="inlineStr"/>
@@ -5756,7 +5759,7 @@
       </c>
       <c r="D229" t="inlineStr">
         <is>
-          <t>[34.4331827]</t>
+          <t>[32.49999999]</t>
         </is>
       </c>
       <c r="E229" t="inlineStr"/>
@@ -5779,7 +5782,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>[2.54169442e+09 2.54169442e+09 4.90525923e+07 0.00000000e+00
+          <t>[2.07540031e+09 2.07540031e+09 4.49669971e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -5803,7 +5806,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>[1175518.62964259]</t>
+          <t>[902219.78162679]</t>
         </is>
       </c>
       <c r="E231" t="inlineStr"/>
@@ -5826,7 +5829,7 @@
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>[3187423.76365581]</t>
+          <t>[2634279.06642127]</t>
         </is>
       </c>
       <c r="E232" t="inlineStr"/>
@@ -5873,26 +5876,26 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>[[2.25650526e+10 5.88608222e+12 2.25650526e+10 5.88608222e+12
-  1.52133333e+10 1.24226667e+11]
- [2.04901053e+10 4.24064551e+12 2.04901053e+10 4.24064551e+12
-  1.40933333e+10 1.24226667e+11]
- [1.84151579e+10 2.94918412e+12 1.84151579e+10 2.94918412e+12
-  1.29733333e+10 1.24226667e+11]
- [1.63402105e+10 1.96745111e+12 1.63402105e+10 1.96745111e+12
-  1.18533333e+10 1.24226667e+11]
- [1.42652632e+10 1.25119959e+12 1.42652632e+10 1.25119959e+12
-  1.07333333e+10 1.24226667e+11]
- [1.21903158e+10 7.56182634e+11 1.21903158e+10 7.56182634e+11
-  9.61333333e+09 1.24226667e+11]
- [1.01153684e+10 4.38153333e+11 1.01153684e+10 4.38153333e+11
-  8.49333333e+09 1.24226667e+11]
- [8.04042105e+09 2.52864774e+11 8.04042105e+09 2.52864774e+11
-  7.37333333e+09 1.24226667e+11]
- [5.96547368e+09 1.56070041e+11 5.96547368e+09 1.56070041e+11
-  6.25333333e+09 1.24226667e+11]
- [3.89052632e+09 1.03522222e+11 3.89052632e+09 1.03522222e+11
-  5.13333333e+09 1.24226667e+11]]</t>
+          <t>[[2.26304633e+10 5.90517775e+12 2.26304633e+10 5.90517775e+12
+  1.52996391e+10 1.30598399e+11]
+ [2.05555159e+10 4.25820929e+12 2.05555159e+10 4.25820929e+12
+  1.41796391e+10 1.30598399e+11]
+ [1.84805686e+10 2.96521614e+12 1.84805686e+10 2.96521614e+12
+  1.30596391e+10 1.30598399e+11]
+ [1.64056212e+10 1.98195139e+12 1.64056212e+10 1.98195139e+12
+  1.19396391e+10 1.30598399e+11]
+ [1.43306738e+10 1.26416811e+12 1.43306738e+10 1.26416811e+12
+  1.08196391e+10 1.30598399e+11]
+ [1.22557264e+10 7.67619410e+11 1.22557264e+10 7.67619410e+11
+  9.69963906e+09 1.30598399e+11]
+ [1.01807791e+10 4.48058360e+11 1.01807791e+10 4.48058360e+11
+  8.57963906e+09 1.30598399e+11]
+ [8.10583171e+09 2.61238050e+11 8.10583171e+09 2.61238050e+11
+  7.45963906e+09 1.30598399e+11]
+ [6.03088434e+09 1.62911568e+11 6.03088434e+09 1.62911568e+11
+  6.33963906e+09 1.30598399e+11]
+ [3.95593697e+09 1.08831999e+11 3.95593697e+09 1.08831999e+11
+  5.21963906e+09 1.30598399e+11]]</t>
         </is>
       </c>
       <c r="E234" t="inlineStr"/>
@@ -5915,9 +5918,9 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>[2.82726365 2.82726365 2.82726365 3.263503   3.263503   3.263503
- 3.74438999 3.74438999 3.74438999 3.82155405 3.82155405 3.82155405
- 3.6822358  3.6822358  3.6822358  3.28697421 3.28697421 3.28697421]</t>
+          <t>[2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296]</t>
         </is>
       </c>
       <c r="E235" t="inlineStr"/>
@@ -5940,9 +5943,9 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
- 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
- 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599 ]</t>
+          <t>[1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219]</t>
         </is>
       </c>
       <c r="E236" t="inlineStr"/>
@@ -5965,9 +5968,9 @@
       </c>
       <c r="D237" t="inlineStr">
         <is>
-          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
- 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
- 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599 ]</t>
+          <t>[1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219]</t>
         </is>
       </c>
       <c r="E237" t="inlineStr"/>
@@ -5990,9 +5993,9 @@
       </c>
       <c r="D238" t="inlineStr">
         <is>
-          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
- 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
- 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073]</t>
+          <t>[44.34615103 44.34615101 44.34615099 44.34615098 44.34615099 44.34615101
+ 44.34615102 44.34615105 44.34615107 44.34615104 44.34615097 44.34615089
+ 44.34615085 44.34615085 44.34615084 44.34615083 44.34615082 44.34615081]</t>
         </is>
       </c>
       <c r="E238" t="inlineStr"/>
@@ -6015,9 +6018,9 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
- 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
- 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073]</t>
+          <t>[44.34615103 44.34615101 44.34615099 44.34615098 44.34615099 44.34615101
+ 44.34615102 44.34615105 44.34615107 44.34615104 44.34615097 44.34615089
+ 44.34615085 44.34615085 44.34615084 44.34615083 44.34615082 44.34615081]</t>
         </is>
       </c>
       <c r="E239" t="inlineStr"/>
@@ -6040,10 +6043,9 @@
       </c>
       <c r="D240" t="inlineStr">
         <is>
-          <t>[ 84.33576062  84.33576062  84.33576062  97.1367864   97.1367864
-  97.1367864  111.18235328 111.18235328 111.18235328 113.42972734
- 113.42972734 113.42972734 109.3708483  109.3708483  109.3708483
-  97.82392145  97.82392145  97.82392145]</t>
+          <t>[88.69230205 88.69230201 88.69230197 88.69230196 88.69230199 88.69230201
+ 88.69230205 88.6923021  88.69230214 88.69230209 88.69230194 88.69230178
+ 88.6923017  88.69230169 88.69230168 88.69230166 88.69230164 88.69230162]</t>
         </is>
       </c>
       <c r="E240" t="inlineStr"/>
@@ -6238,8 +6240,8 @@
       </c>
       <c r="D247" t="inlineStr">
         <is>
-          <t>[1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
- 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
+          <t>[1.29568103 1.29568096 1.29568088 0.85100867 0.85101169 0.8510147
+ 0.53381296 0.47505025 0.41628754 0.37270164 0.34431243 0.31592322]</t>
         </is>
       </c>
       <c r="E247" t="inlineStr"/>
@@ -6262,8 +6264,8 @@
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E248" t="inlineStr"/>
@@ -6286,8 +6288,8 @@
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E249" t="inlineStr"/>
@@ -6310,8 +6312,8 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E250" t="inlineStr"/>
@@ -6334,8 +6336,8 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E251" t="inlineStr"/>
@@ -6358,8 +6360,8 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>[33.21380796 33.21380796 33.21380796 32.22982785 32.22982785 32.22982785
- 19.88323673 16.18153341 12.97038057  5.79213059  4.36751812  3.19804084]</t>
+          <t>[40.26746178 40.26745485 40.26744792 26.50420959 26.50449127 26.50477295
+ 14.9567086  10.54113983  7.093319    5.09068091  4.01375054  3.10053978]</t>
         </is>
       </c>
       <c r="E252" t="inlineStr"/>
@@ -6453,9 +6455,9 @@
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>[10.         10.         10.         10.         10.         10.
- 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
-  5.999     ]</t>
+          <t>[11.18408627 11.18408563 11.18408499 11.18408435 11.18412389 11.18416343
+ 11.18420297 10.01882791  8.85345284  7.68807778  7.12505186  6.56202594
+  5.99900001]</t>
         </is>
       </c>
       <c r="E256" t="inlineStr"/>
@@ -6478,8 +6480,8 @@
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>[0.04     0.04     0.04     0.038801 0.038801 0.038801 0.026301 0.026301
- 0.026301 0.015    0.015    0.015   ]</t>
+          <t>[0.03457072 0.03457072 0.03457072 0.02268197 0.02268197 0.02268197
+ 0.01500039 0.01500039 0.01500039 0.015      0.015      0.015     ]</t>
         </is>
       </c>
       <c r="E257" t="inlineStr"/>
@@ -6584,9 +6586,9 @@
       </c>
       <c r="D261" t="inlineStr">
         <is>
-          <t>[[  2427925.55809668]
- [    29094.73368413]
- [-18668642.37894937]]</t>
+          <t>[[  2427925.55809758]
+ [    29094.73368414]
+ [-15993436.94101516]]</t>
         </is>
       </c>
       <c r="E261" t="inlineStr"/>
@@ -6609,8 +6611,8 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>[[-4.70896222e+06]
- [ 3.55500528e+08]
+          <t>[[-4.70178935e+06]
+ [ 3.54843036e+08]
  [ 1.29946107e+06]]</t>
         </is>
       </c>
@@ -6634,7 +6636,7 @@
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>[1512500.         1512500.         3024999.99999999       0.
+          <t>[1563786.26610091 1563786.26610091 3127572.53220183       0.
        0.               0.        ]</t>
         </is>
       </c>
@@ -6727,7 +6729,7 @@
       </c>
       <c r="D267" t="inlineStr">
         <is>
-          <t>[2142593.51976615]</t>
+          <t>[1869294.67175035]</t>
         </is>
       </c>
       <c r="E267" t="inlineStr"/>
@@ -6750,7 +6752,7 @@
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>[-2.98562705e+00 -4.41060468e-02  1.08214197e+02]</t>
+          <t>[-3.42213845e+00 -5.05545388e-02  1.13442233e+02]</t>
         </is>
       </c>
       <c r="E268" t="inlineStr"/>
@@ -6773,7 +6775,7 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>[3.18866698e+10 3.17491828e+10 2.84709346e+08 7.86163621e+02
+          <t>[3.02649976e+10 3.01275105e+10 2.82981459e+08 7.86163621e+02
  1.35359722e+07 1.70976373e+05]</t>
         </is>
       </c>
@@ -6882,16 +6884,16 @@
           <t>[[      0.        ]
  [      0.        ]
  [      0.        ]
- [ -76069.22818689]
- [ -76419.81487525]
- [ -77475.80310771]
- [ -79250.00595527]
- [ -81764.21915156]
- [ -85049.92502601]
- [ -89149.36708317]
- [-100022.09247963]
- [-115010.75107985]
- [-135096.15327474]
+ [ -78565.31757154]
+ [ -78927.1602561 ]
+ [ -80017.05386019]
+ [ -81848.22904544]
+ [ -84443.19581949]
+ [ -87834.4763627 ]
+ [ -92065.72326944]
+ [-103288.62402897]
+ [-118761.87556321]
+ [-139500.77063907]
  [      0.        ]
  [      0.        ]
  [      0.        ]
@@ -6990,19 +6992,19 @@
       </c>
       <c r="D275" t="inlineStr">
         <is>
-          <t>[[-336.9560439 ]
- [-388.43785582]
- [-424.16473764]
- [-452.12457083]
- [-484.27449749]
- [-510.65946695]
- [-533.22010636]
- [-511.58791739]
- [-487.37587695]
- [-460.61782438]
- [-427.60678303]
- [-391.57616974]
- [-352.18249915]]</t>
+          <t>[[-376.8637364 ]
+ [-433.4947406 ]
+ [-472.91020584]
+ [-503.8274884 ]
+ [-539.45978844]
+ [-568.76856759]
+ [-593.87710694]
+ [-546.37921754]
+ [-494.76103473]
+ [-438.15146599]
+ [-411.93099011]
+ [-383.31695362]
+ [-352.18250007]]</t>
         </is>
       </c>
       <c r="E275" t="inlineStr"/>
@@ -7025,24 +7027,24 @@
       </c>
       <c r="D276" t="inlineStr">
         <is>
-          <t>[[-36123346.97588959]
- [-33960790.79041462]
- [-31421691.94796431]
- [-30879849.66133218]
- [-30336846.93487328]
- [-29791509.30376027]
- [-29181329.17357343]
- [-28566364.10790942]
- [-27945306.30131707]
- [-26658812.50241386]
- [-25329647.43537711]
- [-23942610.16605137]
- [-22780861.82640503]
- [-21842022.14135061]
- [-20903182.45629581]
- [-20484151.47503773]
- [-20065120.49377933]
- [-19646089.51252162]]</t>
+          <t>[[-31622722.37489413]
+ [-29423551.23121068]
+ [-26835481.76696547]
+ [-26339021.94528637]
+ [-25841364.44276518]
+ [-25341297.06371611]
+ [-24837578.11870414]
+ [-24328920.51751414]
+ [-23813974.32813288]
+ [-22758582.61770878]
+ [-21659142.25010826]
+ [-20499951.85134015]
+ [-19536718.54349031]
+ [-18803661.49559565]
+ [-18070604.44770125]
+ [-17704075.92375403]
+ [-17337547.39980648]
+ [-16971018.87585953]]</t>
         </is>
       </c>
       <c r="E276" t="inlineStr"/>
@@ -7065,24 +7067,24 @@
       </c>
       <c r="D277" t="inlineStr">
         <is>
-          <t>[[-3571386.85080247]
- [-8980999.77048393]
- [-9160127.16752138]
- [ 2428093.82801644]
- [ 2428113.53256131]
- [ 2428133.56642783]
- [ 2428177.55584712]
- [ 2428198.07321296]
- [ 2428219.29887818]
- [ 2428588.30264015]
- [ 2428684.72498103]
- [ 2428793.4671491 ]
- [ 2428772.71401341]
- [ 2428620.0939148 ]
- [ 2428670.77338876]
- [ 2428275.82942879]
- [ 2428288.03473593]
- [ 2428300.09340087]]</t>
+          <t>[[-3579144.75489268]
+ [-8863696.04876918]
+ [-8945585.5771961 ]
+ [ 2428075.16753127]
+ [ 2428094.90884762]
+ [ 2428114.99911463]
+ [ 2428135.58832508]
+ [ 2428156.83499969]
+ [ 2428178.90975678]
+ [ 2428501.35821275]
+ [ 2428603.88146218]
+ [ 2428721.3472541 ]
+ [ 2428717.29176938]
+ [ 2428532.63752758]
+ [ 2428581.32421195]
+ [ 2428271.34463096]
+ [ 2428283.09213585]
+ [ 2428294.6982198 ]]</t>
         </is>
       </c>
       <c r="E277" t="inlineStr"/>
@@ -7105,24 +7107,24 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>[[ -46612.79626053]
- [-117471.93621095]
- [-120846.42288106]
- [  29096.92151658]
- [  29097.17898185]
- [  29097.44093214]
- [  29098.01559855]
- [  29098.28422904]
- [  29098.56230757]
- [  29103.37730347]
- [  29104.64273106]
- [  29106.07123526]
- [  29105.80901867]
- [  29103.82156847]
- [  29104.49322739]
- [  29099.32366656]
- [  29099.48597565]
- [  29099.64652502]]</t>
+          <t>[[ -46724.04266973]
+ [-115969.30452781]
+ [-118073.97522221]
+ [  29096.67851973]
+ [  29096.93651114]
+ [  29097.19924445]
+ [  29097.46868375]
+ [  29097.74690746]
+ [  29098.03615519]
+ [  29102.2448058 ]
+ [  29103.59050806]
+ [  29105.13386418]
+ [  29105.09037856]
+ [  29102.68221936]
+ [  29103.3276242 ]
+ [  29099.26843232]
+ [  29099.42469379]
+ [  29099.57925817]]</t>
         </is>
       </c>
       <c r="E278" t="inlineStr"/>
@@ -7145,24 +7147,24 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>[[ -526598.7774628 ]
- [-2406071.56195532]
- [-4715198.34905789]
- [-5431349.17696918]
- [-5382395.25464339]
- [-5333402.76688932]
- [-5284377.98404438]
- [-5235325.59908948]
- [-5186247.67118431]
- [-5088011.01723978]
- [-4989699.00157361]
- [-4891329.46663574]
- [-4792918.5016765 ]
- [-4694465.88006755]
- [-4595969.73165049]
- [-4546715.11585086]
- [-4497449.51364613]
- [-4448174.12628585]]</t>
+          <t>[[ -544552.94323635]
+ [-2424814.09229682]
+ [-4699531.50475682]
+ [-5420967.81261888]
+ [-5372088.75750023]
+ [-5323173.54503663]
+ [-5274224.28235081]
+ [-5225243.09037663]
+ [-5176232.11270024]
+ [-5078116.93615036]
+ [-4979906.92994198]
+ [-4881621.09241059]
+ [-4783279.59214913]
+ [-4684884.82166152]
+ [-4586432.75056777]
+ [-4537196.13107404]
+ [-4487949.6235716 ]
+ [-4438694.38206342]]</t>
         </is>
       </c>
       <c r="E279" t="inlineStr"/>
@@ -7185,24 +7187,24 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>[[4.05032729e+07]
- [1.84726748e+08]
- [3.60998049e+08]
- [4.15644529e+08]
- [4.11562418e+08]
- [4.07477361e+08]
- [4.03389850e+08]
- [3.99300236e+08]
- [3.95208680e+08]
- [3.87019429e+08]
- [3.78824481e+08]
- [3.70625212e+08]
- [3.62422859e+08]
- [3.54217416e+08]
- [3.46008748e+08]
- [3.41903950e+08]
- [3.37798342e+08]
- [3.33692018e+08]]</t>
+          <t>[[4.18779358e+07]
+ [1.86133631e+08]
+ [3.59731319e+08]
+ [4.14774259e+08]
+ [4.10697900e+08]
+ [4.06618781e+08]
+ [4.02537064e+08]
+ [3.98452914e+08]
+ [3.94366498e+08]
+ [3.86186578e+08]
+ [3.77999477e+08]
+ [3.69806660e+08]
+ [3.61609680e+08]
+ [3.53408726e+08]
+ [3.45203500e+08]
+ [3.41100119e+08]
+ [3.36996011e+08]
+ [3.32891265e+08]]</t>
         </is>
       </c>
       <c r="E280" t="inlineStr"/>
@@ -7225,24 +7227,24 @@
       </c>
       <c r="D281" t="inlineStr">
         <is>
-          <t>[[ 214069.90260215]
- [ 467905.66188862]
- [ 808663.37487048]
- [1299618.86705817]
- [1299616.14571376]
- [1299613.41855259]
- [1299591.46407197]
- [1299588.79319843]
- [1299586.10139144]
- [1299580.91306006]
- [1299575.39564019]
- [1299569.69526414]
- [1299567.63171611]
- [1299562.46088873]
- [1299558.28223587]
- [1299565.29142155]
- [1299563.2020827 ]
- [1299561.11275055]]</t>
+          <t>[[ 214095.02179044]
+ [ 467945.83690614]
+ [ 808693.87510854]
+ [1299614.03903596]
+ [1299611.20883329]
+ [1299608.37181529]
+ [1299605.52107169]
+ [1299602.64952416]
+ [1299599.74983575]
+ [1299596.81431136]
+ [1299590.79794144]
+ [1299584.53052683]
+ [1299577.92256964]
+ [1299572.43171568]
+ [1299568.25299883]
+ [1299564.07430886]
+ [1299561.98497395]
+ [1299559.89564576]]</t>
         </is>
       </c>
       <c r="E281" t="inlineStr"/>
@@ -7294,12 +7296,12 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>[11.         11.         11.         11.         11.         11.
- 11.         11.         11.         11.         11.         11.
- 11.         11.         11.         11.         11.         11.
- 10.         10.         10.         10.         10.         10.
- 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
-  5.999     ]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494084 11.18494084 11.18494084
+ 11.18494084 11.18494085 11.18494085 11.18494085 11.18494084 11.18494084
+ 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083
+ 11.18408627 11.18408563 11.18408499 11.18408435 11.18412389 11.18416343
+ 11.18420297 10.01882791  8.85345284  7.68807778  7.12505186  6.56202594
+  5.99900001]</t>
         </is>
       </c>
       <c r="E283" t="inlineStr"/>
@@ -7322,11 +7324,11 @@
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>[0.077      0.077      0.077      0.08897847 0.08897847 0.08897847
- 0.10221371 0.10221371 0.10221371 0.10434048 0.10434048 0.10434048
- 0.10050124 0.10050124 0.10050124 0.08962371 0.08962371 0.08962371
- 0.04       0.04       0.04       0.038801   0.038801   0.038801
- 0.026301   0.026301   0.026301   0.015      0.015      0.015     ]</t>
+          <t>[0.077      0.077      0.077      0.077      0.077      0.077
+ 0.077      0.077      0.077      0.077      0.077      0.077
+ 0.077      0.077      0.077      0.077      0.077      0.077
+ 0.03457072 0.03457072 0.03457072 0.02268197 0.02268197 0.02268197
+ 0.01500039 0.01500039 0.01500039 0.015      0.015      0.015     ]</t>
         </is>
       </c>
       <c r="E284" t="inlineStr"/>
@@ -7474,11 +7476,11 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>[2.82726365 2.82726365 2.82726365 3.263503   3.263503   3.263503
- 3.74438999 3.74438999 3.74438999 3.82155405 3.82155405 3.82155405
- 3.6822358  3.6822358  3.6822358  3.28697421 3.28697421 3.28697421
- 1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
- 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
+          <t>[2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 1.29568103 1.29568096 1.29568088 0.85100867 0.85101169 0.8510147
+ 0.53381296 0.47505025 0.41628754 0.37270164 0.34431243 0.31592322]</t>
         </is>
       </c>
       <c r="E290" t="inlineStr"/>
@@ -7501,11 +7503,11 @@
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
- 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
- 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
- 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E291" t="inlineStr"/>
@@ -7528,11 +7530,11 @@
       </c>
       <c r="D292" t="inlineStr">
         <is>
-          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
- 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
- 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
- 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E292" t="inlineStr"/>
@@ -7555,11 +7557,11 @@
       </c>
       <c r="D293" t="inlineStr">
         <is>
-          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
- 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
- 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
- 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[44.34615103 44.34615101 44.34615099 44.34615098 44.34615099 44.34615101
+ 44.34615102 44.34615105 44.34615107 44.34615104 44.34615097 44.34615089
+ 44.34615085 44.34615085 44.34615084 44.34615083 44.34615082 44.34615081
+ 20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E293" t="inlineStr"/>
@@ -7582,11 +7584,11 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
- 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
- 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
- 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[44.34615103 44.34615101 44.34615099 44.34615098 44.34615099 44.34615101
+ 44.34615102 44.34615105 44.34615107 44.34615104 44.34615097 44.34615089
+ 44.34615085 44.34615085 44.34615084 44.34615083 44.34615082 44.34615081
+ 20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E294" t="inlineStr"/>
@@ -7609,12 +7611,11 @@
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>[ 84.33576062  84.33576062  84.33576062  97.1367864   97.1367864
-  97.1367864  111.18235328 111.18235328 111.18235328 113.42972734
- 113.42972734 113.42972734 109.3708483  109.3708483  109.3708483
-  97.82392145  97.82392145  97.82392145  33.21380796  33.21380796
-  33.21380796  32.22982785  32.22982785  32.22982785  19.88323673
-  16.18153341  12.97038057   5.79213059   4.36751812   3.19804084]</t>
+          <t>[88.69230205 88.69230201 88.69230197 88.69230196 88.69230199 88.69230201
+ 88.69230205 88.6923021  88.69230214 88.69230209 88.69230194 88.69230178
+ 88.6923017  88.69230169 88.69230168 88.69230166 88.69230164 88.69230162
+ 40.26746178 40.26745485 40.26744792 26.50420959 26.50449127 26.50477295
+ 14.9567086  10.54113983  7.093319    5.09068091  4.01375054  3.10053978]</t>
         </is>
       </c>
       <c r="E295" t="inlineStr"/>
@@ -7637,36 +7638,36 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>[[-3.61233470e+07]
- [-3.39607908e+07]
- [-3.14216919e+07]
- [-3.08798497e+07]
- [-3.03368469e+07]
- [-2.97915093e+07]
- [-2.91813292e+07]
- [-2.85663641e+07]
- [-2.79453063e+07]
- [-2.66588125e+07]
- [-2.53296474e+07]
- [-2.39426102e+07]
- [-2.27808618e+07]
- [-2.18420221e+07]
- [-2.09031825e+07]
- [-2.04841515e+07]
- [-2.00651205e+07]
- [-1.96460895e+07]
- [-1.74269003e+07]
- [-1.61860231e+07]
- [-1.49446247e+07]
- [-1.32233993e+07]
- [-1.15016608e+07]
- [-9.77942261e+06]
- [-9.09862410e+06]
- [-8.46264681e+06]
- [-7.87173034e+06]
- [-7.57979326e+06]
- [-7.31395379e+06]
- [ 4.36557457e-10]]</t>
+          <t>[[-3.16227224e+07]
+ [-2.94235512e+07]
+ [-2.68354818e+07]
+ [-2.63390219e+07]
+ [-2.58413644e+07]
+ [-2.53412971e+07]
+ [-2.48375781e+07]
+ [-2.43289205e+07]
+ [-2.38139743e+07]
+ [-2.27585826e+07]
+ [-2.16591423e+07]
+ [-2.04999519e+07]
+ [-1.95367185e+07]
+ [-1.88036615e+07]
+ [-1.80706044e+07]
+ [-1.77040759e+07]
+ [-1.73375474e+07]
+ [-1.69710189e+07]
+ [-1.47917950e+07]
+ [-1.35906139e+07]
+ [-1.23888590e+07]
+ [-1.12580065e+07]
+ [-1.01265820e+07]
+ [-8.99459917e+06]
+ [-8.56617195e+06]
+ [-8.18436560e+06]
+ [-7.84957314e+06]
+ [-7.56981280e+06]
+ [-7.31141845e+06]
+ [-7.58154783e-09]]</t>
         </is>
       </c>
       <c r="E296" t="inlineStr"/>
@@ -7689,36 +7690,36 @@
       </c>
       <c r="D297" t="inlineStr">
         <is>
-          <t>[[-3.57138685e+06]
- [-8.98099977e+06]
- [-9.16012717e+06]
- [ 2.42809383e+06]
- [ 2.42811353e+06]
- [ 2.42813357e+06]
- [ 2.42817756e+06]
- [ 2.42819807e+06]
- [ 2.42821930e+06]
- [ 2.42858830e+06]
- [ 2.42868472e+06]
- [ 2.42879347e+06]
- [ 2.42877271e+06]
- [ 2.42862009e+06]
- [ 2.42867077e+06]
- [ 2.42827583e+06]
- [ 2.42828803e+06]
- [ 2.42830009e+06]
- [ 2.42942913e+06]
- [ 2.43011791e+06]
- [ 2.43073661e+06]
- [ 2.43274959e+06]
- [ 2.43367362e+06]
- [ 2.43439828e+06]
- [ 2.43070100e+06]
- [ 2.43067999e+06]
- [ 2.43061537e+06]
- [ 2.42932413e+06]
- [ 2.42922801e+06]
- [ 1.14939088e+03]]</t>
+          <t>[[-3.57914475e+06]
+ [-8.86369605e+06]
+ [-8.94558558e+06]
+ [ 2.42807517e+06]
+ [ 2.42809491e+06]
+ [ 2.42811500e+06]
+ [ 2.42813559e+06]
+ [ 2.42815683e+06]
+ [ 2.42817891e+06]
+ [ 2.42850136e+06]
+ [ 2.42860388e+06]
+ [ 2.42872135e+06]
+ [ 2.42871729e+06]
+ [ 2.42853264e+06]
+ [ 2.42858132e+06]
+ [ 2.42827134e+06]
+ [ 2.42828309e+06]
+ [ 2.42829470e+06]
+ [ 2.42945481e+06]
+ [ 2.43000472e+06]
+ [ 2.43049789e+06]
+ [ 2.43099496e+06]
+ [ 2.43173321e+06]
+ [ 2.43231322e+06]
+ [ 2.42976153e+06]
+ [ 2.42970272e+06]
+ [ 2.42960981e+06]
+ [ 2.42941768e+06]
+ [ 2.42933487e+06]
+ [ 1.26767025e+03]]</t>
         </is>
       </c>
       <c r="E297" t="inlineStr"/>
@@ -7741,36 +7742,36 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>[[-4.66127963e+04]
- [-1.17471936e+05]
- [-1.20846423e+05]
- [ 2.90969215e+04]
- [ 2.90971790e+04]
- [ 2.90974409e+04]
- [ 2.90980156e+04]
- [ 2.90982842e+04]
- [ 2.90985623e+04]
- [ 2.91033773e+04]
- [ 2.91046427e+04]
- [ 2.91060712e+04]
- [ 2.91058090e+04]
- [ 2.91038216e+04]
- [ 2.91044932e+04]
- [ 2.90993237e+04]
- [ 2.90994860e+04]
- [ 2.90996465e+04]
- [ 2.91145355e+04]
- [ 2.91238056e+04]
- [ 2.91322314e+04]
- [ 2.91595534e+04]
- [ 2.91726762e+04]
- [ 2.91834001e+04]
- [ 2.91331718e+04]
- [ 2.91333875e+04]
- [ 2.91331398e+04]
- [ 2.91153261e+04]
- [ 2.91149474e+04]
- [ 1.84960460e+01]]</t>
+          <t>[[-4.67240427e+04]
+ [-1.15969305e+05]
+ [-1.18073975e+05]
+ [ 2.90966785e+04]
+ [ 2.90969365e+04]
+ [ 2.90971992e+04]
+ [ 2.90974687e+04]
+ [ 2.90977469e+04]
+ [ 2.90980362e+04]
+ [ 2.91022448e+04]
+ [ 2.91035905e+04]
+ [ 2.91051339e+04]
+ [ 2.91050904e+04]
+ [ 2.91026822e+04]
+ [ 2.91033276e+04]
+ [ 2.90992684e+04]
+ [ 2.90994247e+04]
+ [ 2.90995793e+04]
+ [ 2.91148676e+04]
+ [ 2.91222707e+04]
+ [ 2.91289893e+04]
+ [ 2.91359452e+04]
+ [ 2.91464345e+04]
+ [ 2.91550214e+04]
+ [ 2.91202875e+04]
+ [ 2.91198997e+04]
+ [ 2.91192047e+04]
+ [ 2.91172208e+04]
+ [ 2.91170805e+04]
+ [ 2.08141035e+01]]</t>
         </is>
       </c>
       <c r="E298" t="inlineStr"/>
@@ -7793,36 +7794,36 @@
       </c>
       <c r="D299" t="inlineStr">
         <is>
-          <t>[[-5.26598777e+05]
- [-2.40607156e+06]
- [-4.71519835e+06]
- [-5.43134918e+06]
- [-5.38239525e+06]
- [-5.33340277e+06]
- [-5.28437798e+06]
- [-5.23532560e+06]
- [-5.18624767e+06]
- [-5.08801102e+06]
- [-4.98969900e+06]
- [-4.89132947e+06]
- [-4.79291850e+06]
- [-4.69446588e+06]
- [-4.59596973e+06]
- [-4.54671512e+06]
- [-4.49744951e+06]
- [-4.44817413e+06]
- [-4.08976416e+06]
- [-3.72869453e+06]
- [-3.36567846e+06]
- [-2.84455227e+06]
- [-2.32217436e+06]
- [-1.80001961e+06]
- [-1.48754428e+06]
- [-1.17506364e+06]
- [-8.62644874e+05]
- [-5.70954763e+05]
- [-2.78858769e+05]
- [-4.93283089e-04]]</t>
+          <t>[[-5.44552943e+05]
+ [-2.42481409e+06]
+ [-4.69953150e+06]
+ [-5.42096781e+06]
+ [-5.37208876e+06]
+ [-5.32317355e+06]
+ [-5.27422428e+06]
+ [-5.22524309e+06]
+ [-5.17623211e+06]
+ [-5.07811694e+06]
+ [-4.97990693e+06]
+ [-4.88162109e+06]
+ [-4.78327959e+06]
+ [-4.68488482e+06]
+ [-4.58643275e+06]
+ [-4.53719613e+06]
+ [-4.48794962e+06]
+ [-4.43869438e+06]
+ [-4.08100170e+06]
+ [-3.72160224e+06]
+ [-3.36103700e+06]
+ [-2.84374694e+06]
+ [-2.32427264e+06]
+ [-1.80394003e+06]
+ [-1.49179125e+06]
+ [-1.17907316e+06]
+ [-8.65661239e+05]
+ [-5.72511996e+05]
+ [-2.78903600e+05]
+ [-5.66030564e-04]]</t>
         </is>
       </c>
       <c r="E299" t="inlineStr"/>
@@ -7845,36 +7846,36 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>[[ 4.05032729e+07]
- [ 1.84726748e+08]
- [ 3.60998049e+08]
- [ 4.15644529e+08]
- [ 4.11562418e+08]
- [ 4.07477361e+08]
- [ 4.03389850e+08]
- [ 3.99300236e+08]
- [ 3.95208680e+08]
- [ 3.87019429e+08]
- [ 3.78824481e+08]
- [ 3.70625212e+08]
- [ 3.62422859e+08]
- [ 3.54217416e+08]
- [ 3.46008748e+08]
- [ 3.41903950e+08]
- [ 3.37798342e+08]
- [ 3.33692018e+08]
- [ 3.03837180e+08]
- [ 2.73785524e+08]
- [ 2.43592339e+08]
- [ 2.00279949e+08]
- [ 1.56888351e+08]
- [ 1.13528454e+08]
- [ 8.75813616e+07]
- [ 6.16446447e+07]
- [ 3.57262528e+07]
- [ 1.15515326e+07]
- [-1.26120054e+07]
- [ 3.06533657e-02]]</t>
+          <t>[[ 4.18779358e+07]
+ [ 1.86133631e+08]
+ [ 3.59731319e+08]
+ [ 4.14774259e+08]
+ [ 4.10697900e+08]
+ [ 4.06618781e+08]
+ [ 4.02537064e+08]
+ [ 3.98452914e+08]
+ [ 3.94366498e+08]
+ [ 3.86186578e+08]
+ [ 3.77999477e+08]
+ [ 3.69806660e+08]
+ [ 3.61609680e+08]
+ [ 3.53408726e+08]
+ [ 3.45203500e+08]
+ [ 3.41100119e+08]
+ [ 3.36996011e+08]
+ [ 3.32891265e+08]
+ [ 3.03090744e+08]
+ [ 2.73164272e+08]
+ [ 2.43153633e+08]
+ [ 2.00125854e+08]
+ [ 1.56950158e+08]
+ [ 1.13727415e+08]
+ [ 8.78078642e+07]
+ [ 6.18617188e+07]
+ [ 3.58887414e+07]
+ [ 1.16339571e+07]
+ [-1.26097207e+07]
+ [ 3.44734881e-02]]</t>
         </is>
       </c>
       <c r="E300" t="inlineStr"/>
@@ -7897,35 +7898,35 @@
       </c>
       <c r="D301" t="inlineStr">
         <is>
-          <t>[[ 214069.90260215]
- [ 467905.66188862]
- [ 808663.37487048]
- [1299618.86705817]
- [1299616.14571376]
- [1299613.41855259]
- [1299591.46407197]
- [1299588.79319843]
- [1299586.10139144]
- [1299580.91306006]
- [1299575.39564019]
- [1299569.69526414]
- [1299567.63171611]
- [1299562.46088873]
- [1299558.28223587]
- [1299565.29142155]
- [1299563.2020827 ]
- [1299561.11275055]
- [1299689.5032564 ]
- [1299674.34321372]
- [1299659.155116  ]
- [1299649.59058574]
- [1299627.87565582]
- [1299606.15497853]
- [1299648.86747394]
- [1299648.21346755]
- [1299648.45194692]
- [1299792.67972821]
- [1299811.89339675]
+          <t>[[ 214095.02179044]
+ [ 467945.83690614]
+ [ 808693.87510854]
+ [1299614.03903596]
+ [1299611.20883329]
+ [1299608.37181529]
+ [1299605.52107169]
+ [1299602.64952416]
+ [1299599.74983575]
+ [1299596.81431136]
+ [1299590.79794144]
+ [1299584.53052683]
+ [1299577.92256964]
+ [1299572.43171568]
+ [1299568.25299883]
+ [1299564.07430886]
+ [1299561.98497395]
+ [1299559.89564576]
+ [1299663.33780421]
+ [1299648.17452241]
+ [1299632.97884294]
+ [1299699.67202724]
+ [1299677.88842193]
+ [1299656.0946966 ]
+ [1299737.24294329]
+ [1299756.6273149 ]
+ [1299783.32119212]
+ [1299806.28924198]
+ [1299821.43910611]
  [      0.        ]]</t>
         </is>
       </c>
@@ -8071,7 +8072,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>[11.]</t>
+          <t>[11.18494085]</t>
         </is>
       </c>
       <c r="E306" t="inlineStr"/>
@@ -8623,7 +8624,7 @@
       </c>
       <c r="D330" t="inlineStr">
         <is>
-          <t>[3187423.76365581]</t>
+          <t>[2634279.06642127]</t>
         </is>
       </c>
       <c r="E330" t="inlineStr"/>
@@ -8646,7 +8647,7 @@
       </c>
       <c r="D331" t="inlineStr">
         <is>
-          <t>[1175518.62964259]</t>
+          <t>[902219.78162679]</t>
         </is>
       </c>
       <c r="E331" t="inlineStr"/>
@@ -8669,7 +8670,7 @@
       </c>
       <c r="D332" t="inlineStr">
         <is>
-          <t>[4132423.76365581]</t>
+          <t>[3579279.06642127]</t>
         </is>
       </c>
       <c r="E332" t="inlineStr"/>
@@ -8692,7 +8693,7 @@
       </c>
       <c r="D333" t="inlineStr">
         <is>
-          <t>[275.49491758]</t>
+          <t>[238.61860443]</t>
         </is>
       </c>
       <c r="E333" t="inlineStr"/>
@@ -8715,7 +8716,7 @@
       </c>
       <c r="D334" t="inlineStr">
         <is>
-          <t>[1175518.62964259]</t>
+          <t>[902219.78162679]</t>
         </is>
       </c>
       <c r="E334" t="inlineStr"/>
@@ -8784,7 +8785,7 @@
       </c>
       <c r="D337" t="inlineStr">
         <is>
-          <t>[3187423.76365581]</t>
+          <t>[2634279.06642127]</t>
         </is>
       </c>
       <c r="E337" t="inlineStr"/>
@@ -8807,7 +8808,7 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>[3187423.76365581]</t>
+          <t>[2634279.06642127]</t>
         </is>
       </c>
       <c r="E338" t="inlineStr"/>
@@ -8830,9 +8831,9 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
- 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
- 427.60678303 391.57616974 352.18249915]</t>
+          <t>[376.8637364  433.4947406  472.91020584 503.8274884  539.45978844
+ 568.76856759 593.87710694 546.37921754 494.76103473 438.15146599
+ 411.93099011 383.31695362 352.18250007]</t>
         </is>
       </c>
       <c r="E339" t="inlineStr"/>
@@ -9047,9 +9048,9 @@
       </c>
       <c r="D348" t="inlineStr">
         <is>
-          <t>[10.         10.         10.         10.         10.         10.
- 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
-  5.999     ]</t>
+          <t>[11.18408627 11.18408563 11.18408499 11.18408435 11.18412389 11.18416343
+ 11.18420297 10.01882791  8.85345284  7.68807778  7.12505186  6.56202594
+  5.99900001]</t>
         </is>
       </c>
       <c r="E348" t="inlineStr"/>
@@ -9143,9 +9144,9 @@
       </c>
       <c r="D352" t="inlineStr">
         <is>
-          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
- 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
- 427.60678303 391.57616974 352.18249915]</t>
+          <t>[376.8637364  433.4947406  472.91020584 503.8274884  539.45978844
+ 568.76856759 593.87710694 546.37921754 494.76103473 438.15146599
+ 411.93099011 383.31695362 352.18250007]</t>
         </is>
       </c>
       <c r="E352" t="inlineStr"/>
@@ -9285,9 +9286,9 @@
       </c>
       <c r="D358" t="inlineStr">
         <is>
-          <t>[-336.9560439  -388.43785582 -424.16473764 -452.12457083 -484.27449749
- -510.65946695 -533.22010636 -511.58791739 -487.37587695 -460.61782438
- -427.60678303 -391.57616974 -352.18249915]</t>
+          <t>[-376.8637364  -433.4947406  -472.91020584 -503.8274884  -539.45978844
+ -568.76856759 -593.87710694 -546.37921754 -494.76103473 -438.15146599
+ -411.93099011 -383.31695362 -352.18250007]</t>
         </is>
       </c>
       <c r="E358" t="inlineStr"/>
@@ -9335,7 +9336,7 @@
       </c>
       <c r="D360" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
+          <t>[11.18408627 11.18408435 11.18420297  7.68807778  5.99900001]</t>
         </is>
       </c>
       <c r="E360" t="inlineStr"/>
@@ -9358,7 +9359,7 @@
       </c>
       <c r="D361" t="inlineStr">
         <is>
-          <t>[0.04     0.038801 0.026301 0.015   ]</t>
+          <t>[0.03457072 0.02268197 0.01500039 0.015     ]</t>
         </is>
       </c>
       <c r="E361" t="inlineStr"/>
@@ -9423,7 +9424,7 @@
       </c>
       <c r="D364" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
+          <t>[11.18408627 11.18408435 11.18420297  7.68807778  5.99900001]</t>
         </is>
       </c>
       <c r="E364" t="inlineStr"/>
@@ -9446,7 +9447,7 @@
       </c>
       <c r="D365" t="inlineStr">
         <is>
-          <t>[0.04     0.038801 0.026301 0.015   ]</t>
+          <t>[0.03457072 0.02268197 0.01500039 0.015     ]</t>
         </is>
       </c>
       <c r="E365" t="inlineStr"/>
@@ -9682,8 +9683,8 @@
       </c>
       <c r="D375" t="inlineStr">
         <is>
-          <t>[0.04     0.04     0.04     0.038801 0.038801 0.038801 0.026301 0.026301
- 0.026301 0.015    0.015    0.015   ]</t>
+          <t>[0.03457072 0.03457072 0.03457072 0.02268197 0.02268197 0.02268197
+ 0.01500039 0.01500039 0.01500039 0.015      0.015      0.015     ]</t>
         </is>
       </c>
       <c r="E375" t="inlineStr"/>
@@ -9866,8 +9867,8 @@
       </c>
       <c r="D383" t="inlineStr">
         <is>
-          <t>[1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
- 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
+          <t>[1.29568103 1.29568096 1.29568088 0.85100867 0.85101169 0.8510147
+ 0.53381296 0.47505025 0.41628754 0.37270164 0.34431243 0.31592322]</t>
         </is>
       </c>
       <c r="E383" t="inlineStr"/>
@@ -9890,8 +9891,8 @@
       </c>
       <c r="D384" t="inlineStr">
         <is>
-          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E384" t="inlineStr"/>
@@ -9914,8 +9915,8 @@
       </c>
       <c r="D385" t="inlineStr">
         <is>
-          <t>[0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E385" t="inlineStr"/>
@@ -9938,8 +9939,8 @@
       </c>
       <c r="D386" t="inlineStr">
         <is>
-          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E386" t="inlineStr"/>
@@ -9962,8 +9963,8 @@
       </c>
       <c r="D387" t="inlineStr">
         <is>
-          <t>[16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E387" t="inlineStr"/>
@@ -9986,8 +9987,8 @@
       </c>
       <c r="D388" t="inlineStr">
         <is>
-          <t>[33.21380796 33.21380796 33.21380796 32.22982785 32.22982785 32.22982785
- 19.88323673 16.18153341 12.97038057  5.79213059  4.36751812  3.19804084]</t>
+          <t>[40.26746178 40.26745485 40.26744792 26.50420959 26.50449127 26.50477295
+ 14.9567086  10.54113983  7.093319    5.09068091  4.01375054  3.10053978]</t>
         </is>
       </c>
       <c r="E388" t="inlineStr"/>
@@ -10081,18 +10082,18 @@
       </c>
       <c r="D392" t="inlineStr">
         <is>
-          <t>[[-17427765.12991663]
- [-16186366.78221211]
- [-14944587.88685458]
- [-13222849.37497341]
- [-11500611.20008019]
- [ -9777955.21838797]
- [ -9097151.95187112]
- [ -8461409.45930777]
- [ -7870754.04360263]
- [ -7579102.67267725]
- [ -7313593.23878349]
- [ -7074256.2758736 ]]</t>
+          <t>[[-14792255.83552192]
+ [-13590500.82297246]
+ [-12388325.66650094]
+ [-11256905.09900315]
+ [-10124926.22133705]
+ [ -8992478.8642256 ]
+ [ -8564166.31211518]
+ [ -8182867.61212859]
+ [ -7848629.45633108]
+ [ -7569265.06488163]
+ [ -7311132.84144737]
+ [ -7074256.27587361]]</t>
         </is>
       </c>
       <c r="E392" t="inlineStr"/>
@@ -10115,18 +10116,18 @@
       </c>
       <c r="D393" t="inlineStr">
         <is>
-          <t>[[2428340.58969823]
- [2429076.44059267]
- [2429745.66121794]
- [2431464.41489253]
- [2432495.54674606]
- [2433328.43446587]
- [2430320.56243432]
- [2430367.54182217]
- [2430375.83291243]
- [2429248.39987909]
- [2429220.83731715]
- [2429127.58409672]]</t>
+          <t>[[2428261.36452721]
+ [2428847.83671197]
+ [2429381.3576488 ]
+ [2430006.64208273]
+ [2430830.85797564]
+ [2431497.62005671]
+ [2429486.64446499]
+ [2429493.9935887 ]
+ [2429475.38137672]
+ [2429362.02541039]
+ [2429351.56714398]
+ [2429270.62753694]]</t>
         </is>
       </c>
       <c r="E393" t="inlineStr"/>
@@ -10149,18 +10150,18 @@
       </c>
       <c r="D394" t="inlineStr">
         <is>
-          <t>[[29100.21334624]
- [29110.04393666]
- [29119.07546929]
- [29142.38007936]
- [29156.79240186]
- [29168.82090949]
- [29127.92088216]
- [29128.99893601]
- [29129.67529452]
- [29114.12772248]
- [29114.60165251]
- [29114.41196808]]</t>
+          <t>[[29099.16256356]
+ [29107.00041827]
+ [29114.20359966]
+ [29122.78334809]
+ [29134.30955576]
+ [29143.94400109]
+ [29116.50270212]
+ [29116.96096466]
+ [29117.21398107]
+ [29116.24266725]
+ [29117.00381968]
+ [29117.0256052 ]]</t>
         </is>
       </c>
       <c r="E394" t="inlineStr"/>
@@ -10183,18 +10184,18 @@
       </c>
       <c r="D395" t="inlineStr">
         <is>
-          <t>[[-4355770.84979259]
- [-3999369.51509918]
- [-3640497.12021613]
- [-3124519.02847233]
- [-2606354.23982125]
- [-2087563.38387338]
- [-1776650.06345185]
- [-1465466.49623692]
- [-1154071.36764904]
- [ -862996.74568595]
- [ -571078.64832484]
- [ -278501.90073832]]</t>
+          <t>[[-4349162.19795935]
+ [-3994304.57722576]
+ [-3637778.32576996]
+ [-3125468.08331412]
+ [-2610163.11866413]
+ [-2093257.2023268 ]
+ [-1782753.9142576 ]
+ [-1471388.57583626]
+ [-1158966.77594137]
+ [ -866330.09195273]
+ [ -572753.36209753]
+ [ -278501.9279941 ]]</t>
         </is>
       </c>
       <c r="E395" t="inlineStr"/>
@@ -10217,17 +10218,17 @@
       </c>
       <c r="D396" t="inlineStr">
         <is>
-          <t>[[ 3.26042330e+08]
- [ 2.96343964e+08]
- [ 2.66462894e+08]
- [ 2.23535771e+08]
- [ 1.80456648e+08]
- [ 1.37343596e+08]
- [ 1.11509659e+08]
- [ 8.56652885e+07]
- [ 5.98176693e+07]
- [ 3.56818040e+07]
- [ 1.15214098e+07]
+          <t>[[ 3.25427454e+08]
+ [ 2.95845075e+08]
+ [ 2.66139437e+08]
+ [ 2.23485592e+08]
+ [ 1.80620176e+08]
+ [ 1.37649721e+08]
+ [ 1.11849668e+08]
+ [ 8.59996099e+07]
+ [ 6.00934716e+07]
+ [ 3.58676780e+07]
+ [ 1.16138057e+07]
  [-1.26341969e+07]]</t>
         </is>
       </c>
@@ -10251,18 +10252,18 @@
       </c>
       <c r="D397" t="inlineStr">
         <is>
-          <t>[[1299689.54225215]
- [1299674.3537992 ]
- [1299659.15932317]
- [1299649.59012126]
- [1299627.86871814]
- [1299606.14173766]
- [1299648.83929164]
- [1299648.18318422]
- [1299648.4245459 ]
- [1299792.63859019]
- [1299811.86142551]
- [1299836.63664036]]</t>
+          <t>[[1299663.37640344]
+ [1299648.18035189]
+ [1299632.97741208]
+ [1299699.66175321]
+ [1299677.86720602]
+ [1299656.06280409]
+ [1299737.17782783]
+ [1299756.55809997]
+ [1299783.26219625]
+ [1299806.24772884]
+ [1299821.41302364]
+ [1299840.40625841]]</t>
         </is>
       </c>
       <c r="E397" t="inlineStr"/>
@@ -10436,19 +10437,19 @@
       </c>
       <c r="D403" t="inlineStr">
         <is>
-          <t>[[-336.9560439 ]
- [-388.43785582]
- [-424.16473764]
- [-452.12457083]
- [-484.27449749]
- [-510.65946695]
- [-533.22010636]
- [-511.58791739]
- [-487.37587695]
- [-460.61782438]
- [-427.60678303]
- [-391.57616974]
- [-352.18249915]]</t>
+          <t>[[-376.8637364 ]
+ [-433.4947406 ]
+ [-472.91020584]
+ [-503.8274884 ]
+ [-539.45978844]
+ [-568.76856759]
+ [-593.87710694]
+ [-546.37921754]
+ [-494.76103473]
+ [-438.15146599]
+ [-411.93099011]
+ [-383.31695362]
+ [-352.18250007]]</t>
         </is>
       </c>
       <c r="E403" t="inlineStr"/>
@@ -10471,7 +10472,7 @@
       </c>
       <c r="D404" t="inlineStr">
         <is>
-          <t>[1175518.62964259]</t>
+          <t>[902219.78162679]</t>
         </is>
       </c>
       <c r="E404" t="inlineStr"/>
@@ -10494,7 +10495,7 @@
       </c>
       <c r="D405" t="inlineStr">
         <is>
-          <t>[59.4435992]</t>
+          <t>[55.50197793]</t>
         </is>
       </c>
       <c r="E405" t="inlineStr"/>
@@ -10517,7 +10518,7 @@
       </c>
       <c r="D406" t="inlineStr">
         <is>
-          <t>[5.79150755e+09 5.79150755e+09 2.73584130e+07 0.00000000e+00
+          <t>[4.16983530e+09 4.16983530e+09 2.56305263e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -10572,10 +10573,10 @@
       </c>
       <c r="D408" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          76069.22818689
-  76419.81487525  77475.80310771  79250.00595527  81764.21915156
-  85049.92502601  89149.36708317 100022.09247963 115010.75107985
- 135096.15327474      0.              0.              0.
+          <t>[     0.              0.              0.          78565.31757154
+  78927.1602561   80017.05386019  81848.22904544  84443.19581949
+  87834.4763627   92065.72326944 103288.62402897 118761.87556321
+ 139500.77063907      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -10826,10 +10827,10 @@
       </c>
       <c r="D418" t="inlineStr">
         <is>
-          <t>[     0.              0.              0.          76069.22818689
-  76419.81487525  77475.80310771  79250.00595527  81764.21915156
-  85049.92502601  89149.36708317 100022.09247963 115010.75107985
- 135096.15327474      0.              0.              0.
+          <t>[     0.              0.              0.          78565.31757154
+  78927.1602561   80017.05386019  81848.22904544  84443.19581949
+  87834.4763627   92065.72326944 103288.62402897 118761.87556321
+ 139500.77063907      0.              0.              0.
       0.              0.              0.        ]</t>
         </is>
       </c>
@@ -11211,10 +11212,10 @@
       </c>
       <c r="D434" t="inlineStr">
         <is>
-          <t>[      0.               0.               0.          -76069.22818689
-  -76419.81487525  -77475.80310771  -79250.00595527  -81764.21915156
-  -85049.92502601  -89149.36708317 -100022.09247963 -115010.75107985
- -135096.15327474       0.               0.               0.
+          <t>[      0.               0.               0.          -78565.31757154
+  -78927.1602561   -80017.05386019  -81848.22904544  -84443.19581949
+  -87834.4763627   -92065.72326944 -103288.62402897 -118761.87556321
+ -139500.77063907       0.               0.               0.
        0.               0.               0.        ]</t>
         </is>
       </c>
@@ -11261,8 +11262,8 @@
       <c r="C436" t="inlineStr"/>
       <c r="D436" t="inlineStr">
         <is>
-          <t>[142.85714286 123.62540609 107.61766064 105.42408783 109.45138599
- 122.73537912]</t>
+          <t>[145.25897199 145.25897198 145.25897204 145.25897195 145.25897182
+ 145.25897179]</t>
         </is>
       </c>
       <c r="E436" t="inlineStr"/>
@@ -11319,7 +11320,7 @@
       <c r="C439" t="inlineStr"/>
       <c r="D439" t="inlineStr">
         <is>
-          <t>[1.1555646  1.14874645 1.02080713 0.96320469 0.89176721]</t>
+          <t>[1. 1. 1. 1. 1.]</t>
         </is>
       </c>
       <c r="E439" t="inlineStr"/>
@@ -11363,8 +11364,10 @@
       </c>
       <c r="D441" t="inlineStr">
         <is>
-          <t>[5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5 5.5
- 5.5]</t>
+          <t>[5.59247042 5.59247042 5.59247042 5.59247042 5.59247042 5.59247042
+ 5.59247042 5.59247042 5.59247042 5.59247042 5.59247042 5.59247042
+ 5.59247042 5.59247042 5.59247041 5.59247041 5.59247041 5.59247041
+ 5.59247041]</t>
         </is>
       </c>
       <c r="E441" t="inlineStr"/>
@@ -11410,7 +11413,7 @@
       </c>
       <c r="D443" t="inlineStr">
         <is>
-          <t>[4751.65888855]</t>
+          <t>[4912.77945995]</t>
         </is>
       </c>
       <c r="E443" t="inlineStr"/>
@@ -11433,7 +11436,7 @@
       </c>
       <c r="D444" t="inlineStr">
         <is>
-          <t>[47761243.48631421]</t>
+          <t>[49380745.01655622]</t>
         </is>
       </c>
       <c r="E444" t="inlineStr"/>
@@ -11475,7 +11478,7 @@
       </c>
       <c r="D446" t="inlineStr">
         <is>
-          <t>[95.03317777]</t>
+          <t>[98.25558898]</t>
         </is>
       </c>
       <c r="E446" t="inlineStr"/>
@@ -11498,7 +11501,7 @@
       </c>
       <c r="D447" t="inlineStr">
         <is>
-          <t>[718.68840689]</t>
+          <t>[768.25370371]</t>
         </is>
       </c>
       <c r="E447" t="inlineStr"/>
@@ -11521,7 +11524,7 @@
       </c>
       <c r="D448" t="inlineStr">
         <is>
-          <t>[718.68840689]</t>
+          <t>[768.25370371]</t>
         </is>
       </c>
       <c r="E448" t="inlineStr"/>
@@ -11544,8 +11547,8 @@
       </c>
       <c r="D449" t="inlineStr">
         <is>
-          <t>[4.87045036e+06 4.87045036e+06 2.27379167e+05 1.01472840e+09
- 1.01472840e+09 0.00000000e+00]</t>
+          <t>[5.03559895e+06 5.03559895e+06 2.39041712e+05 1.04913610e+09
+ 1.04913610e+09 0.00000000e+00]</t>
         </is>
       </c>
       <c r="E449" t="inlineStr"/>
@@ -11617,8 +11620,10 @@
       </c>
       <c r="D452" t="inlineStr">
         <is>
-          <t>[11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11.
- 11.]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494084 11.18494084 11.18494084
+ 11.18494084 11.18494085 11.18494085 11.18494085 11.18494084 11.18494084
+ 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083
+ 11.18494083]</t>
         </is>
       </c>
       <c r="E452" t="inlineStr"/>
@@ -11872,8 +11877,8 @@
       </c>
       <c r="D463" t="inlineStr">
         <is>
-          <t>[22052.65645424 25455.32343855 29206.24191018 29808.12162885
- 28721.4392631  25638.39882899]</t>
+          <t>[22426.03710819 22426.03710633 22426.03711527 22426.03710191
+ 22426.03708127 22426.03707681]</t>
         </is>
       </c>
       <c r="E463" t="inlineStr">
@@ -11900,8 +11905,8 @@
       </c>
       <c r="D464" t="inlineStr">
         <is>
-          <t>[328909.46641626 378833.46697552 433611.1778083  442375.93663105
- 426546.30836535 381513.2936722 ]</t>
+          <t>[345899.97784072 345899.97775639 345899.97817177 345899.97755249
+ 345899.97659803 345899.97639289]</t>
         </is>
       </c>
       <c r="E464" t="inlineStr">
@@ -11928,8 +11933,8 @@
       </c>
       <c r="D465" t="inlineStr">
         <is>
-          <t>[328909.46641626 378833.46697552 433611.1778083  442375.93663105
- 426546.30836535 381513.2936722 ]</t>
+          <t>[345899.97784072 345899.97775639 345899.97817177 345899.97755249
+ 345899.97659803 345899.97639289]</t>
         </is>
       </c>
       <c r="E465" t="inlineStr">
@@ -11956,8 +11961,8 @@
       </c>
       <c r="D466" t="inlineStr">
         <is>
-          <t>[7.88184679e+12 9.07820434e+12 1.03908741e+13 1.06009091e+13
- 1.02215746e+13 9.14242257e+12]</t>
+          <t>[8.28900019e+12 8.28900019e+12 8.28900020e+12 8.28900018e+12
+ 8.28900016e+12 8.28900015e+12]</t>
         </is>
       </c>
       <c r="E466" t="inlineStr">
@@ -11984,8 +11989,8 @@
       </c>
       <c r="D467" t="inlineStr">
         <is>
-          <t>[7.88184679e+12 9.07820434e+12 1.03908741e+13 1.06009091e+13
- 1.02215746e+13 9.14242257e+12]</t>
+          <t>[8.28900019e+12 8.28900019e+12 8.28900020e+12 8.28900018e+12
+ 8.28900016e+12 8.28900015e+12]</t>
         </is>
       </c>
       <c r="E467" t="inlineStr">
@@ -12012,8 +12017,8 @@
       </c>
       <c r="D468" t="inlineStr">
         <is>
-          <t>[6.25030450e+12 7.19901604e+12 8.23996319e+12 8.40652091e+12
- 8.10570866e+12 7.24994109e+12]</t>
+          <t>[6.57317715e+12 6.57317715e+12 6.57317716e+12 6.57317714e+12
+ 6.57317713e+12 6.57317712e+12]</t>
         </is>
       </c>
       <c r="E468" t="inlineStr">
@@ -12040,8 +12045,8 @@
       </c>
       <c r="D469" t="inlineStr">
         <is>
-          <t>[5.28460495e+11 6.10000562e+11 6.99885979e+11 7.14309169e+11
- 6.88268374e+11 6.14387703e+11]</t>
+          <t>[5.37408030e+11 5.37408030e+11 5.37408031e+11 5.37408030e+11
+ 5.37408030e+11 5.37408030e+11]</t>
         </is>
       </c>
       <c r="E469" t="inlineStr">
@@ -12149,12 +12154,12 @@
       </c>
       <c r="D473" t="inlineStr">
         <is>
-          <t>[[0.         0.         0.37845781 0.1395612  0.1395612  0.        ]
- [0.         0.         0.32786855 0.12116934 0.12116934 0.        ]
- [0.         0.         0.28576083 0.10586212 0.10586212 0.        ]
- [0.         0.         0.27999081 0.10376469 0.10376469 0.        ]
- [0.         0.         0.29058432 0.10761551 0.10761551 0.        ]
- [0.         0.         0.32552735 0.12031822 0.12031822 0.        ]]</t>
+          <t>[[0.         0.         0.3721567  0.13493715 0.13493715 0.        ]
+ [0.         0.         0.3721567  0.13493715 0.13493715 0.        ]
+ [0.         0.         0.3721567  0.13493715 0.13493715 0.        ]
+ [0.         0.         0.3721567  0.13493715 0.13493715 0.        ]
+ [0.         0.         0.3721567  0.13493715 0.13493715 0.        ]
+ [0.         0.         0.3721567  0.13493715 0.13493715 0.        ]]</t>
         </is>
       </c>
       <c r="E473" t="inlineStr"/>
@@ -12177,12 +12182,12 @@
       </c>
       <c r="D474" t="inlineStr">
         <is>
-          <t>[[0.62132644 0.62132644 0.         0.         0.         0.0697806 ]
- [0.53799878 0.53799878 0.         0.         0.         0.06058467]
- [0.4686384  0.4686384  0.         0.         0.         0.05293106]
- [0.45913365 0.45913365 0.         0.         0.         0.05188234]
- [0.4765839  0.4765839  0.         0.         0.         0.05380776]
- [0.53414241 0.53414241 0.         0.         0.         0.06015911]]</t>
+          <t>[[0.61101457 0.61101457 0.         0.         0.         0.06746858]
+ [0.61101457 0.61101457 0.         0.         0.         0.06746858]
+ [0.61101457 0.61101457 0.         0.         0.         0.06746858]
+ [0.61101457 0.61101457 0.         0.         0.         0.06746858]
+ [0.61101457 0.61101457 0.         0.         0.         0.06746858]
+ [0.61101457 0.61101457 0.         0.         0.         0.06746858]]</t>
         </is>
       </c>
       <c r="E474" t="inlineStr"/>
@@ -12205,7 +12210,7 @@
       </c>
       <c r="D475" t="inlineStr">
         <is>
-          <t>[1184.91130973]</t>
+          <t>[1127.0058174]</t>
         </is>
       </c>
       <c r="E475" t="inlineStr"/>
@@ -12228,7 +12233,7 @@
       </c>
       <c r="D476" t="inlineStr">
         <is>
-          <t>[3980261.24221089]</t>
+          <t>[3565596.39650365]</t>
         </is>
       </c>
       <c r="E476" t="inlineStr"/>
@@ -12251,7 +12256,7 @@
       </c>
       <c r="D477" t="inlineStr">
         <is>
-          <t>[1648375.1234354]</t>
+          <t>[1457692.41156949]</t>
         </is>
       </c>
       <c r="E477" t="inlineStr"/>
@@ -12274,7 +12279,7 @@
       </c>
       <c r="D478" t="inlineStr">
         <is>
-          <t>[34.4331827]</t>
+          <t>[32.49999999]</t>
         </is>
       </c>
       <c r="E478" t="inlineStr"/>
@@ -12297,7 +12302,7 @@
       </c>
       <c r="D479" t="inlineStr">
         <is>
-          <t>[2.54169442e+09 2.54169442e+09 4.90525923e+07 0.00000000e+00
+          <t>[2.07540031e+09 2.07540031e+09 4.49669971e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -12321,7 +12326,9 @@
       </c>
       <c r="D480" t="inlineStr">
         <is>
-          <t>[11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11. 11.]</t>
+          <t>[11.18494084 11.18494084 11.18494084 11.18494084 11.18494084 11.18494084
+ 11.18494084 11.18494085 11.18494085 11.18494085 11.18494084 11.18494083
+ 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083]</t>
         </is>
       </c>
       <c r="E480" t="inlineStr"/>
@@ -12344,9 +12351,8 @@
       </c>
       <c r="D481" t="inlineStr">
         <is>
-          <t>[0.08239    0.08239    0.08239    0.09520697 0.09520697 0.09520697
- 0.10936867 0.10936867 0.10936867 0.11164431 0.11164431 0.11164431
- 0.10753633 0.10753633 0.10753633 0.09589737 0.09589737 0.09589737]</t>
+          <t>[0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239
+ 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239 0.08239]</t>
         </is>
       </c>
       <c r="E481" t="inlineStr"/>
@@ -12394,7 +12400,7 @@
       </c>
       <c r="D483" t="inlineStr">
         <is>
-          <t>[1748375.1234354]</t>
+          <t>[1557692.41156949]</t>
         </is>
       </c>
       <c r="E483" t="inlineStr"/>
@@ -12417,7 +12423,7 @@
       </c>
       <c r="D484" t="inlineStr">
         <is>
-          <t>[4480261.24221089]</t>
+          <t>[4065596.39650365]</t>
         </is>
       </c>
       <c r="E484" t="inlineStr"/>
@@ -12440,7 +12446,7 @@
       </c>
       <c r="D485" t="inlineStr">
         <is>
-          <t>[36.18148127]</t>
+          <t>[34.58641961]</t>
         </is>
       </c>
       <c r="E485" t="inlineStr"/>
@@ -12463,7 +12469,7 @@
       </c>
       <c r="D486" t="inlineStr">
         <is>
-          <t>[2.96570692e+09 2.96570692e+09 5.20775923e+07 0.00000000e+00
+          <t>[2.49946410e+09 2.49946410e+09 4.80945696e+07 0.00000000e+00
  0.00000000e+00 0.00000000e+00]</t>
         </is>
       </c>
@@ -12487,7 +12493,7 @@
       </c>
       <c r="D487" t="inlineStr">
         <is>
-          <t>[2923893.75307798]</t>
+          <t>[2459912.19319628]</t>
         </is>
       </c>
       <c r="E487" t="inlineStr"/>
@@ -12510,7 +12516,7 @@
       </c>
       <c r="D488" t="inlineStr">
         <is>
-          <t>[7667685.0058667]</t>
+          <t>[6699875.46292491]</t>
         </is>
       </c>
       <c r="E488" t="inlineStr"/>
@@ -12560,7 +12566,7 @@
       </c>
       <c r="D490" t="inlineStr">
         <is>
-          <t>[0.21999755]</t>
+          <t>[0.21998844]</t>
         </is>
       </c>
       <c r="E490" t="inlineStr"/>
@@ -12583,7 +12589,7 @@
       </c>
       <c r="D491" t="inlineStr">
         <is>
-          <t>[0.22134505]</t>
+          <t>[0.2216603]</t>
         </is>
       </c>
       <c r="E491" t="inlineStr"/>
@@ -12606,7 +12612,7 @@
       </c>
       <c r="D492" t="inlineStr">
         <is>
-          <t>[0.21999755 0.22134505 0.92117535 1.01638648 1.15669516 2.0485555 ]</t>
+          <t>[0.21998844 0.2216603  0.84261382 0.96692084 1.11887862 2.14129927]</t>
         </is>
       </c>
       <c r="E492" t="inlineStr"/>
@@ -12629,7 +12635,7 @@
       </c>
       <c r="D493" t="inlineStr">
         <is>
-          <t>[0.22134505 1.15669516 2.16529265]</t>
+          <t>[0.2216603  1.11887862 2.22759097]</t>
         </is>
       </c>
       <c r="E493" t="inlineStr"/>
@@ -12652,7 +12658,7 @@
       </c>
       <c r="D494" t="inlineStr">
         <is>
-          <t>[0.21999755 1.01638648 2.0485555 ]</t>
+          <t>[0.21998844 0.96692084 2.14129927]</t>
         </is>
       </c>
       <c r="E494" t="inlineStr"/>
@@ -12675,7 +12681,7 @@
       </c>
       <c r="D495" t="inlineStr">
         <is>
-          <t>[4.49500558 0.         0.        ]</t>
+          <t>[4.18050453 0.         0.        ]</t>
         </is>
       </c>
       <c r="E495" t="inlineStr"/>
@@ -12694,9 +12700,9 @@
       <c r="C496" t="inlineStr"/>
       <c r="D496" t="inlineStr">
         <is>
-          <t>[[ 0.55427077  0.5457551   2.07469104 -4.02909738  1.85438047]
- [-2.46956588 -0.10350813  6.57977706 -6.90431     3.89760695]
- [-4.7733934   4.65370807  9.71866059 -1.375797   -7.22317826]]</t>
+          <t>[[ 0.61009339  0.66628588  0.06879366 -0.66361217  0.31843925]
+ [-2.6889188  -0.55816236  6.18956061 -6.48576756  4.54328811]
+ [-5.21591345  2.50018118 15.4976308  -5.7306484  -6.05125012]]</t>
         </is>
       </c>
       <c r="E496" t="inlineStr"/>
@@ -12715,9 +12721,9 @@
       <c r="C497" t="inlineStr"/>
       <c r="D497" t="inlineStr">
         <is>
-          <t>[[ 0.54901338  0.54222202  2.08831205 -4.05198517  1.87243771]
- [-2.49204522 -0.43200223  7.21681417 -8.90689773  5.61413101]
- [-4.28862793  3.69929876  8.14639839 -0.02219398 -6.53487523]]</t>
+          <t>[[ 0.60333886  0.66210024  0.08454193 -0.69131156  0.34133053]
+ [-2.80839674 -0.82512583  6.69793959 -8.44112441  6.37670739]
+ [-4.80834343  2.0407609  13.38266184 -3.9445848  -5.67049451]]</t>
         </is>
       </c>
       <c r="E497" t="inlineStr"/>
@@ -12736,7 +12742,7 @@
       <c r="C498" t="inlineStr"/>
       <c r="D498" t="inlineStr">
         <is>
-          <t>[[ -0.37046014   8.78814819 -22.55378557  24.22299285  -9.08689533]
+          <t>[[  0.18945177   4.02422028 -12.6538915   17.93748206  -8.49726261]
  [  0.           0.           0.           0.           0.        ]
  [  0.           0.           0.           0.           0.        ]]</t>
         </is>
@@ -12757,9 +12763,9 @@
       <c r="C499" t="inlineStr"/>
       <c r="D499" t="inlineStr">
         <is>
-          <t>[[ 1.26998237  0.90469816 -3.80129328  4.14778648 -1.52117373]
- [-1.38300795  5.21937195 -8.02311143  6.90137788 -1.71463045]
- [ 0.13856119  4.05804497 -5.24306741  6.15051553 -4.10405427]]</t>
+          <t>[[  0.80627152   1.91533583  -5.10413751   5.41742883  -2.03489867]
+ [ -1.64646127   7.46457636 -16.11073435  16.87903088  -5.58641162]
+ [  0.23497298   1.27282728   2.21858705  -1.53060708  -1.19578023]]</t>
         </is>
       </c>
       <c r="E499" t="inlineStr"/>
@@ -12778,9 +12784,12 @@
       <c r="C500" t="inlineStr"/>
       <c r="D500" t="inlineStr">
         <is>
-          <t>[[ 1.25695893  0.92266435 -3.81647118  4.14850008 -1.51165218]
- [-1.5459125   5.31553908 -8.04385047  6.47682499 -1.2026011 ]
- [-0.12934916  4.35351419 -6.0359276   6.94963259 -4.13787003]]</t>
+          <t>[[ 7.90204683e-01  1.95478763e+00 -5.18966416e+00  5.50041780e+00
+  -2.05574596e+00]
+ [-1.85578955e+00  8.09782203e+00 -1.77599537e+01  1.83330744e+01
+  -5.81515318e+00]
+ [ 1.78293469e-02  1.95849793e+00  1.16229059e-01  8.06227135e-01
+  -1.89878347e+00]]</t>
         </is>
       </c>
       <c r="E500" t="inlineStr"/>
@@ -12799,7 +12808,7 @@
       <c r="C501" t="inlineStr"/>
       <c r="D501" t="inlineStr">
         <is>
-          <t>[[ -24.52354263  191.15304427 -535.87123688  615.41382219 -245.17208694]
+          <t>[[  -6.20124416   49.81463092 -132.01629333  149.32794296  -59.92503638]
  [   0.            0.            0.            0.            0.        ]
  [   0.            0.            0.            0.            0.        ]]</t>
         </is>
@@ -12824,37 +12833,37 @@
       </c>
       <c r="D502" t="inlineStr">
         <is>
-          <t>[[1.58283357e-04]
- [3.31093003e-04]
- [1.77440549e-05]
- [2.97887336e-03]
- [4.01191585e-03]
- [5.16384957e-03]
- [6.43350597e-03]
- [7.80880180e-03]
- [9.28490152e-03]
- [1.08607824e-02]
- [1.43029322e-02]
- [1.81242559e-02]
- [2.23167179e-02]
- [2.68807713e-02]
- [3.18130653e-02]
- [3.71052640e-02]
- [3.98918630e-02]
- [4.27755621e-02]
- [4.57551948e-02]
- [7.50776058e-02]
- [1.17733957e-01]
- [1.72405073e-01]
- [2.69056055e-01]
- [3.84190550e-01]
- [5.13803785e-01]
- [5.98169622e-01]
- [6.87785919e-01]
- [7.81970594e-01]
- [8.74468209e-01]
- [9.69054622e-01]
- [1.06164387e+00]]</t>
+          <t>[[1.58168727e-04]
+ [3.22149188e-04]
+ [8.07768945e-06]
+ [2.87537899e-03]
+ [3.87754832e-03]
+ [5.00965548e-03]
+ [6.27042243e-03]
+ [7.65857028e-03]
+ [9.17281932e-03]
+ [1.08118890e-02]
+ [1.44593725e-02]
+ [1.85907559e-02]
+ [2.31957710e-02]
+ [2.82641415e-02]
+ [3.37855964e-02]
+ [3.97498632e-02]
+ [4.28948323e-02]
+ [4.61466465e-02]
+ [4.95040197e-02]
+ [8.03255836e-02]
+ [1.22118050e-01]
+ [1.73797846e-01]
+ [2.67398087e-01]
+ [3.83458372e-01]
+ [5.17132378e-01]
+ [6.05814081e-01]
+ [7.02103389e-01]
+ [8.06162686e-01]
+ [9.09122846e-01]
+ [1.01442194e+00]
+ [1.11763651e+00]]</t>
         </is>
       </c>
       <c r="E502" t="inlineStr"/>
@@ -12877,7 +12886,7 @@
       </c>
       <c r="D503" t="inlineStr">
         <is>
-          <t>[1.06164387]</t>
+          <t>[1.11763651]</t>
         </is>
       </c>
       <c r="E503" t="inlineStr"/>
@@ -12900,24 +12909,24 @@
       </c>
       <c r="D504" t="inlineStr">
         <is>
-          <t>[[-36123346.97588959]
- [-33960790.79041462]
- [-31421691.94796431]
- [-30879849.66133218]
- [-30336846.93487328]
- [-29791509.30376027]
- [-29181329.17357343]
- [-28566364.10790942]
- [-27945306.30131707]
- [-26658812.50241386]
- [-25329647.43537711]
- [-23942610.16605137]
- [-22780861.82640503]
- [-21842022.14135061]
- [-20903182.45629581]
- [-20484151.47503773]
- [-20065120.49377933]
- [-19646089.51252162]]</t>
+          <t>[[-31622722.37489413]
+ [-29423551.23121068]
+ [-26835481.76696547]
+ [-26339021.94528637]
+ [-25841364.44276518]
+ [-25341297.06371611]
+ [-24837578.11870414]
+ [-24328920.51751414]
+ [-23813974.32813288]
+ [-22758582.61770878]
+ [-21659142.25010826]
+ [-20499951.85134015]
+ [-19536718.54349031]
+ [-18803661.49559565]
+ [-18070604.44770125]
+ [-17704075.92375403]
+ [-17337547.39980648]
+ [-16971018.87585953]]</t>
         </is>
       </c>
       <c r="E504" t="inlineStr"/>
@@ -12940,24 +12949,24 @@
       </c>
       <c r="D505" t="inlineStr">
         <is>
-          <t>[[-3571386.85080247]
- [-8980999.77048393]
- [-9160127.16752138]
- [ 2428093.82801644]
- [ 2428113.53256131]
- [ 2428133.56642783]
- [ 2428177.55584712]
- [ 2428198.07321296]
- [ 2428219.29887818]
- [ 2428588.30264015]
- [ 2428684.72498103]
- [ 2428793.4671491 ]
- [ 2428772.71401341]
- [ 2428620.0939148 ]
- [ 2428670.77338876]
- [ 2428275.82942879]
- [ 2428288.03473593]
- [ 2428300.09340087]]</t>
+          <t>[[-3579144.75489268]
+ [-8863696.04876918]
+ [-8945585.5771961 ]
+ [ 2428075.16753127]
+ [ 2428094.90884762]
+ [ 2428114.99911463]
+ [ 2428135.58832508]
+ [ 2428156.83499969]
+ [ 2428178.90975678]
+ [ 2428501.35821275]
+ [ 2428603.88146218]
+ [ 2428721.3472541 ]
+ [ 2428717.29176938]
+ [ 2428532.63752758]
+ [ 2428581.32421195]
+ [ 2428271.34463096]
+ [ 2428283.09213585]
+ [ 2428294.6982198 ]]</t>
         </is>
       </c>
       <c r="E505" t="inlineStr"/>
@@ -12980,24 +12989,24 @@
       </c>
       <c r="D506" t="inlineStr">
         <is>
-          <t>[[ -46612.79626053]
- [-117471.93621095]
- [-120846.42288106]
- [  29096.92151658]
- [  29097.17898185]
- [  29097.44093214]
- [  29098.01559855]
- [  29098.28422904]
- [  29098.56230757]
- [  29103.37730347]
- [  29104.64273106]
- [  29106.07123526]
- [  29105.80901867]
- [  29103.82156847]
- [  29104.49322739]
- [  29099.32366656]
- [  29099.48597565]
- [  29099.64652502]]</t>
+          <t>[[ -46724.04266973]
+ [-115969.30452781]
+ [-118073.97522221]
+ [  29096.67851973]
+ [  29096.93651114]
+ [  29097.19924445]
+ [  29097.46868375]
+ [  29097.74690746]
+ [  29098.03615519]
+ [  29102.2448058 ]
+ [  29103.59050806]
+ [  29105.13386418]
+ [  29105.09037856]
+ [  29102.68221936]
+ [  29103.3276242 ]
+ [  29099.26843232]
+ [  29099.42469379]
+ [  29099.57925817]]</t>
         </is>
       </c>
       <c r="E506" t="inlineStr"/>
@@ -13020,24 +13029,24 @@
       </c>
       <c r="D507" t="inlineStr">
         <is>
-          <t>[[ -526598.7774628 ]
- [-2406071.56195532]
- [-4715198.34905789]
- [-5431349.17696918]
- [-5382395.25464339]
- [-5333402.76688932]
- [-5284377.98404438]
- [-5235325.59908948]
- [-5186247.67118431]
- [-5088011.01723978]
- [-4989699.00157361]
- [-4891329.46663574]
- [-4792918.5016765 ]
- [-4694465.88006755]
- [-4595969.73165049]
- [-4546715.11585086]
- [-4497449.51364613]
- [-4448174.12628585]]</t>
+          <t>[[ -544552.94323635]
+ [-2424814.09229682]
+ [-4699531.50475682]
+ [-5420967.81261888]
+ [-5372088.75750023]
+ [-5323173.54503663]
+ [-5274224.28235081]
+ [-5225243.09037663]
+ [-5176232.11270024]
+ [-5078116.93615036]
+ [-4979906.92994198]
+ [-4881621.09241059]
+ [-4783279.59214913]
+ [-4684884.82166152]
+ [-4586432.75056777]
+ [-4537196.13107404]
+ [-4487949.6235716 ]
+ [-4438694.38206342]]</t>
         </is>
       </c>
       <c r="E507" t="inlineStr"/>
@@ -13060,24 +13069,24 @@
       </c>
       <c r="D508" t="inlineStr">
         <is>
-          <t>[[4.05032729e+07]
- [1.84726748e+08]
- [3.60998049e+08]
- [4.15644529e+08]
- [4.11562418e+08]
- [4.07477361e+08]
- [4.03389850e+08]
- [3.99300236e+08]
- [3.95208680e+08]
- [3.87019429e+08]
- [3.78824481e+08]
- [3.70625212e+08]
- [3.62422859e+08]
- [3.54217416e+08]
- [3.46008748e+08]
- [3.41903950e+08]
- [3.37798342e+08]
- [3.33692018e+08]]</t>
+          <t>[[4.18779358e+07]
+ [1.86133631e+08]
+ [3.59731319e+08]
+ [4.14774259e+08]
+ [4.10697900e+08]
+ [4.06618781e+08]
+ [4.02537064e+08]
+ [3.98452914e+08]
+ [3.94366498e+08]
+ [3.86186578e+08]
+ [3.77999477e+08]
+ [3.69806660e+08]
+ [3.61609680e+08]
+ [3.53408726e+08]
+ [3.45203500e+08]
+ [3.41100119e+08]
+ [3.36996011e+08]
+ [3.32891265e+08]]</t>
         </is>
       </c>
       <c r="E508" t="inlineStr"/>
@@ -13100,24 +13109,24 @@
       </c>
       <c r="D509" t="inlineStr">
         <is>
-          <t>[[ 214069.90260215]
- [ 467905.66188862]
- [ 808663.37487048]
- [1299618.86705817]
- [1299616.14571376]
- [1299613.41855259]
- [1299591.46407197]
- [1299588.79319843]
- [1299586.10139144]
- [1299580.91306006]
- [1299575.39564019]
- [1299569.69526414]
- [1299567.63171611]
- [1299562.46088873]
- [1299558.28223587]
- [1299565.29142155]
- [1299563.2020827 ]
- [1299561.11275055]]</t>
+          <t>[[ 214095.02179044]
+ [ 467945.83690614]
+ [ 808693.87510854]
+ [1299614.03903596]
+ [1299611.20883329]
+ [1299608.37181529]
+ [1299605.52107169]
+ [1299602.64952416]
+ [1299599.74983575]
+ [1299596.81431136]
+ [1299590.79794144]
+ [1299584.53052683]
+ [1299577.92256964]
+ [1299572.43171568]
+ [1299568.25299883]
+ [1299564.07430886]
+ [1299561.98497395]
+ [1299559.89564576]]</t>
         </is>
       </c>
       <c r="E509" t="inlineStr"/>
@@ -13140,9 +13149,9 @@
       </c>
       <c r="D510" t="inlineStr">
         <is>
-          <t>[[ 2.42809383e+06]
- [ 2.90969215e+04]
- [-3.14216919e+07]]</t>
+          <t>[[  2428075.16753127]
+ [    29096.67851973]
+ [-26835481.76696553]]</t>
         </is>
       </c>
       <c r="E510" t="inlineStr"/>
@@ -13165,9 +13174,9 @@
       </c>
       <c r="D511" t="inlineStr">
         <is>
-          <t>[[-5.48026241e+06]
- [ 4.19723529e+08]
- [ 1.29961887e+06]]</t>
+          <t>[[-5.46980861e+06]
+ [ 4.18847693e+08]
+ [ 1.29961404e+06]]</t>
         </is>
       </c>
       <c r="E511" t="inlineStr"/>
@@ -13219,12 +13228,12 @@
       </c>
       <c r="D513" t="inlineStr">
         <is>
-          <t>[11.         11.         11.         11.         11.         11.
- 11.         11.         11.         11.         11.         11.
- 11.         11.         11.         11.         11.         11.
- 10.         10.         10.         10.         10.         10.
- 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
-  5.999     ]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494084 11.18494084 11.18494084
+ 11.18494084 11.18494085 11.18494085 11.18494085 11.18494084 11.18494084
+ 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083 11.18494083
+ 11.18408627 11.18408563 11.18408499 11.18408435 11.18412389 11.18416343
+ 11.18420297 10.01882791  8.85345284  7.68807778  7.12505186  6.56202594
+  5.99900001]</t>
         </is>
       </c>
       <c r="E513" t="inlineStr"/>
@@ -13247,11 +13256,11 @@
       </c>
       <c r="D514" t="inlineStr">
         <is>
-          <t>[0.077      0.077      0.077      0.08897847 0.08897847 0.08897847
- 0.10221371 0.10221371 0.10221371 0.10434048 0.10434048 0.10434048
- 0.10050124 0.10050124 0.10050124 0.08962371 0.08962371 0.08962371
- 0.04       0.04       0.04       0.038801   0.038801   0.038801
- 0.026301   0.026301   0.026301   0.015      0.015      0.015     ]</t>
+          <t>[0.077      0.077      0.077      0.077      0.077      0.077
+ 0.077      0.077      0.077      0.077      0.077      0.077
+ 0.077      0.077      0.077      0.077      0.077      0.077
+ 0.03457072 0.03457072 0.03457072 0.02268197 0.02268197 0.02268197
+ 0.01500039 0.01500039 0.01500039 0.015      0.015      0.015     ]</t>
         </is>
       </c>
       <c r="E514" t="inlineStr"/>
@@ -13350,11 +13359,11 @@
       </c>
       <c r="D518" t="inlineStr">
         <is>
-          <t>[2.82726365 2.82726365 2.82726365 3.263503   3.263503   3.263503
- 3.74438999 3.74438999 3.74438999 3.82155405 3.82155405 3.82155405
- 3.6822358  3.6822358  3.6822358  3.28697421 3.28697421 3.28697421
- 1.33922325 1.33922325 1.33922325 1.29923633 1.29923633 1.29923633
- 0.85346398 0.79682429 0.74018461 0.3890889  0.35414478 0.31920067]</t>
+          <t>[2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296 2.87513296
+ 1.29568103 1.29568096 1.29568088 0.85100867 0.85101169 0.8510147
+ 0.53381296 0.47505025 0.41628754 0.37270164 0.34431243 0.31592322]</t>
         </is>
       </c>
       <c r="E518" t="inlineStr"/>
@@ -13377,11 +13386,11 @@
       </c>
       <c r="D519" t="inlineStr">
         <is>
-          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
- 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
- 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
- 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E519" t="inlineStr"/>
@@ -13404,11 +13413,11 @@
       </c>
       <c r="D520" t="inlineStr">
         <is>
-          <t>[1.60945991 1.60945991 1.60945991 1.85874026 1.85874026 1.85874026
- 2.13384134 2.13384134 2.13384134 2.17801504 2.17801504 2.17801504
- 2.09826642 2.09826642 2.09826642 1.8721599  1.8721599  1.8721599
- 0.76132308 0.76132308 0.76132308 0.73855119 0.73855119 0.73855119
- 0.48489791 0.452757   0.42061614 0.2209853  0.20115569 0.1813261 ]</t>
+          <t>[1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219 1.63662219
+ 0.73626823 0.73626818 0.73626814 0.48335423 0.48335594 0.48335765
+ 0.30311155 0.26976558 0.23641964 0.21168607 0.19557616 0.17946626]</t>
         </is>
       </c>
       <c r="E520" t="inlineStr"/>
@@ -13431,12 +13440,11 @@
       </c>
       <c r="D521" t="inlineStr">
         <is>
-          <t>[ 84.33576062  84.33576062  84.33576062  97.1367864   97.1367864
-  97.1367864  111.18235328 111.18235328 111.18235328 113.42972734
- 113.42972734 113.42972734 109.3708483  109.3708483  109.3708483
-  97.82392145  97.82392145  97.82392145  33.21380796  33.21380796
-  33.21380796  32.22982785  32.22982785  32.22982785  19.88323673
-  16.18153341  12.97038057   5.79213059   4.36751812   3.19804084]</t>
+          <t>[88.69230205 88.69230201 88.69230197 88.69230196 88.69230199 88.69230201
+ 88.69230205 88.6923021  88.69230214 88.69230209 88.69230194 88.69230178
+ 88.6923017  88.69230169 88.69230168 88.69230166 88.69230164 88.69230162
+ 40.26746178 40.26745485 40.26744792 26.50420959 26.50449127 26.50477295
+ 14.9567086  10.54113983  7.093319    5.09068091  4.01375054  3.10053978]</t>
         </is>
       </c>
       <c r="E521" t="inlineStr"/>
@@ -13459,11 +13467,11 @@
       </c>
       <c r="D522" t="inlineStr">
         <is>
-          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
- 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
- 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
- 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[44.34615103 44.34615101 44.34615099 44.34615098 44.34615099 44.34615101
+ 44.34615102 44.34615105 44.34615107 44.34615104 44.34615097 44.34615089
+ 44.34615085 44.34615085 44.34615084 44.34615083 44.34615082 44.34615081
+ 20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E522" t="inlineStr"/>
@@ -13486,11 +13494,11 @@
       </c>
       <c r="D523" t="inlineStr">
         <is>
-          <t>[42.16788031 42.16788031 42.16788031 48.5683932  48.5683932  48.5683932
- 55.59117664 55.59117664 55.59117664 56.71486367 56.71486367 56.71486367
- 54.68542415 54.68542415 54.68542415 48.91196073 48.91196073 48.91196073
- 16.60690398 16.60690398 16.60690398 16.11491392 16.11491392 16.11491392
-  9.94161836  8.0907667   6.48519028  2.8960653   2.18375906  1.59902042]</t>
+          <t>[44.34615103 44.34615101 44.34615099 44.34615098 44.34615099 44.34615101
+ 44.34615102 44.34615105 44.34615107 44.34615104 44.34615097 44.34615089
+ 44.34615085 44.34615085 44.34615084 44.34615083 44.34615082 44.34615081
+ 20.13373089 20.13372743 20.13372396 13.25210479 13.25224563 13.25238648
+  7.4783543   5.27056992  3.5466595   2.54534046  2.00687527  1.55026989]</t>
         </is>
       </c>
       <c r="E523" t="inlineStr"/>
@@ -13615,36 +13623,36 @@
       </c>
       <c r="D527" t="inlineStr">
         <is>
-          <t>[[-3.61233470e+07]
- [-3.39607908e+07]
- [-3.14216919e+07]
- [-3.08798497e+07]
- [-3.03368469e+07]
- [-2.97915093e+07]
- [-2.91813292e+07]
- [-2.85663641e+07]
- [-2.79453063e+07]
- [-2.66588125e+07]
- [-2.53296474e+07]
- [-2.39426102e+07]
- [-2.27808618e+07]
- [-2.18420221e+07]
- [-2.09031825e+07]
- [-2.04841515e+07]
- [-2.00651205e+07]
- [-1.96460895e+07]
- [-1.74269003e+07]
- [-1.61860231e+07]
- [-1.49446247e+07]
- [-1.32233993e+07]
- [-1.15016608e+07]
- [-9.77942261e+06]
- [-9.09862410e+06]
- [-8.46264681e+06]
- [-7.87173034e+06]
- [-7.57979326e+06]
- [-7.31395379e+06]
- [ 4.36557457e-10]]</t>
+          <t>[[-3.16227224e+07]
+ [-2.94235512e+07]
+ [-2.68354818e+07]
+ [-2.63390219e+07]
+ [-2.58413644e+07]
+ [-2.53412971e+07]
+ [-2.48375781e+07]
+ [-2.43289205e+07]
+ [-2.38139743e+07]
+ [-2.27585826e+07]
+ [-2.16591423e+07]
+ [-2.04999519e+07]
+ [-1.95367185e+07]
+ [-1.88036615e+07]
+ [-1.80706044e+07]
+ [-1.77040759e+07]
+ [-1.73375474e+07]
+ [-1.69710189e+07]
+ [-1.47917950e+07]
+ [-1.35906139e+07]
+ [-1.23888590e+07]
+ [-1.12580065e+07]
+ [-1.01265820e+07]
+ [-8.99459917e+06]
+ [-8.56617195e+06]
+ [-8.18436560e+06]
+ [-7.84957314e+06]
+ [-7.56981280e+06]
+ [-7.31141845e+06]
+ [-7.58154783e-09]]</t>
         </is>
       </c>
       <c r="E527" t="inlineStr"/>
@@ -13667,36 +13675,36 @@
       </c>
       <c r="D528" t="inlineStr">
         <is>
-          <t>[[-3.57138685e+06]
- [-8.98099977e+06]
- [-9.16012717e+06]
- [ 2.42809383e+06]
- [ 2.42811353e+06]
- [ 2.42813357e+06]
- [ 2.42817756e+06]
- [ 2.42819807e+06]
- [ 2.42821930e+06]
- [ 2.42858830e+06]
- [ 2.42868472e+06]
- [ 2.42879347e+06]
- [ 2.42877271e+06]
- [ 2.42862009e+06]
- [ 2.42867077e+06]
- [ 2.42827583e+06]
- [ 2.42828803e+06]
- [ 2.42830009e+06]
- [ 2.42942913e+06]
- [ 2.43011791e+06]
- [ 2.43073661e+06]
- [ 2.43274959e+06]
- [ 2.43367362e+06]
- [ 2.43439828e+06]
- [ 2.43070100e+06]
- [ 2.43067999e+06]
- [ 2.43061537e+06]
- [ 2.42932413e+06]
- [ 2.42922801e+06]
- [ 1.14939088e+03]]</t>
+          <t>[[-3.57914475e+06]
+ [-8.86369605e+06]
+ [-8.94558558e+06]
+ [ 2.42807517e+06]
+ [ 2.42809491e+06]
+ [ 2.42811500e+06]
+ [ 2.42813559e+06]
+ [ 2.42815683e+06]
+ [ 2.42817891e+06]
+ [ 2.42850136e+06]
+ [ 2.42860388e+06]
+ [ 2.42872135e+06]
+ [ 2.42871729e+06]
+ [ 2.42853264e+06]
+ [ 2.42858132e+06]
+ [ 2.42827134e+06]
+ [ 2.42828309e+06]
+ [ 2.42829470e+06]
+ [ 2.42945481e+06]
+ [ 2.43000472e+06]
+ [ 2.43049789e+06]
+ [ 2.43099496e+06]
+ [ 2.43173321e+06]
+ [ 2.43231322e+06]
+ [ 2.42976153e+06]
+ [ 2.42970272e+06]
+ [ 2.42960981e+06]
+ [ 2.42941768e+06]
+ [ 2.42933487e+06]
+ [ 1.26767025e+03]]</t>
         </is>
       </c>
       <c r="E528" t="inlineStr"/>
@@ -13719,36 +13727,36 @@
       </c>
       <c r="D529" t="inlineStr">
         <is>
-          <t>[[-4.66127963e+04]
- [-1.17471936e+05]
- [-1.20846423e+05]
- [ 2.90969215e+04]
- [ 2.90971790e+04]
- [ 2.90974409e+04]
- [ 2.90980156e+04]
- [ 2.90982842e+04]
- [ 2.90985623e+04]
- [ 2.91033773e+04]
- [ 2.91046427e+04]
- [ 2.91060712e+04]
- [ 2.91058090e+04]
- [ 2.91038216e+04]
- [ 2.91044932e+04]
- [ 2.90993237e+04]
- [ 2.90994860e+04]
- [ 2.90996465e+04]
- [ 2.91145355e+04]
- [ 2.91238056e+04]
- [ 2.91322314e+04]
- [ 2.91595534e+04]
- [ 2.91726762e+04]
- [ 2.91834001e+04]
- [ 2.91331718e+04]
- [ 2.91333875e+04]
- [ 2.91331398e+04]
- [ 2.91153261e+04]
- [ 2.91149474e+04]
- [ 1.84960460e+01]]</t>
+          <t>[[-4.67240427e+04]
+ [-1.15969305e+05]
+ [-1.18073975e+05]
+ [ 2.90966785e+04]
+ [ 2.90969365e+04]
+ [ 2.90971992e+04]
+ [ 2.90974687e+04]
+ [ 2.90977469e+04]
+ [ 2.90980362e+04]
+ [ 2.91022448e+04]
+ [ 2.91035905e+04]
+ [ 2.91051339e+04]
+ [ 2.91050904e+04]
+ [ 2.91026822e+04]
+ [ 2.91033276e+04]
+ [ 2.90992684e+04]
+ [ 2.90994247e+04]
+ [ 2.90995793e+04]
+ [ 2.91148676e+04]
+ [ 2.91222707e+04]
+ [ 2.91289893e+04]
+ [ 2.91359452e+04]
+ [ 2.91464345e+04]
+ [ 2.91550214e+04]
+ [ 2.91202875e+04]
+ [ 2.91198997e+04]
+ [ 2.91192047e+04]
+ [ 2.91172208e+04]
+ [ 2.91170805e+04]
+ [ 2.08141035e+01]]</t>
         </is>
       </c>
       <c r="E529" t="inlineStr"/>
@@ -13771,36 +13779,36 @@
       </c>
       <c r="D530" t="inlineStr">
         <is>
-          <t>[[-5.26598777e+05]
- [-2.40607156e+06]
- [-4.71519835e+06]
- [-5.43134918e+06]
- [-5.38239525e+06]
- [-5.33340277e+06]
- [-5.28437798e+06]
- [-5.23532560e+06]
- [-5.18624767e+06]
- [-5.08801102e+06]
- [-4.98969900e+06]
- [-4.89132947e+06]
- [-4.79291850e+06]
- [-4.69446588e+06]
- [-4.59596973e+06]
- [-4.54671512e+06]
- [-4.49744951e+06]
- [-4.44817413e+06]
- [-4.08976416e+06]
- [-3.72869453e+06]
- [-3.36567846e+06]
- [-2.84455227e+06]
- [-2.32217436e+06]
- [-1.80001961e+06]
- [-1.48754428e+06]
- [-1.17506364e+06]
- [-8.62644874e+05]
- [-5.70954763e+05]
- [-2.78858769e+05]
- [-4.93283089e-04]]</t>
+          <t>[[-5.44552943e+05]
+ [-2.42481409e+06]
+ [-4.69953150e+06]
+ [-5.42096781e+06]
+ [-5.37208876e+06]
+ [-5.32317355e+06]
+ [-5.27422428e+06]
+ [-5.22524309e+06]
+ [-5.17623211e+06]
+ [-5.07811694e+06]
+ [-4.97990693e+06]
+ [-4.88162109e+06]
+ [-4.78327959e+06]
+ [-4.68488482e+06]
+ [-4.58643275e+06]
+ [-4.53719613e+06]
+ [-4.48794962e+06]
+ [-4.43869438e+06]
+ [-4.08100170e+06]
+ [-3.72160224e+06]
+ [-3.36103700e+06]
+ [-2.84374694e+06]
+ [-2.32427264e+06]
+ [-1.80394003e+06]
+ [-1.49179125e+06]
+ [-1.17907316e+06]
+ [-8.65661239e+05]
+ [-5.72511996e+05]
+ [-2.78903600e+05]
+ [-5.66030564e-04]]</t>
         </is>
       </c>
       <c r="E530" t="inlineStr"/>
@@ -13823,36 +13831,36 @@
       </c>
       <c r="D531" t="inlineStr">
         <is>
-          <t>[[ 4.05032729e+07]
- [ 1.84726748e+08]
- [ 3.60998049e+08]
- [ 4.15644529e+08]
- [ 4.11562418e+08]
- [ 4.07477361e+08]
- [ 4.03389850e+08]
- [ 3.99300236e+08]
- [ 3.95208680e+08]
- [ 3.87019429e+08]
- [ 3.78824481e+08]
- [ 3.70625212e+08]
- [ 3.62422859e+08]
- [ 3.54217416e+08]
- [ 3.46008748e+08]
- [ 3.41903950e+08]
- [ 3.37798342e+08]
- [ 3.33692018e+08]
- [ 3.03837180e+08]
- [ 2.73785524e+08]
- [ 2.43592339e+08]
- [ 2.00279949e+08]
- [ 1.56888351e+08]
- [ 1.13528454e+08]
- [ 8.75813616e+07]
- [ 6.16446447e+07]
- [ 3.57262528e+07]
- [ 1.15515326e+07]
- [-1.26120054e+07]
- [ 3.06533657e-02]]</t>
+          <t>[[ 4.18779358e+07]
+ [ 1.86133631e+08]
+ [ 3.59731319e+08]
+ [ 4.14774259e+08]
+ [ 4.10697900e+08]
+ [ 4.06618781e+08]
+ [ 4.02537064e+08]
+ [ 3.98452914e+08]
+ [ 3.94366498e+08]
+ [ 3.86186578e+08]
+ [ 3.77999477e+08]
+ [ 3.69806660e+08]
+ [ 3.61609680e+08]
+ [ 3.53408726e+08]
+ [ 3.45203500e+08]
+ [ 3.41100119e+08]
+ [ 3.36996011e+08]
+ [ 3.32891265e+08]
+ [ 3.03090744e+08]
+ [ 2.73164272e+08]
+ [ 2.43153633e+08]
+ [ 2.00125854e+08]
+ [ 1.56950158e+08]
+ [ 1.13727415e+08]
+ [ 8.78078642e+07]
+ [ 6.18617188e+07]
+ [ 3.58887414e+07]
+ [ 1.16339571e+07]
+ [-1.26097207e+07]
+ [ 3.44734881e-02]]</t>
         </is>
       </c>
       <c r="E531" t="inlineStr"/>
@@ -13875,35 +13883,35 @@
       </c>
       <c r="D532" t="inlineStr">
         <is>
-          <t>[[ 214069.90260215]
- [ 467905.66188862]
- [ 808663.37487048]
- [1299618.86705817]
- [1299616.14571376]
- [1299613.41855259]
- [1299591.46407197]
- [1299588.79319843]
- [1299586.10139144]
- [1299580.91306006]
- [1299575.39564019]
- [1299569.69526414]
- [1299567.63171611]
- [1299562.46088873]
- [1299558.28223587]
- [1299565.29142155]
- [1299563.2020827 ]
- [1299561.11275055]
- [1299689.5032564 ]
- [1299674.34321372]
- [1299659.155116  ]
- [1299649.59058574]
- [1299627.87565582]
- [1299606.15497853]
- [1299648.86747394]
- [1299648.21346755]
- [1299648.45194692]
- [1299792.67972821]
- [1299811.89339675]
+          <t>[[ 214095.02179044]
+ [ 467945.83690614]
+ [ 808693.87510854]
+ [1299614.03903596]
+ [1299611.20883329]
+ [1299608.37181529]
+ [1299605.52107169]
+ [1299602.64952416]
+ [1299599.74983575]
+ [1299596.81431136]
+ [1299590.79794144]
+ [1299584.53052683]
+ [1299577.92256964]
+ [1299572.43171568]
+ [1299568.25299883]
+ [1299564.07430886]
+ [1299561.98497395]
+ [1299559.89564576]
+ [1299663.33780421]
+ [1299648.17452241]
+ [1299632.97884294]
+ [1299699.67202724]
+ [1299677.88842193]
+ [1299656.0946966 ]
+ [1299737.24294329]
+ [1299756.6273149 ]
+ [1299783.32119212]
+ [1299806.28924198]
+ [1299821.43910611]
  [      0.        ]]</t>
         </is>
       </c>
@@ -13927,24 +13935,24 @@
       </c>
       <c r="D533" t="inlineStr">
         <is>
-          <t>[[-7493457.5293111 ]
- [12084249.57549396]
- [35975545.69216007]
- [37610411.33137283]
- [37314496.88095672]
- [37018964.30323167]
- [32120083.294518  ]
- [31879678.51544838]
- [31640708.7096287 ]
- [30559062.8958482 ]
- [30112097.61916249]
- [29679856.9200609 ]
- [30267262.75396389]
- [29696904.16724063]
- [29126221.1770942 ]
- [32217532.71577787]
- [31883319.16482491]
- [31549025.04878658]]</t>
+          <t>[[-5717047.58208181]
+ [13241403.30780891]
+ [36035754.83154424]
+ [43150461.68749074]
+ [42809447.77226739]
+ [42468923.8116652 ]
+ [42129342.3329161 ]
+ [41791171.77137601]
+ [41454902.62197696]
+ [40790339.36173861]
+ [40140191.0409963 ]
+ [39510103.5680188 ]
+ [38811335.15602817]
+ [38032008.07348464]
+ [37252142.15583126]
+ [36862112.35941464]
+ [36471990.8722423 ]
+ [36081788.90634568]]</t>
         </is>
       </c>
       <c r="E533" t="inlineStr"/>
@@ -13967,24 +13975,24 @@
       </c>
       <c r="D534" t="inlineStr">
         <is>
-          <t>[[2233146.75679488]
- [5611124.66811099]
- [5744661.88449172]
- [1379991.28185071]
- [1380001.72968485]
- [1380012.35438049]
- [1202307.51439414]
- [1202316.99831437]
- [1202326.81316458]
- [1178140.98071276]
- [1178184.98770823]
- [1178234.64277084]
- [1222949.25834957]
- [1222876.25591098]
- [1222900.20089956]
- [1370204.29938101]
- [1370210.70185411]
- [1370217.02599413]]</t>
+          <t>[[2200595.63067661]
+ [5445817.13979051]
+ [5517351.19414379]
+ [1565642.64963939]
+ [1565654.53427989]
+ [1565666.631724  ]
+ [1565679.03313202]
+ [1565691.83491716]
+ [1565705.14094274]
+ [1565901.99354178]
+ [1565964.26367264]
+ [1566035.64887681]
+ [1566032.75461788]
+ [1565919.57250078]
+ [1565949.05994626]
+ [1565759.37840982]
+ [1565766.42533821]
+ [1565773.38585053]]</t>
         </is>
       </c>
       <c r="E534" t="inlineStr"/>
@@ -14009,17 +14017,17 @@
         <is>
           <t>[[       -0.        ]
  [       -0.        ]
- [ -7627447.09919977]
- [-12675152.21247375]
- [-11655839.92170454]
- [-10644440.5885838 ]
- [ -8382556.02585416]
- [ -7517473.3600212 ]
- [ -6659956.66271766]
- [ -5281090.90962319]
- [ -3651879.35714917]
- [ -2062686.25009233]
- [  -664113.42747926]
+ [ -7756589.86996475]
+ [-14911301.7112367 ]
+ [-13712162.41615859]
+ [-12522332.08195711]
+ [-11342013.20746825]
+ [-10171513.54406095]
+ [ -9011251.01016109]
+ [ -7295680.16047002]
+ [ -5044969.72597852]
+ [ -2849543.66293664]
+ [  -883384.93182847]
  [       -0.        ]
  [       -0.        ]
  [       -0.        ]
@@ -14083,24 +14091,24 @@
       <c r="C537" t="inlineStr"/>
       <c r="D537" t="inlineStr">
         <is>
-          <t>[[0.04289747]
- [0.07888609]
- [0.21132756]
- [0.23075016]
- [0.22571849]
- [0.22076848]
- [0.18866726]
- [0.18459539]
- [0.18060859]
- [0.17079569]
- [0.16359171]
- [0.15683455]
- [0.15605734]
- [0.15145061]
- [0.14855509]
- [0.16433325]
- [0.16263776]
- [0.16094197]]</t>
+          <t>[[0.03495317]
+ [0.08270107]
+ [0.21155737]
+ [0.26603822]
+ [0.26013385]
+ [0.25432657]
+ [0.24862202]
+ [0.24302641]
+ [0.23754651]
+ [0.22874501]
+ [0.21859413]
+ [0.20906781]
+ [0.20019244]
+ [0.19395852]
+ [0.19000165]
+ [0.18802276]
+ [0.18604364]
+ [0.18406423]]</t>
         </is>
       </c>
       <c r="E537" t="inlineStr"/>
@@ -14119,24 +14127,24 @@
       <c r="C538" t="inlineStr"/>
       <c r="D538" t="inlineStr">
         <is>
-          <t>[[0.06517142]
- [0.08107839]
- [0.16551556]
- [0.0485888 ]
- [0.04607327]
- [0.04367489]
- [0.03339134]
- [0.03162263]
- [0.0299975 ]
- [0.03394068]
- [0.02998886]
- [0.02691042]
- [0.02650527]
- [0.02546888]
- [0.02449908]
- [0.02617813]
- [0.02569723]
- [0.02521719]]</t>
+          <t>[[0.05796322]
+ [0.07398982]
+ [0.16201668]
+ [0.05865868]
+ [0.05527596]
+ [0.05200991]
+ [0.04887638]
+ [0.04589437]
+ [0.04308624]
+ [0.05562255]
+ [0.047452  ]
+ [0.04034144]
+ [0.03470508]
+ [0.03240992]
+ [0.03133657]
+ [0.02814213]
+ [0.02763261]
+ [0.02712418]]</t>
         </is>
       </c>
       <c r="E538" t="inlineStr"/>
@@ -14155,24 +14163,24 @@
       <c r="C539" t="inlineStr"/>
       <c r="D539" t="inlineStr">
         <is>
-          <t>[[0.08447172]
- [0.16285742]
- [0.25873801]
- [0.25047413]
- [0.24764075]
- [0.24480281]
- [0.21105853]
- [0.2084927 ]
- [0.20591841]
- [0.19670041]
- [0.19154174]
- [0.18630866]
- [0.18814666]
- [0.18331159]
- [0.17847625]
- [0.19706939]
- [0.19443731]
- [0.19180519]]</t>
+          <t>[[0.08197556]
+ [0.16390511]
+ [0.26250405]
+ [0.29434501]
+ [0.29099654]
+ [0.28764246]
+ [0.28428057]
+ [0.2809086 ]
+ [0.27752415]
+ [0.27070542]
+ [0.26380308]
+ [0.25678912]
+ [0.25013708]
+ [0.24390965]
+ [0.23768118]
+ [0.23456704]
+ [0.23145283]
+ [0.22833862]]</t>
         </is>
       </c>
       <c r="E539" t="inlineStr"/>
@@ -14195,36 +14203,36 @@
       </c>
       <c r="D540" t="inlineStr">
         <is>
-          <t>[[-7.49345753e+06]
- [ 1.20842496e+07]
- [ 3.59755457e+07]
- [ 3.76104113e+07]
- [ 3.73144969e+07]
- [ 3.70189643e+07]
- [ 3.21200833e+07]
- [ 3.18796785e+07]
- [ 3.16407087e+07]
- [ 3.05590629e+07]
- [ 3.01120976e+07]
- [ 2.96798569e+07]
- [ 3.02672628e+07]
- [ 2.96969042e+07]
- [ 2.91262212e+07]
- [ 3.22175327e+07]
- [ 3.18833192e+07]
- [ 2.98432988e+07]
- [ 7.84747709e+07]
- [ 7.03527526e+07]
- [ 6.21885106e+07]
- [ 5.19696214e+07]
- [ 3.98306986e+07]
- [ 2.77020271e+07]
- [ 3.19822276e+07]
- [ 2.38206137e+07]
- [ 1.25048784e+07]
- [-4.04261505e+06]
- [-3.22409417e+05]
- [ 6.08299014e-02]]</t>
+          <t>[[-5.71704758e+06]
+ [ 1.32414033e+07]
+ [ 3.60357548e+07]
+ [ 4.31504617e+07]
+ [ 4.28094478e+07]
+ [ 4.24689238e+07]
+ [ 4.21293423e+07]
+ [ 4.17911718e+07]
+ [ 4.14549026e+07]
+ [ 4.07903394e+07]
+ [ 4.01401910e+07]
+ [ 3.95101036e+07]
+ [ 3.88113352e+07]
+ [ 3.80320081e+07]
+ [ 3.72521422e+07]
+ [ 3.68621124e+07]
+ [ 3.64719909e+07]
+ [ 3.60801850e+07]
+ [ 7.27733357e+07]
+ [ 6.53878920e+07]
+ [ 5.79795123e+07]
+ [ 7.12275443e+07]
+ [ 5.43363144e+07]
+ [ 3.74261759e+07]
+ [ 4.62012310e+07]
+ [ 3.81585574e+07]
+ [ 2.30020852e+07]
+ [-3.36361946e+06]
+ [ 2.70290644e+05]
+ [ 6.98395483e-02]]</t>
         </is>
       </c>
       <c r="E540" t="inlineStr"/>
@@ -14247,36 +14255,36 @@
       </c>
       <c r="D541" t="inlineStr">
         <is>
-          <t>[[2.23314676e+06]
- [5.61112467e+06]
- [5.74466188e+06]
- [1.37999128e+06]
- [1.38000173e+06]
- [1.38001235e+06]
- [1.20230751e+06]
- [1.20231700e+06]
- [1.20232681e+06]
- [1.17814098e+06]
- [1.17818499e+06]
- [1.17823464e+06]
- [1.22294926e+06]
- [1.22287626e+06]
- [1.22290020e+06]
- [1.37020430e+06]
- [1.37021070e+06]
- [1.36689585e+06]
- [3.38694610e+06]
- [3.38784861e+06]
- [3.38865907e+06]
- [3.49580729e+06]
- [3.49705519e+06]
- [3.49803311e+06]
- [5.32952133e+06]
- [5.73199810e+06]
- [6.19988214e+06]
- [1.18614448e+07]
- [1.31245905e+07]
- [6.33962609e+03]]</t>
+          <t>[[2.20059563e+06]
+ [5.44581714e+06]
+ [5.51735119e+06]
+ [1.56564265e+06]
+ [1.56565453e+06]
+ [1.56566663e+06]
+ [1.56567903e+06]
+ [1.56569183e+06]
+ [1.56570514e+06]
+ [1.56590199e+06]
+ [1.56596426e+06]
+ [1.56603565e+06]
+ [1.56603275e+06]
+ [1.56591957e+06]
+ [1.56594906e+06]
+ [1.56575938e+06]
+ [1.56576643e+06]
+ [1.56577026e+06]
+ [3.48041159e+06]
+ [3.48115665e+06]
+ [3.48182464e+06]
+ [5.30400867e+06]
+ [5.30551182e+06]
+ [5.30668754e+06]
+ [8.47727510e+06]
+ [9.58911900e+06]
+ [1.10351910e+07]
+ [1.24228969e+07]
+ [1.35304316e+07]
+ [7.06450947e+03]]</t>
         </is>
       </c>
       <c r="E541" t="inlineStr"/>
@@ -14301,34 +14309,34 @@
         <is>
           <t>[[-0.00000000e+00]
  [-0.00000000e+00]
- [-7.62744710e+06]
- [-1.26751522e+07]
- [-1.16558399e+07]
- [-1.06444406e+07]
- [-8.38255603e+06]
- [-7.51747336e+06]
- [-6.65995666e+06]
- [-5.28109091e+06]
- [-3.65187936e+06]
- [-2.06268625e+06]
- [-6.64113427e+05]
+ [-7.75658987e+06]
+ [-1.49113017e+07]
+ [-1.37121624e+07]
+ [-1.25223321e+07]
+ [-1.13420132e+07]
+ [-1.01715135e+07]
+ [-9.01125101e+06]
+ [-7.29568016e+06]
+ [-5.04496973e+06]
+ [-2.84954366e+06]
+ [-8.83384932e+05]
  [-0.00000000e+00]
  [-0.00000000e+00]
  [-0.00000000e+00]
  [-0.00000000e+00]
- [-1.38226070e+03]
- [-6.37727477e+03]
- [-7.14427391e+03]
- [-7.70875864e+03]
- [-8.50011278e+03]
- [-9.03966576e+03]
- [-9.49210348e+03]
- [-1.40303966e+04]
- [-1.33902336e+04]
- [-1.26912628e+04]
- [-2.08826573e+04]
- [-1.93167339e+04]
- [-1.76762289e+04]]</t>
+ [-1.71661371e+03]
+ [-8.26006188e+03]
+ [-9.25350457e+03]
+ [-9.98464366e+03]
+ [-1.62927612e+04]
+ [-1.73270215e+04]
+ [-1.81943081e+04]
+ [-2.69782275e+04]
+ [-2.45417022e+04]
+ [-2.19430879e+04]
+ [-2.00031422e+04]
+ [-1.87804306e+04]
+ [-1.74947349e+04]]</t>
         </is>
       </c>
       <c r="E542" t="inlineStr"/>
@@ -14399,36 +14407,36 @@
       <c r="C544" t="inlineStr"/>
       <c r="D544" t="inlineStr">
         <is>
-          <t>[[4.28974749e-02]
- [7.88860917e-02]
- [2.11327556e-01]
- [2.30750165e-01]
- [2.25718487e-01]
- [2.20768480e-01]
- [1.88667257e-01]
- [1.84595387e-01]
- [1.80608592e-01]
- [1.70795691e-01]
- [1.63591709e-01]
- [1.56834551e-01]
- [1.56057343e-01]
- [1.51450613e-01]
- [1.48555089e-01]
- [1.64333246e-01]
- [1.62637763e-01]
- [1.52292039e-01]
- [4.00327783e-01]
- [3.59142193e-01]
- [3.17775596e-01]
- [2.66176932e-01]
- [2.04969183e-01]
- [1.44273661e-01]
- [1.69367633e-01]
- [1.31309334e-01]
- [8.38725544e-02]
- [1.06503471e-01]
- [1.15649998e-01]
- [1.05855485e-04]]</t>
+          <t>[[3.49531651e-02]
+ [8.27010749e-02]
+ [2.11557365e-01]
+ [2.66038222e-01]
+ [2.60133853e-01]
+ [2.54326572e-01]
+ [2.48622020e-01]
+ [2.43026406e-01]
+ [2.37546514e-01]
+ [2.28745008e-01]
+ [2.18594130e-01]
+ [2.09067808e-01]
+ [2.00192443e-01]
+ [1.93958518e-01]
+ [1.90001652e-01]
+ [1.88022758e-01]
+ [1.86043638e-01]
+ [1.84060442e-01]
+ [3.71483664e-01]
+ [3.34059971e-01]
+ [2.96555698e-01]
+ [3.65373865e-01]
+ [2.80374946e-01]
+ [1.96087672e-01]
+ [2.46672469e-01]
+ [2.11758348e-01]
+ [1.52178025e-01]
+ [1.10778001e-01]
+ [1.19223354e-01]
+ [1.08602513e-04]]</t>
         </is>
       </c>
       <c r="E544" t="inlineStr"/>
@@ -14447,36 +14455,36 @@
       <c r="C545" t="inlineStr"/>
       <c r="D545" t="inlineStr">
         <is>
-          <t>[[0.06517142]
- [0.08107839]
- [0.16551556]
- [0.0485888 ]
- [0.04607327]
- [0.04367489]
- [0.03339134]
- [0.03162263]
- [0.0299975 ]
- [0.03394068]
- [0.02998886]
- [0.02691042]
- [0.02650527]
- [0.02546888]
- [0.02449908]
- [0.02617813]
- [0.02569723]
- [0.02603512]
- [0.11264868]
- [0.1072023 ]
- [0.1017812 ]
- [0.10666565]
- [0.09898535]
- [0.0914236 ]
- [0.17445981]
- [0.17064628]
- [0.16781383]
- [0.54871723]
- [0.54737998]
- [0.00234186]]</t>
+          <t>[[0.05796322]
+ [0.07398982]
+ [0.16201668]
+ [0.05865868]
+ [0.05527596]
+ [0.05200991]
+ [0.04887638]
+ [0.04589437]
+ [0.04308624]
+ [0.05562255]
+ [0.047452  ]
+ [0.04034144]
+ [0.03470508]
+ [0.03240992]
+ [0.03133657]
+ [0.02814213]
+ [0.02763261]
+ [0.02712375]
+ [0.13075662]
+ [0.12417947]
+ [0.11762306]
+ [0.29775932]
+ [0.28339462]
+ [0.26903962]
+ [0.57917708]
+ [0.56915087]
+ [0.56403602]
+ [0.5511337 ]
+ [0.54953359]
+ [0.00232401]]</t>
         </is>
       </c>
       <c r="E545" t="inlineStr"/>
@@ -14495,36 +14503,36 @@
       <c r="C546" t="inlineStr"/>
       <c r="D546" t="inlineStr">
         <is>
-          <t>[[1.93459039e-01]
- [3.34017754e-01]
- [5.04148090e-01]
- [4.80211833e-01]
- [4.74203166e-01]
- [4.68191007e-01]
- [4.00883477e-01]
- [3.95464372e-01]
- [3.90029023e-01]
- [3.71189428e-01]
- [3.60288147e-01]
- [3.49208296e-01]
- [3.52020409e-01]
- [3.42216977e-01]
- [3.32434656e-01]
- [3.67894944e-01]
- [3.62601467e-01]
- [3.48185814e-01]
- [9.20762948e-01]
- [8.29017780e-01]
- [7.38198019e-01]
- [6.30827493e-01]
- [5.01451044e-01]
- [3.74633818e-01]
- [4.91929873e-01]
- [4.48171765e-01]
- [3.84438425e-01]
- [5.66298940e-01]
- [7.51708203e-01]
- [4.46387277e-10]]</t>
+          <t>[[1.81485293e-01]
+ [3.30076230e-01]
+ [5.07038597e-01]
+ [5.64402631e-01]
+ [5.57314266e-01]
+ [5.50221618e-01]
+ [5.43118351e-01]
+ [5.35997951e-01]
+ [5.28853639e-01]
+ [5.14458989e-01]
+ [4.99874867e-01]
+ [4.85024297e-01]
+ [4.71235199e-01]
+ [4.58669391e-01]
+ [4.46130722e-01]
+ [4.39872414e-01]
+ [4.33621202e-01]
+ [4.27366911e-01]
+ [8.78488100e-01]
+ [7.90048265e-01]
+ [7.02357699e-01]
+ [9.12337923e-01]
+ [7.28954799e-01]
+ [5.48390273e-01]
+ [7.77865924e-01]
+ [7.86794433e-01]
+ [7.84974619e-01]
+ [6.64872907e-01]
+ [8.48162864e-01]
+ [5.68076748e-10]]</t>
         </is>
       </c>
       <c r="E546" t="inlineStr"/>
@@ -14566,7 +14574,7 @@
       <c r="C548" t="inlineStr"/>
       <c r="D548" t="inlineStr">
         <is>
-          <t>[0.90909091]</t>
+          <t>[0.9999236]</t>
         </is>
       </c>
       <c r="E548" t="inlineStr"/>
@@ -14613,26 +14621,26 @@
       </c>
       <c r="D550" t="inlineStr">
         <is>
-          <t>[[2.25650526e+10 5.88608222e+12 2.25650526e+10 5.88608222e+12
-  1.52133333e+10 1.24226667e+11]
- [2.04901053e+10 4.24064551e+12 2.04901053e+10 4.24064551e+12
-  1.40933333e+10 1.24226667e+11]
- [1.84151579e+10 2.94918412e+12 1.84151579e+10 2.94918412e+12
-  1.29733333e+10 1.24226667e+11]
- [1.63402105e+10 1.96745111e+12 1.63402105e+10 1.96745111e+12
-  1.18533333e+10 1.24226667e+11]
- [1.42652632e+10 1.25119959e+12 1.42652632e+10 1.25119959e+12
-  1.07333333e+10 1.24226667e+11]
- [1.21903158e+10 7.56182634e+11 1.21903158e+10 7.56182634e+11
-  9.61333333e+09 1.24226667e+11]
- [1.01153684e+10 4.38153333e+11 1.01153684e+10 4.38153333e+11
-  8.49333333e+09 1.24226667e+11]
- [8.04042105e+09 2.52864774e+11 8.04042105e+09 2.52864774e+11
-  7.37333333e+09 1.24226667e+11]
- [5.96547368e+09 1.56070041e+11 5.96547368e+09 1.56070041e+11
-  6.25333333e+09 1.24226667e+11]
- [3.89052632e+09 1.03522222e+11 3.89052632e+09 1.03522222e+11
-  5.13333333e+09 1.24226667e+11]]</t>
+          <t>[[2.26304633e+10 5.90517775e+12 2.26304633e+10 5.90517775e+12
+  1.52996391e+10 1.30598399e+11]
+ [2.05555159e+10 4.25820929e+12 2.05555159e+10 4.25820929e+12
+  1.41796391e+10 1.30598399e+11]
+ [1.84805686e+10 2.96521614e+12 1.84805686e+10 2.96521614e+12
+  1.30596391e+10 1.30598399e+11]
+ [1.64056212e+10 1.98195139e+12 1.64056212e+10 1.98195139e+12
+  1.19396391e+10 1.30598399e+11]
+ [1.43306738e+10 1.26416811e+12 1.43306738e+10 1.26416811e+12
+  1.08196391e+10 1.30598399e+11]
+ [1.22557264e+10 7.67619410e+11 1.22557264e+10 7.67619410e+11
+  9.69963906e+09 1.30598399e+11]
+ [1.01807791e+10 4.48058360e+11 1.01807791e+10 4.48058360e+11
+  8.57963906e+09 1.30598399e+11]
+ [8.10583171e+09 2.61238050e+11 8.10583171e+09 2.61238050e+11
+  7.45963906e+09 1.30598399e+11]
+ [6.03088434e+09 1.62911568e+11 6.03088434e+09 1.62911568e+11
+  6.33963906e+09 1.30598399e+11]
+ [3.95593697e+09 1.08831999e+11 3.95593697e+09 1.08831999e+11
+  5.21963906e+09 1.30598399e+11]]</t>
         </is>
       </c>
       <c r="E550" t="inlineStr"/>
@@ -14655,9 +14663,9 @@
       </c>
       <c r="D551" t="inlineStr">
         <is>
-          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
- 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
- 427.60678303 391.57616974 352.18249915]</t>
+          <t>[376.8637364  433.4947406  472.91020584 503.8274884  539.45978844
+ 568.76856759 593.87710694 546.37921754 494.76103473 438.15146599
+ 411.93099011 383.31695362 352.18250007]</t>
         </is>
       </c>
       <c r="E551" t="inlineStr"/>
@@ -14776,9 +14784,9 @@
       </c>
       <c r="D556" t="inlineStr">
         <is>
-          <t>[336.9560439  388.43785582 424.16473764 452.12457083 484.27449749
- 510.65946695 533.22010636 511.58791739 487.37587695 460.61782438
- 427.60678303 391.57616974 352.18249915]</t>
+          <t>[376.8637364  433.4947406  472.91020584 503.8274884  539.45978844
+ 568.76856759 593.87710694 546.37921754 494.76103473 438.15146599
+ 411.93099011 383.31695362 352.18250007]</t>
         </is>
       </c>
       <c r="E556" t="inlineStr"/>
@@ -14966,9 +14974,9 @@
       </c>
       <c r="D564" t="inlineStr">
         <is>
-          <t>[-336.9560439  -388.43785582 -424.16473764 -452.12457083 -484.27449749
- -510.65946695 -533.22010636 -511.58791739 -487.37587695 -460.61782438
- -427.60678303 -391.57616974 -352.18249915]</t>
+          <t>[-376.8637364  -433.4947406  -472.91020584 -503.8274884  -539.45978844
+ -568.76856759 -593.87710694 -546.37921754 -494.76103473 -438.15146599
+ -411.93099011 -383.31695362 -352.18250007]</t>
         </is>
       </c>
       <c r="E564" t="inlineStr"/>
@@ -15012,7 +15020,7 @@
       <c r="C566" t="inlineStr"/>
       <c r="D566" t="inlineStr">
         <is>
-          <t>[250.         257.72533448 343.6766274  469.23586931]</t>
+          <t>[323.51319955 493.08516358 629.05982495 456.23592651]</t>
         </is>
       </c>
       <c r="E566" t="inlineStr"/>
@@ -15031,7 +15039,7 @@
       <c r="C567" t="inlineStr"/>
       <c r="D567" t="inlineStr">
         <is>
-          <t>[1.         1.         0.80780761 0.74262732]</t>
+          <t>[0.99999983 0.99998939 0.68740507 0.78029908]</t>
         </is>
       </c>
       <c r="E567" t="inlineStr"/>
@@ -15050,7 +15058,7 @@
       <c r="C568" t="inlineStr"/>
       <c r="D568" t="inlineStr">
         <is>
-          <t>[1.         1.         0.80780761 0.74262732]</t>
+          <t>[0.99999983 1.00001061 0.68740507 0.78029908]</t>
         </is>
       </c>
       <c r="E568" t="inlineStr"/>
@@ -15069,7 +15077,7 @@
       <c r="C569" t="inlineStr"/>
       <c r="D569" t="inlineStr">
         <is>
-          <t>[0.97002493 0.67784333 0.57032058]</t>
+          <t>[0.65610347 0.6613352  0.99997425]</t>
         </is>
       </c>
       <c r="E569" t="inlineStr"/>
@@ -15112,9 +15120,9 @@
       </c>
       <c r="D571" t="inlineStr">
         <is>
-          <t>[5.         5.         5.         5.         5.         5.
- 5.         4.67967935 4.35935869 4.03903804 3.69252536 3.34601268
- 2.9995    ]</t>
+          <t>[5.59204313 5.59204281 5.59204249 5.59204217 5.59206194 5.59208171
+ 5.59210149 5.00941395 4.42672642 3.84403889 3.56252593 3.28101297
+ 2.99950001]</t>
         </is>
       </c>
       <c r="E571" t="inlineStr"/>
@@ -15365,9 +15373,9 @@
       </c>
       <c r="D582" t="inlineStr">
         <is>
-          <t>[10.         10.         10.         10.         10.         10.
- 10.          9.35935869  8.71871739  8.07807608  7.38505072  6.69202536
-  5.999     ]</t>
+          <t>[11.18408627 11.18408563 11.18408499 11.18408435 11.18412389 11.18416343
+ 11.18420297 10.01882791  8.85345284  7.68807778  7.12505186  6.56202594
+  5.99900001]</t>
         </is>
       </c>
       <c r="E582" t="inlineStr"/>
@@ -15620,7 +15628,7 @@
       </c>
       <c r="D593" t="inlineStr">
         <is>
-          <t>[10445.94134309 10134.04334639  6215.22949562  2762.32930662]</t>
+          <t>[10106.31148001  6637.8911669   3705.39194753  2685.63692717]</t>
         </is>
       </c>
       <c r="E593" t="inlineStr">
@@ -15647,7 +15655,7 @@
       </c>
       <c r="D594" t="inlineStr">
         <is>
-          <t>[129533.85103079 125696.32860397  63107.98029353  17033.32067808]</t>
+          <t>[157043.07391748 103367.51595026  41110.44534766  15653.62709329]</t>
         </is>
       </c>
       <c r="E594" t="inlineStr">
@@ -15674,7 +15682,7 @@
       </c>
       <c r="D595" t="inlineStr">
         <is>
-          <t>[129533.85103079 125696.32860397  63107.98029353  17033.32067808]</t>
+          <t>[157043.07391748 103367.51595026  41110.44534766  15653.62709329]</t>
         </is>
       </c>
       <c r="E595" t="inlineStr">
@@ -15701,7 +15709,7 @@
       </c>
       <c r="D596" t="inlineStr">
         <is>
-          <t>[3.10409420e+12 3.01213344e+12 1.51229284e+12 4.08179264e+11]</t>
+          <t>[3.76331354e+12 2.47705526e+12 9.85153255e+11 3.75116873e+11]</t>
         </is>
       </c>
       <c r="E596" t="inlineStr">
@@ -15728,7 +15736,7 @@
       </c>
       <c r="D597" t="inlineStr">
         <is>
-          <t>[3.10409420e+12 3.01213344e+12 1.51229284e+12 4.08179264e+11]</t>
+          <t>[3.76331354e+12 2.47705526e+12 9.85153255e+11 3.75116873e+11]</t>
         </is>
       </c>
       <c r="E597" t="inlineStr">
@@ -15755,7 +15763,7 @@
       </c>
       <c r="D598" t="inlineStr">
         <is>
-          <t>[2.46154670e+12 2.38862182e+12 1.19924822e+12 3.23686156e+11]</t>
+          <t>[2.98430764e+12 1.96430482e+12 7.81226532e+11 2.97467680e+11]</t>
         </is>
       </c>
       <c r="E598" t="inlineStr">
@@ -15782,7 +15790,7 @@
       </c>
       <c r="D599" t="inlineStr">
         <is>
-          <t>[2.50322103e+11 2.42847911e+11 1.48939120e+11 6.61952865e+10]</t>
+          <t>[2.42183357e+11 1.59067605e+11 8.87944392e+10 6.43574629e+10]</t>
         </is>
       </c>
       <c r="E599" t="inlineStr">
@@ -15890,10 +15898,10 @@
       </c>
       <c r="D603" t="inlineStr">
         <is>
-          <t>[[0.         0.         0.7989706  0.32215517 0.32215517 0.        ]
- [0.         0.         0.82356072 0.3319906  0.3319906  0.        ]
- [0.         0.         1.34283054 0.59770421 0.59770421 0.        ]
- [0.         0.         3.02136316 1.72437423 1.72437423 0.        ]]</t>
+          <t>[[0.         0.         0.82582058 0.29718718 0.29718718 0.        ]
+ [0.         0.         1.25732703 0.45150966 0.45150966 0.        ]
+ [0.         0.         2.2523933  0.95783477 0.95783477 0.        ]
+ [0.         0.         3.1076427  1.82437512 1.82437512 0.        ]]</t>
         </is>
       </c>
       <c r="E603" t="inlineStr"/>
@@ -15916,10 +15924,10 @@
       </c>
       <c r="D604" t="inlineStr">
         <is>
-          <t>[[1.3135028  1.3135028  0.         0.         0.         0.16107759]
- [1.35400229 1.35400229 0.         0.         0.         0.1659953 ]
- [2.20869034 2.20869034 0.         0.         0.         0.29885211]
- [4.97127384 4.97127384 0.         0.         0.         0.86218712]]</t>
+          <t>[[1.35820075 1.35820075 0.         0.         0.         0.14859359]
+ [2.06886875 2.06886875 0.         0.         0.         0.22575483]
+ [3.70692216 3.70692216 0.         0.         0.         0.47891738]
+ [5.11309767 5.11309767 0.         0.         0.         0.91218756]]</t>
         </is>
       </c>
       <c r="E604" t="inlineStr"/>
@@ -15942,7 +15950,7 @@
       </c>
       <c r="D605" t="inlineStr">
         <is>
-          <t>[603.37566942]</t>
+          <t>[538.04446253]</t>
         </is>
       </c>
       <c r="E605" t="inlineStr"/>
@@ -15965,7 +15973,7 @@
       </c>
       <c r="D606" t="inlineStr">
         <is>
-          <t>[3187423.76365581]</t>
+          <t>[2634279.06642127]</t>
         </is>
       </c>
       <c r="E606" t="inlineStr"/>
@@ -15988,8 +15996,8 @@
       </c>
       <c r="D607" t="inlineStr">
         <is>
-          <t>[10.         10.         10.         10.         10.         10.
-  9.67967935  9.03903804  8.39839673  7.7315634   7.03853804  6.34551268]</t>
+          <t>[11.18408595 11.18408531 11.18408467 11.18410412 11.18414366 11.1841832
+ 10.60151544  9.43614038  8.27076531  7.40656482  6.8435389   6.28051298]</t>
         </is>
       </c>
       <c r="E607" t="inlineStr"/>
@@ -16012,8 +16020,8 @@
       </c>
       <c r="D608" t="inlineStr">
         <is>
-          <t>[0.0428     0.0428     0.0428     0.04151707 0.04151707 0.04151707
- 0.02814207 0.02814207 0.02814207 0.01605    0.01605    0.01605   ]</t>
+          <t>[0.03699067 0.03699067 0.03699067 0.02426971 0.02426971 0.02426971
+ 0.01605041 0.01605041 0.01605041 0.01605    0.01605    0.01605   ]</t>
         </is>
       </c>
       <c r="E608" t="inlineStr"/>
@@ -16060,18 +16068,18 @@
       </c>
       <c r="D610" t="inlineStr">
         <is>
-          <t>[[85160115.64781867]
- [77144862.65686788]
- [69074882.4691234 ]
- [59186173.25535725]
- [47144587.25933338]
- [35092813.37801799]
- [43633613.40594918]
- [37240893.81442108]
- [28105994.82361823]
- [28164299.01609978]
- [-2061129.37148159]
- [ 2912294.9222079 ]]</t>
+          <t>[[78977330.53100972]
+ [71687907.39719652]
+ [64364570.89823939]
+ [81086751.93953487]
+ [64327032.71320929]
+ [47523809.95883623]
+ [63247229.2027448 ]
+ [59770500.5592005 ]
+ [51227773.62108448]
+ [31890861.54058476]
+ [-1408131.10055944]
+ [ 3205961.07731805]]</t>
         </is>
       </c>
       <c r="E610" t="inlineStr"/>
@@ -16094,18 +16102,18 @@
       </c>
       <c r="D611" t="inlineStr">
         <is>
-          <t>[[ 3385516.18198728]
- [ 3386480.52306403]
- [ 3387357.33789641]
- [ 3494067.01412618]
- [ 3495459.93285181]
- [ 3496584.40829886]
- [ 5328736.66915661]
- [ 5731307.92404687]
- [ 6199312.57267463]
- [11861102.04008803]
- [13124554.77252488]
- [14686980.33880659]]</t>
+          <t>[[ 3478790.51921752]
+ [ 3479585.23603949]
+ [ 3480308.02840145]
+ [ 5301963.77949318]
+ [ 5303644.79884254]
+ [ 5305000.03062618]
+ [ 8476368.10072889]
+ [ 9588345.15638592]
+ [11034622.34489116]
+ [12422633.90046385]
+ [13530516.99860838]
+ [14853548.28567418]]</t>
         </is>
       </c>
       <c r="E611" t="inlineStr"/>
@@ -16128,18 +16136,18 @@
       </c>
       <c r="D612" t="inlineStr">
         <is>
-          <t>[[ -6377.27477098]
- [ -7144.27390968]
- [ -7708.75864117]
- [ -8500.11278108]
- [ -9039.66575638]
- [ -9492.10348399]
- [-14030.3966498 ]
- [-13390.233557  ]
- [-12691.26282513]
- [-20882.65728422]
- [-19316.73388956]
- [-17676.22885516]]</t>
+          <t>[[ -8260.06188286]
+ [ -9253.50456648]
+ [ -9984.64365945]
+ [-16292.76120689]
+ [-17327.02154816]
+ [-18194.30814025]
+ [-26978.2275431 ]
+ [-24541.70220934]
+ [-21943.08793898]
+ [-20003.14219473]
+ [-18780.43060259]
+ [-17494.73491964]]</t>
         </is>
       </c>
       <c r="E612" t="inlineStr"/>
@@ -16192,18 +16200,18 @@
       <c r="C614" t="inlineStr"/>
       <c r="D614" t="inlineStr">
         <is>
-          <t>[[0.43424776]
- [0.39358338]
- [0.35266569]
- [0.30266886]
- [0.24181473]
- [0.1811783 ]
- [0.22690854]
- [0.19609057]
- [0.15308259]
- [0.17737901]
- [0.11610867]
- [0.13025544]]</t>
+          <t>[[0.40294274]
+ [0.36598317]
+ [0.32887787]
+ [0.41516282]
+ [0.33059222]
+ [0.2462742 ]
+ [0.33035721]
+ [0.31562871]
+ [0.27819179]
+ [0.19574083]
+ [0.11942777]
+ [0.1318904 ]]</t>
         </is>
       </c>
       <c r="E614" t="inlineStr"/>
@@ -16222,18 +16230,18 @@
       <c r="C615" t="inlineStr"/>
       <c r="D615" t="inlineStr">
         <is>
-          <t>[[0.11263765]
- [0.10718942]
- [0.10176716]
- [0.10664006]
- [0.09895912]
- [0.09139726]
- [0.17443303]
- [0.17062383]
- [0.16779618]
- [0.54868759]
- [0.5473687 ]
- [0.5494845 ]]</t>
+          <t>[[0.13073664]
+ [0.12415682]
+ [0.11759869]
+ [0.29768726]
+ [0.28332035]
+ [0.26896443]
+ [0.57908071]
+ [0.56907933]
+ [0.56399101]
+ [0.55111081]
+ [0.54952755]
+ [0.55049923]]</t>
         </is>
       </c>
       <c r="E615" t="inlineStr"/>
@@ -16252,18 +16260,18 @@
       <c r="C616" t="inlineStr"/>
       <c r="D616" t="inlineStr">
         <is>
-          <t>[[1.153462  ]
- [1.04809631]
- [0.9428673 ]
- [0.81865437]
- [0.66548001]
- [0.51362695]
- [0.68369468]
- [0.63849648]
- [0.56491612]
- [0.85718382]
- [0.57120487]
- [0.74229725]]</t>
+          <t>[[1.45343185]
+ [1.31964761]
+ [1.18607128]
+ [1.5447502 ]
+ [1.26273998]
+ [0.98228499]
+ [1.40676614]
+ [1.46838453]
+ [1.49646396]
+ [1.32422759]
+ [0.81350345]
+ [1.0262705 ]]</t>
         </is>
       </c>
       <c r="E616" t="inlineStr"/>
@@ -16379,7 +16387,7 @@
       </c>
       <c r="D621" t="inlineStr">
         <is>
-          <t>[0.24028912]</t>
+          <t>[0.23814302]</t>
         </is>
       </c>
       <c r="E621" t="inlineStr"/>
@@ -16402,7 +16410,7 @@
       </c>
       <c r="D622" t="inlineStr">
         <is>
-          <t>[0.24257794]</t>
+          <t>[0.24098164]</t>
         </is>
       </c>
       <c r="E622" t="inlineStr"/>
@@ -16425,7 +16433,7 @@
       </c>
       <c r="D623" t="inlineStr">
         <is>
-          <t>[0.24028912 0.24257794 0.82002628 0.94741571 1.11042389 2.45606311]</t>
+          <t>[0.23814302 0.24098164 0.76174059 0.93480142 1.1041958  2.79755514]</t>
         </is>
       </c>
       <c r="E623" t="inlineStr"/>
@@ -16444,12 +16452,9 @@
       <c r="C624" t="inlineStr"/>
       <c r="D624" t="inlineStr">
         <is>
-          <t>[[ 1.34501898e+00  2.63037747e-02 -1.62860718e+00  1.86305912e+00
-  -6.05774696e-01]
- [ 2.43922509e+02 -1.26897846e+02 -5.50694287e+02  9.84822297e+02
-  -5.50152673e+02]
- [-6.62604757e+01  2.04175058e+02 -3.45153122e+02  3.55715411e+02
-  -1.47476871e+02]]</t>
+          <t>[[   0.86491943    1.2044536    -3.44585294    3.70478147   -1.32830156]
+ [  39.12251229  -39.69201637   11.68179039   30.29379381  -40.40608012]
+ [ -85.43856898  249.21924955 -453.31433153  514.46391515 -223.93026419]]</t>
         </is>
       </c>
       <c r="E624" t="inlineStr"/>
@@ -16468,12 +16473,9 @@
       <c r="C625" t="inlineStr"/>
       <c r="D625" t="inlineStr">
         <is>
-          <t>[[ 1.33441864e+00  1.08008412e-02 -1.53938295e+00  1.73648648e+00
-  -5.42323007e-01]
- [ 3.34067160e+01 -2.76697235e+00 -1.17287288e+02  1.86946290e+02
-  -9.92987464e+01]
- [-6.28982452e+01  1.89813976e+02 -3.17392821e+02  3.25276034e+02
-  -1.33798945e+02]]</t>
+          <t>[[   0.852171      1.20558999   -3.4138549     3.64538116   -1.28928725]
+ [  17.41696058  -12.43144769   -8.84307623   31.51680736  -26.65924402]
+ [ -82.67891862  239.296315   -435.95689804  493.98911591 -213.64961425]]</t>
         </is>
       </c>
       <c r="E625" t="inlineStr"/>
@@ -16492,7 +16494,7 @@
       <c r="C626" t="inlineStr"/>
       <c r="D626" t="inlineStr">
         <is>
-          <t>[[  7.20897396 -26.02206851  41.96140358 -31.41461906   9.26631002]
+          <t>[[  5.3576499  -18.13912974  29.03252846 -20.90583897   5.65479035]
  [  0.           0.           0.           0.           0.        ]
  [  0.           0.           0.           0.           0.        ]]</t>
         </is>
@@ -16517,7 +16519,7 @@
       </c>
       <c r="D627" t="inlineStr">
         <is>
-          <t>[0.24257794 1.11042389 2.52992596]</t>
+          <t>[0.24098164 1.1041958  2.8545326 ]</t>
         </is>
       </c>
       <c r="E627" t="inlineStr"/>
@@ -16540,7 +16542,7 @@
       </c>
       <c r="D628" t="inlineStr">
         <is>
-          <t>[0.24028912 0.94741571 2.45606311]</t>
+          <t>[0.23814302 0.93480142 2.79755514]</t>
         </is>
       </c>
       <c r="E628" t="inlineStr"/>
@@ -16563,7 +16565,7 @@
       </c>
       <c r="D629" t="inlineStr">
         <is>
-          <t>[4.93880443 0.         0.        ]</t>
+          <t>[4.43493175 0.         0.        ]</t>
         </is>
       </c>
       <c r="E629" t="inlineStr"/>
@@ -16587,18 +16589,18 @@
       <c r="D630" t="inlineStr">
         <is>
           <t>[[0.        ]
- [0.00807209]
- [0.03045285]
- [0.06583858]
- [0.13671459]
- [0.2282204 ]
- [0.33638004]
- [0.40917257]
- [0.48865184]
- [0.57448606]
- [0.66205771]
- [0.75623898]
- [0.85318342]]</t>
+ [0.00674769]
+ [0.02527514]
+ [0.0545112 ]
+ [0.117935  ]
+ [0.20644077]
+ [0.3152169 ]
+ [0.39061906]
+ [0.47571108]
+ [0.57162185]
+ [0.67090024]
+ [0.7775548 ]
+ [0.88717111]]</t>
         </is>
       </c>
       <c r="E630" t="inlineStr"/>
@@ -16621,7 +16623,7 @@
       </c>
       <c r="D631" t="inlineStr">
         <is>
-          <t>[0.85318342]</t>
+          <t>[0.88717111]</t>
         </is>
       </c>
       <c r="E631" t="inlineStr"/>
@@ -16644,18 +16646,18 @@
       </c>
       <c r="D632" t="inlineStr">
         <is>
-          <t>[[-17427765.12991663]
- [-16186366.78221211]
- [-14944587.88685458]
- [-13222849.37497341]
- [-11500611.20008019]
- [ -9777955.21838797]
- [ -9097151.95187112]
- [ -8461409.45930777]
- [ -7870754.04360263]
- [ -7579102.67267725]
- [ -7313593.23878349]
- [ -7074256.2758736 ]]</t>
+          <t>[[-14792255.83552192]
+ [-13590500.82297246]
+ [-12388325.66650094]
+ [-11256905.09900315]
+ [-10124926.22133705]
+ [ -8992478.8642256 ]
+ [ -8564166.31211518]
+ [ -8182867.61212859]
+ [ -7848629.45633108]
+ [ -7569265.06488163]
+ [ -7311132.84144737]
+ [ -7074256.27587361]]</t>
         </is>
       </c>
       <c r="E632" t="inlineStr"/>
@@ -16678,18 +16680,18 @@
       </c>
       <c r="D633" t="inlineStr">
         <is>
-          <t>[[2428340.58969823]
- [2429076.44059267]
- [2429745.66121794]
- [2431464.41489253]
- [2432495.54674606]
- [2433328.43446587]
- [2430320.56243432]
- [2430367.54182217]
- [2430375.83291243]
- [2429248.39987909]
- [2429220.83731715]
- [2429127.58409672]]</t>
+          <t>[[2428261.36452721]
+ [2428847.83671197]
+ [2429381.3576488 ]
+ [2430006.64208273]
+ [2430830.85797564]
+ [2431497.62005671]
+ [2429486.64446499]
+ [2429493.9935887 ]
+ [2429475.38137672]
+ [2429362.02541039]
+ [2429351.56714398]
+ [2429270.62753694]]</t>
         </is>
       </c>
       <c r="E633" t="inlineStr"/>
@@ -16712,18 +16714,18 @@
       </c>
       <c r="D634" t="inlineStr">
         <is>
-          <t>[[29100.21334624]
- [29110.04393666]
- [29119.07546929]
- [29142.38007936]
- [29156.79240186]
- [29168.82090949]
- [29127.92088216]
- [29128.99893601]
- [29129.67529452]
- [29114.12772248]
- [29114.60165251]
- [29114.41196808]]</t>
+          <t>[[29099.16256356]
+ [29107.00041827]
+ [29114.20359966]
+ [29122.78334809]
+ [29134.30955576]
+ [29143.94400109]
+ [29116.50270212]
+ [29116.96096466]
+ [29117.21398107]
+ [29116.24266725]
+ [29117.00381968]
+ [29117.0256052 ]]</t>
         </is>
       </c>
       <c r="E634" t="inlineStr"/>
@@ -16746,18 +16748,18 @@
       </c>
       <c r="D635" t="inlineStr">
         <is>
-          <t>[[-4355770.84979259]
- [-3999369.51509918]
- [-3640497.12021613]
- [-3124519.02847233]
- [-2606354.23982125]
- [-2087563.38387338]
- [-1776650.06345185]
- [-1465466.49623692]
- [-1154071.36764904]
- [ -862996.74568595]
- [ -571078.64832484]
- [ -278501.90073832]]</t>
+          <t>[[-4349162.19795935]
+ [-3994304.57722576]
+ [-3637778.32576996]
+ [-3125468.08331412]
+ [-2610163.11866413]
+ [-2093257.2023268 ]
+ [-1782753.9142576 ]
+ [-1471388.57583626]
+ [-1158966.77594137]
+ [ -866330.09195273]
+ [ -572753.36209753]
+ [ -278501.9279941 ]]</t>
         </is>
       </c>
       <c r="E635" t="inlineStr"/>
@@ -16780,17 +16782,17 @@
       </c>
       <c r="D636" t="inlineStr">
         <is>
-          <t>[[ 3.26042330e+08]
- [ 2.96343964e+08]
- [ 2.66462894e+08]
- [ 2.23535771e+08]
- [ 1.80456648e+08]
- [ 1.37343596e+08]
- [ 1.11509659e+08]
- [ 8.56652885e+07]
- [ 5.98176693e+07]
- [ 3.56818040e+07]
- [ 1.15214098e+07]
+          <t>[[ 3.25427454e+08]
+ [ 2.95845075e+08]
+ [ 2.66139437e+08]
+ [ 2.23485592e+08]
+ [ 1.80620176e+08]
+ [ 1.37649721e+08]
+ [ 1.11849668e+08]
+ [ 8.59996099e+07]
+ [ 6.00934716e+07]
+ [ 3.58676780e+07]
+ [ 1.16138057e+07]
  [-1.26341969e+07]]</t>
         </is>
       </c>
@@ -16814,18 +16816,18 @@
       </c>
       <c r="D637" t="inlineStr">
         <is>
-          <t>[[1299689.54225215]
- [1299674.3537992 ]
- [1299659.15932317]
- [1299649.59012126]
- [1299627.86871814]
- [1299606.14173766]
- [1299648.83929164]
- [1299648.18318422]
- [1299648.4245459 ]
- [1299792.63859019]
- [1299811.86142551]
- [1299836.63664036]]</t>
+          <t>[[1299663.37640344]
+ [1299648.18035189]
+ [1299632.97741208]
+ [1299699.66175321]
+ [1299677.86720602]
+ [1299656.06280409]
+ [1299737.17782783]
+ [1299756.55809997]
+ [1299783.26219625]
+ [1299806.24772884]
+ [1299821.41302364]
+ [1299840.40625841]]</t>
         </is>
       </c>
       <c r="E637" t="inlineStr"/>
@@ -16848,9 +16850,9 @@
       </c>
       <c r="D638" t="inlineStr">
         <is>
-          <t>[[  2427925.55809668]
- [    29094.73368413]
- [-18668642.37894937]]</t>
+          <t>[[  2427925.55809758]
+ [    29094.73368414]
+ [-15993436.94101516]]</t>
         </is>
       </c>
       <c r="E638" t="inlineStr"/>
@@ -16873,8 +16875,8 @@
       </c>
       <c r="D639" t="inlineStr">
         <is>
-          <t>[[-4.70896222e+06]
- [ 3.55500528e+08]
+          <t>[[-4.70178935e+06]
+ [ 3.54843036e+08]
  [ 1.29946107e+06]]</t>
         </is>
       </c>
@@ -16898,7 +16900,7 @@
       </c>
       <c r="D640" t="inlineStr">
         <is>
-          <t>[2142593.51976615]</t>
+          <t>[1869294.67175035]</t>
         </is>
       </c>
       <c r="E640" t="inlineStr"/>
@@ -16921,7 +16923,7 @@
       </c>
       <c r="D641" t="inlineStr">
         <is>
-          <t>[-2.98562705e+00 -4.41060468e-02  1.08214197e+02]</t>
+          <t>[-3.42213845e+00 -5.05545388e-02  1.13442233e+02]</t>
         </is>
       </c>
       <c r="E641" t="inlineStr"/>
@@ -16944,7 +16946,7 @@
       </c>
       <c r="D642" t="inlineStr">
         <is>
-          <t>[3.18866698e+10 3.17491828e+10 2.84709346e+08 7.86163621e+02
+          <t>[3.02649976e+10 3.01275105e+10 2.82981459e+08 7.86163621e+02
  1.35359722e+07 1.70976373e+05]</t>
         </is>
       </c>
@@ -19585,7 +19587,8 @@
       </c>
       <c r="D737" t="inlineStr">
         <is>
-          <t>[11. 11. 11. 11. 11. 11. 11.]</t>
+          <t>[11.18494085 11.18494084 11.18494084 11.18494085 11.18494083 11.18494083
+ 11.18494083]</t>
         </is>
       </c>
       <c r="E737" t="inlineStr">
@@ -19612,8 +19615,7 @@
       </c>
       <c r="D738" t="inlineStr">
         <is>
-          <t>[[0.077      0.077      0.10095695 0.10347047 0.1052105  0.09579198
-  0.08345544]]</t>
+          <t>[[0.077 0.077 0.077 0.077 0.077 0.077 0.077]]</t>
         </is>
       </c>
       <c r="E738" t="inlineStr">
@@ -19829,7 +19831,7 @@
       </c>
       <c r="D746" t="inlineStr">
         <is>
-          <t>[10.         10.         10.          8.07807608  5.999     ]</t>
+          <t>[11.18408627 11.18408435 11.18420297  7.68807778  5.99900001]</t>
         </is>
       </c>
       <c r="E746" t="inlineStr">
@@ -19879,7 +19881,7 @@
       </c>
       <c r="D748" t="inlineStr">
         <is>
-          <t>[[0.04       0.04       0.03760199 0.015      0.015     ]]</t>
+          <t>[[0.03877828 0.03036317 0.01500077 0.015      0.015     ]]</t>
         </is>
       </c>
       <c r="E748" t="inlineStr">

</xml_diff>